<commit_message>
changes to liability model so that asset_mv and methods containing asset_mv work with plan_data.xlsx instead of plan_mkt_value_data
</commit_message>
<xml_diff>
--- a/data/time_series/plan_data.xlsx
+++ b/data/time_series/plan_data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\Projects\UPS_MV-git\data\time_series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02652E32-DA1D-442F-B1BD-1BD3C17488EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mkt_value" sheetId="1" r:id="rId1"/>
     <sheet name="return" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -44,11 +45,14 @@
   <si>
     <t>Retirement</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -84,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,12 +111,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -124,6 +139,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,6 +236,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -253,6 +288,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -428,21 +480,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D147"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2:E146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -455,8 +508,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>40178</v>
       </c>
@@ -469,8 +525,12 @@
       <c r="D2" s="4">
         <v>12670331040.15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="4">
+        <f>SUM(B2,C2,D2)</f>
+        <v>15633809775.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>40209</v>
       </c>
@@ -483,8 +543,12 @@
       <c r="D3" s="4">
         <v>12454714514.059999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E66" si="0">SUM(B3,C3,D3)</f>
+        <v>15489729218.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>40237</v>
       </c>
@@ -497,8 +561,12 @@
       <c r="D4" s="4">
         <v>12582416484.82</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>15775048697.139999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>40268</v>
       </c>
@@ -511,8 +579,12 @@
       <c r="D5" s="4">
         <v>13025662728.84</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>16704873758.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>40298</v>
       </c>
@@ -525,8 +597,12 @@
       <c r="D6" s="4">
         <v>13260440725.690001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>17132130003.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>40329</v>
       </c>
@@ -539,8 +615,12 @@
       <c r="D7" s="4">
         <v>12652381383.559999</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>16351241876.799999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>40359</v>
       </c>
@@ -553,8 +633,12 @@
       <c r="D8" s="4">
         <v>12475038374.799999</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>16127227316.289999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>40390</v>
       </c>
@@ -567,8 +651,12 @@
       <c r="D9" s="4">
         <v>12970168980.82</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>16894210925.619999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>40421</v>
       </c>
@@ -581,8 +669,12 @@
       <c r="D10" s="4">
         <v>12942973012.129999</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>16864762411.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>40451</v>
       </c>
@@ -595,8 +687,12 @@
       <c r="D11" s="4">
         <v>13480205460.32</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>17683853962.580002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>40482</v>
       </c>
@@ -609,8 +705,12 @@
       <c r="D12" s="4">
         <v>13443063041.030001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>17795005221.620003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>40512</v>
       </c>
@@ -623,8 +723,12 @@
       <c r="D13" s="4">
         <v>14814700195.870001</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>19628314376.709999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>40543</v>
       </c>
@@ -637,8 +741,12 @@
       <c r="D14" s="4">
         <v>15090047197.559999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>20035126948.73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>40574</v>
       </c>
@@ -651,8 +759,12 @@
       <c r="D15" s="4">
         <v>15034722562.559999</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>21163701726.799999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>40602</v>
       </c>
@@ -665,8 +777,12 @@
       <c r="D16" s="4">
         <v>15339223946.43</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>21592868236.349998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>40633</v>
       </c>
@@ -679,8 +795,12 @@
       <c r="D17" s="4">
         <v>15338075937.65</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>21597393553.599998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>40663</v>
       </c>
@@ -693,8 +813,12 @@
       <c r="D18" s="4">
         <v>15759188122.620001</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>22196442158.830002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>40694</v>
       </c>
@@ -707,8 +831,12 @@
       <c r="D19" s="4">
         <v>15817399042.18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>22284623894.07</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>40724</v>
       </c>
@@ -721,8 +849,12 @@
       <c r="D20" s="4">
         <v>15518354156.139999</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>21869129586.239998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>40755</v>
       </c>
@@ -735,8 +867,12 @@
       <c r="D21" s="4">
         <v>15643951036.32</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>22052015022.439999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>40786</v>
       </c>
@@ -749,8 +885,12 @@
       <c r="D22" s="4">
         <v>15501631744.309999</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>21857152498.610001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>40816</v>
       </c>
@@ -763,8 +903,12 @@
       <c r="D23" s="4">
         <v>15478669634.76</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>21890587182.540001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>40847</v>
       </c>
@@ -777,8 +921,12 @@
       <c r="D24" s="4">
         <v>15988684918.42</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="4">
+        <f t="shared" si="0"/>
+        <v>22617832290.32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>40877</v>
       </c>
@@ -791,8 +939,12 @@
       <c r="D25" s="4">
         <v>15838131556.610001</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>22404660643.810001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>40908</v>
       </c>
@@ -805,8 +957,12 @@
       <c r="D26" s="4">
         <v>15979851739.540001</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
+        <f t="shared" si="0"/>
+        <v>22610566714.970001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>40939</v>
       </c>
@@ -819,8 +975,12 @@
       <c r="D27" s="4">
         <v>16380190274.370001</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="4">
+        <f t="shared" si="0"/>
+        <v>23182541487.510002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>40968</v>
       </c>
@@ -833,8 +993,12 @@
       <c r="D28" s="4">
         <v>16632293380.49</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="4">
+        <f t="shared" si="0"/>
+        <v>23538890877.400002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>40999</v>
       </c>
@@ -847,8 +1011,12 @@
       <c r="D29" s="4">
         <v>16525290668.17</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>23568457835.099998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>41029</v>
       </c>
@@ -861,8 +1029,12 @@
       <c r="D30" s="4">
         <v>16649048720.639999</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="4">
+        <f t="shared" si="0"/>
+        <v>23750894239.669998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>41060</v>
       </c>
@@ -875,8 +1047,12 @@
       <c r="D31" s="4">
         <v>16487003754.48</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="4">
+        <f t="shared" si="0"/>
+        <v>23525188092.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>41090</v>
       </c>
@@ -889,8 +1065,12 @@
       <c r="D32" s="4">
         <v>16666683230.139999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <f t="shared" si="0"/>
+        <v>23966952669.709999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>41121</v>
       </c>
@@ -903,8 +1083,12 @@
       <c r="D33" s="4">
         <v>16994661825.91</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="4">
+        <f t="shared" si="0"/>
+        <v>24445028323.779999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>41152</v>
       </c>
@@ -917,8 +1101,12 @@
       <c r="D34" s="4">
         <v>17060740670.370001</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="4">
+        <f t="shared" si="0"/>
+        <v>24546173849.48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>41182</v>
       </c>
@@ -931,8 +1119,12 @@
       <c r="D35" s="4">
         <v>17161797379.67</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="4">
+        <f t="shared" si="0"/>
+        <v>24697695785.049999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>41213</v>
       </c>
@@ -945,8 +1137,12 @@
       <c r="D36" s="4">
         <v>17142269583.370001</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="4">
+        <f t="shared" si="0"/>
+        <v>24675625120.169998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>41243</v>
       </c>
@@ -959,8 +1155,12 @@
       <c r="D37" s="4">
         <v>17226232669.720001</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="4">
+        <f t="shared" si="0"/>
+        <v>24802249901.279999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>41274</v>
       </c>
@@ -973,8 +1173,12 @@
       <c r="D38" s="4">
         <v>17291185714.259998</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="4">
+        <f t="shared" si="0"/>
+        <v>24895725823.459999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>41305</v>
       </c>
@@ -987,8 +1191,12 @@
       <c r="D39" s="4">
         <v>16688192891.540001</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="4">
+        <f t="shared" si="0"/>
+        <v>25170361391.66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>41333</v>
       </c>
@@ -1001,8 +1209,12 @@
       <c r="D40" s="4">
         <v>16760318931.09</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="4">
+        <f t="shared" si="0"/>
+        <v>25279056931.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>41364</v>
       </c>
@@ -1015,8 +1227,12 @@
       <c r="D41" s="4">
         <v>16965972358.16</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="4">
+        <f t="shared" si="0"/>
+        <v>25595461395.489998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>41394</v>
       </c>
@@ -1029,8 +1245,12 @@
       <c r="D42" s="4">
         <v>17344551325.700001</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="4">
+        <f t="shared" si="0"/>
+        <v>26172807411.43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>41425</v>
       </c>
@@ -1043,8 +1263,12 @@
       <c r="D43" s="4">
         <v>17009919681.780001</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="4">
+        <f t="shared" si="0"/>
+        <v>25673836920.309998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>41455</v>
       </c>
@@ -1057,8 +1281,12 @@
       <c r="D44" s="4">
         <v>16655048859.379999</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="4">
+        <f t="shared" si="0"/>
+        <v>25144097226.379997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>41486</v>
       </c>
@@ -1071,8 +1299,12 @@
       <c r="D45" s="4">
         <v>16844754449.469999</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="4">
+        <f t="shared" si="0"/>
+        <v>25436535483.029999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>41517</v>
       </c>
@@ -1085,8 +1317,12 @@
       <c r="D46" s="4">
         <v>16611704230.01</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="4">
+        <f t="shared" si="0"/>
+        <v>25090551978.139999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>41547</v>
       </c>
@@ -1099,8 +1335,12 @@
       <c r="D47" s="4">
         <v>16745140477.25</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="4">
+        <f t="shared" si="0"/>
+        <v>25528342822.260002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>41578</v>
       </c>
@@ -1113,8 +1353,12 @@
       <c r="D48" s="4">
         <v>17068600956.34</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="4">
+        <f t="shared" si="0"/>
+        <v>26027210514.610001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>41608</v>
       </c>
@@ -1127,8 +1371,12 @@
       <c r="D49" s="4">
         <v>17048811459.129999</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="4">
+        <f t="shared" si="0"/>
+        <v>26003668184.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>41639</v>
       </c>
@@ -1141,8 +1389,12 @@
       <c r="D50" s="4">
         <v>17124920453.700001</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="4">
+        <f t="shared" si="0"/>
+        <v>26126136558.370003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>41670</v>
       </c>
@@ -1155,8 +1407,12 @@
       <c r="D51" s="4">
         <v>17108427415.48</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="4">
+        <f t="shared" si="0"/>
+        <v>26107545286.209999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>41698</v>
       </c>
@@ -1169,8 +1425,12 @@
       <c r="D52" s="4">
         <v>17452044700.369999</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="4">
+        <f t="shared" si="0"/>
+        <v>26638014657</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>41729</v>
       </c>
@@ -1183,8 +1443,12 @@
       <c r="D53" s="4">
         <v>17534458681.869999</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="4">
+        <f t="shared" si="0"/>
+        <v>26769907188.32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>41759</v>
       </c>
@@ -1197,8 +1461,12 @@
       <c r="D54" s="4">
         <v>17527323843.169998</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="4">
+        <f t="shared" si="0"/>
+        <v>26765961123.209999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>41790</v>
       </c>
@@ -1211,8 +1479,12 @@
       <c r="D55" s="4">
         <v>17802031711.889999</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="4">
+        <f t="shared" si="0"/>
+        <v>27191839755.379997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>41820</v>
       </c>
@@ -1225,8 +1497,12 @@
       <c r="D56" s="4">
         <v>17885536456.360001</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="4">
+        <f t="shared" si="0"/>
+        <v>27325539811.990002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>41851</v>
       </c>
@@ -1239,8 +1515,12 @@
       <c r="D57" s="4">
         <v>17771447283.099998</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="4">
+        <f t="shared" si="0"/>
+        <v>27156693166.089996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>41882</v>
       </c>
@@ -1253,8 +1533,12 @@
       <c r="D58" s="4">
         <v>18152061725.919998</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="4">
+        <f t="shared" si="0"/>
+        <v>27744061638.859997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>41912</v>
       </c>
@@ -1267,8 +1551,12 @@
       <c r="D59" s="4">
         <v>17760389482.459999</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="4">
+        <f t="shared" si="0"/>
+        <v>27150516717.209999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>41943</v>
       </c>
@@ -1281,8 +1569,12 @@
       <c r="D60" s="4">
         <v>17913492320.950001</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="4">
+        <f t="shared" si="0"/>
+        <v>27371582530.760002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>41973</v>
       </c>
@@ -1295,8 +1587,12 @@
       <c r="D61" s="4">
         <v>18161633085.610001</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="4">
+        <f t="shared" si="0"/>
+        <v>27755791534.099998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>42004</v>
       </c>
@@ -1309,8 +1605,12 @@
       <c r="D62" s="4">
         <v>18347484059.09</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="4">
+        <f t="shared" si="0"/>
+        <v>28782286672.540001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>42035</v>
       </c>
@@ -1323,8 +1623,12 @@
       <c r="D63" s="4">
         <v>18722609505.799999</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="4">
+        <f t="shared" si="0"/>
+        <v>29377893373.27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>42063</v>
       </c>
@@ -1337,8 +1641,12 @@
       <c r="D64" s="4">
         <v>18813632546.84</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="4">
+        <f t="shared" si="0"/>
+        <v>29527582270.599998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>42094</v>
       </c>
@@ -1351,8 +1659,12 @@
       <c r="D65" s="4">
         <v>18773915353.099998</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="4">
+        <f t="shared" si="0"/>
+        <v>29472066114.919998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>42124</v>
       </c>
@@ -1365,8 +1677,12 @@
       <c r="D66" s="4">
         <v>18729047234.330002</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="4">
+        <f t="shared" si="0"/>
+        <v>29408499309.230003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>42155</v>
       </c>
@@ -1379,8 +1695,12 @@
       <c r="D67" s="4">
         <v>18647811742.490002</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="4">
+        <f t="shared" ref="E67:E130" si="1">SUM(B67,C67,D67)</f>
+        <v>29287873259.310001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>42185</v>
       </c>
@@ -1393,8 +1713,12 @@
       <c r="D68" s="4">
         <v>18237344817.240002</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="4">
+        <f t="shared" si="1"/>
+        <v>28649880311.460003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>42216</v>
       </c>
@@ -1407,8 +1731,12 @@
       <c r="D69" s="4">
         <v>18376949304.200001</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="4">
+        <f t="shared" si="1"/>
+        <v>28876049490.889999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>42247</v>
       </c>
@@ -1421,8 +1749,12 @@
       <c r="D70" s="4">
         <v>17823822010.27</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="4">
+        <f t="shared" si="1"/>
+        <v>28013794466.529999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>42277</v>
       </c>
@@ -1435,8 +1767,12 @@
       <c r="D71" s="4">
         <v>17611674082.799999</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="4">
+        <f t="shared" si="1"/>
+        <v>27687481033.779999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>42308</v>
       </c>
@@ -1449,8 +1785,12 @@
       <c r="D72" s="4">
         <v>18048333376.560001</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="4">
+        <f t="shared" si="1"/>
+        <v>28326214032.700001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>42338</v>
       </c>
@@ -1463,8 +1803,12 @@
       <c r="D73" s="4">
         <v>17923305130.990002</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="4">
+        <f t="shared" si="1"/>
+        <v>28136428854.080002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>42369</v>
       </c>
@@ -1477,8 +1821,12 @@
       <c r="D74" s="4">
         <v>17720678489.540001</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="4">
+        <f t="shared" si="1"/>
+        <v>28846123319.360001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>42400</v>
       </c>
@@ -1491,8 +1839,12 @@
       <c r="D75" s="4">
         <v>17401580107.799999</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="4">
+        <f t="shared" si="1"/>
+        <v>28336242435.290001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>42429</v>
       </c>
@@ -1505,8 +1857,12 @@
       <c r="D76" s="4">
         <v>17468918255.400002</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="4">
+        <f t="shared" si="1"/>
+        <v>28455548735.700001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>42460</v>
       </c>
@@ -1519,8 +1875,12 @@
       <c r="D77" s="4">
         <v>18015825215.720001</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="4">
+        <f t="shared" si="1"/>
+        <v>29356543183.02</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>42490</v>
       </c>
@@ -1533,8 +1893,12 @@
       <c r="D78" s="4">
         <v>18123427852.610001</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="4">
+        <f t="shared" si="1"/>
+        <v>29541899253.779999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>42521</v>
       </c>
@@ -1547,8 +1911,12 @@
       <c r="D79" s="4">
         <v>18098420744.150002</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="4">
+        <f t="shared" si="1"/>
+        <v>29511294102.970001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>42551</v>
       </c>
@@ -1561,8 +1929,12 @@
       <c r="D80" s="4">
         <v>18221304108.220001</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="4">
+        <f t="shared" si="1"/>
+        <v>29721707293.18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>42582</v>
       </c>
@@ -1575,8 +1947,12 @@
       <c r="D81" s="4">
         <v>18547786478.41</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="4">
+        <f t="shared" si="1"/>
+        <v>30265017930.439999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>42613</v>
       </c>
@@ -1589,8 +1965,12 @@
       <c r="D82" s="4">
         <v>18508832479.779999</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="4">
+        <f t="shared" si="1"/>
+        <v>30212130836.659996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>42643</v>
       </c>
@@ -1603,8 +1983,12 @@
       <c r="D83" s="4">
         <v>18773993442.110001</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="4">
+        <f t="shared" si="1"/>
+        <v>31311065698.300003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>42674</v>
       </c>
@@ -1617,8 +2001,12 @@
       <c r="D84" s="4">
         <v>18430042970.950001</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="4">
+        <f t="shared" si="1"/>
+        <v>30735579110.59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>42704</v>
       </c>
@@ -1631,8 +2019,12 @@
       <c r="D85" s="4">
         <v>18157757460.240002</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="4">
+        <f t="shared" si="1"/>
+        <v>30294027553</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>42735</v>
       </c>
@@ -1645,8 +2037,12 @@
       <c r="D86" s="4">
         <v>18519115493.09</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="4">
+        <f t="shared" si="1"/>
+        <v>31134438714.84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>42766</v>
       </c>
@@ -1659,8 +2055,12 @@
       <c r="D87" s="4">
         <v>18672728045.689999</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="4">
+        <f t="shared" si="1"/>
+        <v>31406508587.93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>42794</v>
       </c>
@@ -1673,8 +2073,12 @@
       <c r="D88" s="4">
         <v>18935552854.389999</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="4">
+        <f t="shared" si="1"/>
+        <v>31862808989.720001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>42825</v>
       </c>
@@ -1687,8 +2091,12 @@
       <c r="D89" s="4">
         <v>19799498475.639999</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="4">
+        <f t="shared" si="1"/>
+        <v>34237099341.939999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>42855</v>
       </c>
@@ -1701,8 +2109,12 @@
       <c r="D90" s="4">
         <v>20002234967.919998</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="4">
+        <f t="shared" si="1"/>
+        <v>34601102374.349998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>42886</v>
       </c>
@@ -1715,8 +2127,12 @@
       <c r="D91" s="4">
         <v>20236725707.75</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="4">
+        <f t="shared" si="1"/>
+        <v>35025362965.57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>42916</v>
       </c>
@@ -1729,8 +2145,12 @@
       <c r="D92" s="4">
         <v>20274704112.169998</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="4">
+        <f t="shared" si="1"/>
+        <v>35106467417.43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>42947</v>
       </c>
@@ -1743,8 +2163,12 @@
       <c r="D93" s="4">
         <v>20438444305.610001</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="4">
+        <f t="shared" si="1"/>
+        <v>35405676882.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>42978</v>
       </c>
@@ -1757,8 +2181,12 @@
       <c r="D94" s="4">
         <v>20590369678.540001</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="4">
+        <f t="shared" si="1"/>
+        <v>35685401140.059998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>43008</v>
       </c>
@@ -1771,8 +2199,12 @@
       <c r="D95" s="4">
         <v>20690747320.220001</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="4">
+        <f t="shared" si="1"/>
+        <v>35874830645.559998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>43039</v>
       </c>
@@ -1785,8 +2217,12 @@
       <c r="D96" s="4">
         <v>20816031800.59</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="4">
+        <f t="shared" si="1"/>
+        <v>36114807334.970001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>43069</v>
       </c>
@@ -1799,8 +2235,12 @@
       <c r="D97" s="4">
         <v>21026669979.09</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="4">
+        <f t="shared" si="1"/>
+        <v>36495501947.440002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>43100</v>
       </c>
@@ -1813,8 +2253,12 @@
       <c r="D98" s="4">
         <v>24225492187.240002</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="4">
+        <f t="shared" si="1"/>
+        <v>41855947325.630005</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>43131</v>
       </c>
@@ -1827,8 +2271,12 @@
       <c r="D99" s="4">
         <v>24550452831.880001</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="4">
+        <f t="shared" si="1"/>
+        <v>42583608483.910004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>43159</v>
       </c>
@@ -1841,8 +2289,12 @@
       <c r="D100" s="4">
         <v>23751543939.110001</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="4">
+        <f t="shared" si="1"/>
+        <v>41211539283.339996</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>43190</v>
       </c>
@@ -1855,8 +2307,12 @@
       <c r="D101" s="4">
         <v>23895593642.490002</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="4">
+        <f t="shared" si="1"/>
+        <v>41345361923.699997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>43220</v>
       </c>
@@ -1869,8 +2325,12 @@
       <c r="D102" s="4">
         <v>23668065334.799999</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="4">
+        <f t="shared" si="1"/>
+        <v>41046653376.559998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>43251</v>
       </c>
@@ -1883,8 +2343,12 @@
       <c r="D103" s="4">
         <v>23850014619.049999</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="4">
+        <f t="shared" si="1"/>
+        <v>41313125652.080002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>43281</v>
       </c>
@@ -1897,8 +2361,12 @@
       <c r="D104" s="4">
         <v>23743724505.990002</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="4">
+        <f t="shared" si="1"/>
+        <v>41120926179.029999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>43312</v>
       </c>
@@ -1911,8 +2379,12 @@
       <c r="D105" s="4">
         <v>23810476668.130001</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="4">
+        <f t="shared" si="1"/>
+        <v>41384483579.770004</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>43343</v>
       </c>
@@ -1925,8 +2397,12 @@
       <c r="D106" s="4">
         <v>23982305364.470001</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="4">
+        <f t="shared" si="1"/>
+        <v>41662699191.550003</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>43373</v>
       </c>
@@ -1939,8 +2415,12 @@
       <c r="D107" s="4">
         <v>23633877037.77</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="4">
+        <f t="shared" si="1"/>
+        <v>41186844593.330002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>43404</v>
       </c>
@@ -1953,8 +2433,12 @@
       <c r="D108" s="4">
         <v>22616086896.59</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="4">
+        <f t="shared" si="1"/>
+        <v>39382932997.410004</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>43434</v>
       </c>
@@ -1967,8 +2451,12 @@
       <c r="D109" s="4">
         <v>22855316166.619999</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="4">
+        <f t="shared" si="1"/>
+        <v>39775062674.709999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>43465</v>
       </c>
@@ -1981,8 +2469,12 @@
       <c r="D110" s="4">
         <v>22914691512.650002</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="4">
+        <f t="shared" si="1"/>
+        <v>39522884974.100006</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>43496</v>
       </c>
@@ -1995,8 +2487,12 @@
       <c r="D111" s="4">
         <v>23486649000.34</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="4">
+        <f t="shared" si="1"/>
+        <v>40669954095.649994</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>43524</v>
       </c>
@@ -2009,8 +2505,12 @@
       <c r="D112" s="4">
         <v>23478741957.66</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="4">
+        <f t="shared" si="1"/>
+        <v>40797714345.529999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>43555</v>
       </c>
@@ -2023,8 +2523,12 @@
       <c r="D113" s="4">
         <v>24171159309.130001</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="4">
+        <f t="shared" si="1"/>
+        <v>41816004324.669998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>43585</v>
       </c>
@@ -2037,8 +2541,12 @@
       <c r="D114" s="4">
         <v>24607805892.509998</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="4">
+        <f t="shared" si="1"/>
+        <v>42743010048.029999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>43616</v>
       </c>
@@ -2051,8 +2559,12 @@
       <c r="D115" s="4">
         <v>25031219112.639999</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="4">
+        <f t="shared" si="1"/>
+        <v>43049509347.520004</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>43646</v>
       </c>
@@ -2065,8 +2577,12 @@
       <c r="D116" s="4">
         <v>25624099438.360001</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="4">
+        <f t="shared" si="1"/>
+        <v>44201801916.779999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>43677</v>
       </c>
@@ -2079,8 +2595,12 @@
       <c r="D117" s="4">
         <v>25654690308.73</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="4">
+        <f t="shared" si="1"/>
+        <v>44289184114.949997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>43708</v>
       </c>
@@ -2093,8 +2613,12 @@
       <c r="D118" s="4">
         <v>27075142517.599998</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="4">
+        <f t="shared" si="1"/>
+        <v>46120218348.729996</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>43738</v>
       </c>
@@ -2107,8 +2631,12 @@
       <c r="D119" s="4">
         <v>26732490993.099998</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="4">
+        <f t="shared" si="1"/>
+        <v>46949500920.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>43769</v>
       </c>
@@ -2121,8 +2649,12 @@
       <c r="D120" s="4">
         <v>26631956752.709999</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="4">
+        <f t="shared" si="1"/>
+        <v>46865616845.860001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>43799</v>
       </c>
@@ -2135,8 +2667,12 @@
       <c r="D121" s="4">
         <v>26718171624.689999</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="4">
+        <f t="shared" si="1"/>
+        <v>47123526214.259995</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>43830</v>
       </c>
@@ -2149,8 +2685,12 @@
       <c r="D122" s="4">
         <v>25905410180.560001</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="4">
+        <f t="shared" si="1"/>
+        <v>46141543427.790001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>43861</v>
       </c>
@@ -2163,8 +2703,12 @@
       <c r="D123" s="4">
         <v>26801714204.060001</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="4">
+        <f t="shared" si="1"/>
+        <v>47197571777.949997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>43890</v>
       </c>
@@ -2177,8 +2721,12 @@
       <c r="D124" s="4">
         <v>27210513709.580002</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="4">
+        <f t="shared" si="1"/>
+        <v>47123736418.860001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>43921</v>
       </c>
@@ -2191,8 +2739,12 @@
       <c r="D125" s="4">
         <v>26774758277.919998</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="4">
+        <f t="shared" si="1"/>
+        <v>45203938859.300003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>43951</v>
       </c>
@@ -2205,8 +2757,12 @@
       <c r="D126" s="4">
         <v>27673823035.060001</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="4">
+        <f t="shared" si="1"/>
+        <v>47063924664.940002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>43982</v>
       </c>
@@ -2219,8 +2775,12 @@
       <c r="D127" s="4">
         <v>27458625451.310001</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="4">
+        <f t="shared" si="1"/>
+        <v>47081053140.339996</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>44012</v>
       </c>
@@ -2233,8 +2793,12 @@
       <c r="D128" s="4">
         <v>27604176824.200001</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="4">
+        <f t="shared" si="1"/>
+        <v>47426479912.610001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>44043</v>
       </c>
@@ -2247,8 +2811,12 @@
       <c r="D129" s="4">
         <v>28739709723.02</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="4">
+        <f t="shared" si="1"/>
+        <v>49195581002.360001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>44074</v>
       </c>
@@ -2261,8 +2829,12 @@
       <c r="D130" s="4">
         <v>28157559771.860001</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="4">
+        <f t="shared" si="1"/>
+        <v>48906000373.669998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>44104</v>
       </c>
@@ -2275,8 +2847,12 @@
       <c r="D131" s="4">
         <v>27927113005.669998</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="4">
+        <f t="shared" ref="E131:E146" si="2">SUM(B131,C131,D131)</f>
+        <v>49328610123.339996</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>44135</v>
       </c>
@@ -2289,8 +2865,12 @@
       <c r="D132" s="4">
         <v>27087051809.869999</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="4">
+        <f t="shared" si="2"/>
+        <v>48025973012.379997</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>44165</v>
       </c>
@@ -2303,8 +2883,12 @@
       <c r="D133" s="4">
         <v>28190375144.73</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="4">
+        <f t="shared" si="2"/>
+        <v>50439922757.960007</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>44196</v>
       </c>
@@ -2317,8 +2901,12 @@
       <c r="D134" s="4">
         <v>28978673408.57</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="4">
+        <f t="shared" si="2"/>
+        <v>52788406154.489998</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>44227</v>
       </c>
@@ -2331,8 +2919,12 @@
       <c r="D135" s="4">
         <v>28129381368.68</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="4">
+        <f t="shared" si="2"/>
+        <v>51587924289.860001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>44255</v>
       </c>
@@ -2345,8 +2937,12 @@
       <c r="D136" s="4">
         <v>27127339708.720001</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="4">
+        <f t="shared" si="2"/>
+        <v>50499267741.220001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>44286</v>
       </c>
@@ -2359,8 +2955,12 @@
       <c r="D137" s="4">
         <v>26762917954.490002</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="4">
+        <f t="shared" si="2"/>
+        <v>50392639291.639999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>44316</v>
       </c>
@@ -2373,8 +2973,12 @@
       <c r="D138" s="4">
         <v>27451228205.639999</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="4">
+        <f t="shared" si="2"/>
+        <v>51700906918.139999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>44347</v>
       </c>
@@ -2387,8 +2991,12 @@
       <c r="D139" s="4">
         <v>27744608720.27</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="4">
+        <f t="shared" si="2"/>
+        <v>52378479915.339996</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>44377</v>
       </c>
@@ -2401,8 +3009,12 @@
       <c r="D140" s="4">
         <v>28450323789.220001</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="4">
+        <f t="shared" si="2"/>
+        <v>53479086658.270004</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>44408</v>
       </c>
@@ -2415,8 +3027,12 @@
       <c r="D141" s="4">
         <v>29059023657.560001</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="4">
+        <f t="shared" si="2"/>
+        <v>54428674790.350006</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>44439</v>
       </c>
@@ -2429,8 +3045,12 @@
       <c r="D142" s="4">
         <v>29181824781.040001</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="4">
+        <f t="shared" si="2"/>
+        <v>54870263825.589996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>44469</v>
       </c>
@@ -2443,8 +3063,12 @@
       <c r="D143" s="4">
         <v>28189152287.09</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="4">
+        <f t="shared" si="2"/>
+        <v>52900976752.919998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>44500</v>
       </c>
@@ -2457,8 +3081,12 @@
       <c r="D144" s="4">
         <v>28782352603.84</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="4">
+        <f t="shared" si="2"/>
+        <v>54300695591.470001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>44530</v>
       </c>
@@ -2471,8 +3099,12 @@
       <c r="D145" s="4">
         <v>29177585592.27</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="4">
+        <f t="shared" si="2"/>
+        <v>55089285603.900002</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>44561</v>
       </c>
@@ -2485,12 +3117,16 @@
       <c r="D146" s="4">
         <v>29368978607.23</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="4">
+        <f t="shared" si="2"/>
+        <v>55524799409.729996</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C147" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A142">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A142">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2498,21 +3134,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2526,7 +3162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>39478</v>
       </c>
@@ -2537,7 +3173,7 @@
         <v>-3.8365000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>39507</v>
       </c>
@@ -2551,7 +3187,7 @@
         <v>-7.5599999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>39538</v>
       </c>
@@ -2565,7 +3201,7 @@
         <v>-6.9950000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>39568</v>
       </c>
@@ -2579,7 +3215,7 @@
         <v>2.7694E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>39599</v>
       </c>
@@ -2593,7 +3229,7 @@
         <v>7.6380000000000007E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>39629</v>
       </c>
@@ -2607,7 +3243,7 @@
         <v>-4.6011000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>39660</v>
       </c>
@@ -2621,7 +3257,7 @@
         <v>-1.4590000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>39691</v>
       </c>
@@ -2635,7 +3271,7 @@
         <v>5.04E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>39721</v>
       </c>
@@ -2649,7 +3285,7 @@
         <v>-7.9836000000000004E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>39752</v>
       </c>
@@ -2663,7 +3299,7 @@
         <v>-0.121084</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>39782</v>
       </c>
@@ -2677,7 +3313,7 @@
         <v>-1.4885000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>39813</v>
       </c>
@@ -2691,7 +3327,7 @@
         <v>2.8576000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>39844</v>
       </c>
@@ -2705,7 +3341,7 @@
         <v>-5.5410000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>39872</v>
       </c>
@@ -2719,7 +3355,7 @@
         <v>-5.4608999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>39903</v>
       </c>
@@ -2733,7 +3369,7 @@
         <v>2.3186999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>39933</v>
       </c>
@@ -2747,7 +3383,7 @@
         <v>4.6708999999999987E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>39964</v>
       </c>
@@ -2761,7 +3397,7 @@
         <v>4.0049000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>39994</v>
       </c>
@@ -2775,7 +3411,7 @@
         <v>3.3969999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>40025</v>
       </c>
@@ -2789,7 +3425,7 @@
         <v>5.4760999999999997E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>40056</v>
       </c>
@@ -2803,7 +3439,7 @@
         <v>2.6283999999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>40086</v>
       </c>
@@ -2817,7 +3453,7 @@
         <v>3.2212999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>40117</v>
       </c>
@@ -2831,7 +3467,7 @@
         <v>-1.3511E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>40147</v>
       </c>
@@ -2845,7 +3481,7 @@
         <v>2.9205999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>40178</v>
       </c>
@@ -2859,7 +3495,7 @@
         <v>1.2245000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>40209</v>
       </c>
@@ -2873,7 +3509,7 @@
         <v>-1.3906E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>40237</v>
       </c>
@@ -2887,7 +3523,7 @@
         <v>1.3596E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>40268</v>
       </c>
@@ -2901,7 +3537,7 @@
         <v>3.9373999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>40298</v>
       </c>
@@ -2915,7 +3551,7 @@
         <v>2.1406000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>40329</v>
       </c>
@@ -2929,7 +3565,7 @@
         <v>-4.2691999999999987E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>40359</v>
       </c>
@@ -2943,7 +3579,7 @@
         <v>-1.0512000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>40390</v>
       </c>
@@ -2957,7 +3593,7 @@
         <v>4.3425000000000012E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>40421</v>
       </c>
@@ -2971,7 +3607,7 @@
         <v>1.5499999999999999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>40451</v>
       </c>
@@ -2985,7 +3621,7 @@
         <v>4.5331000000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>40482</v>
       </c>
@@ -2999,7 +3635,7 @@
         <v>9.7619999999999998E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>40512</v>
       </c>
@@ -3013,7 +3649,7 @@
         <v>-6.3109999999999998E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>40543</v>
       </c>
@@ -3027,7 +3663,7 @@
         <v>2.9354000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>40574</v>
       </c>
@@ -3041,7 +3677,7 @@
         <v>-1.1150000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>40602</v>
       </c>
@@ -3055,7 +3691,7 @@
         <v>2.3307999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>40633</v>
       </c>
@@ -3069,7 +3705,7 @@
         <v>2.4940000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40663</v>
       </c>
@@ -3083,7 +3719,7 @@
         <v>3.0134000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>40694</v>
       </c>
@@ -3097,7 +3733,7 @@
         <v>6.2509999999999996E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>40724</v>
       </c>
@@ -3111,7 +3747,7 @@
         <v>-1.6388E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>40755</v>
       </c>
@@ -3125,7 +3761,7 @@
         <v>1.0779E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>40786</v>
       </c>
@@ -3139,7 +3775,7 @@
         <v>-6.4880000000000007E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>40816</v>
       </c>
@@ -3153,7 +3789,7 @@
         <v>1.2030000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>40847</v>
       </c>
@@ -3167,7 +3803,7 @@
         <v>3.5729999999999998E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>40877</v>
       </c>
@@ -3181,7 +3817,7 @@
         <v>-6.8320000000000004E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>40908</v>
       </c>
@@ -3195,7 +3831,7 @@
         <v>1.1629E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>40939</v>
       </c>
@@ -3209,7 +3845,7 @@
         <v>2.7751000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>40968</v>
       </c>
@@ -3223,7 +3859,7 @@
         <v>1.8407E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>40999</v>
       </c>
@@ -3237,7 +3873,7 @@
         <v>-3.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>41029</v>
       </c>
@@ -3251,7 +3887,7 @@
         <v>1.0168999999999999E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>41060</v>
       </c>
@@ -3265,7 +3901,7 @@
         <v>-7.1130000000000004E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>41090</v>
       </c>
@@ -3279,7 +3915,7 @@
         <v>1.3662000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>41121</v>
       </c>
@@ -3293,7 +3929,7 @@
         <v>2.2415000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>41152</v>
       </c>
@@ -3307,7 +3943,7 @@
         <v>6.5459999999999997E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>41182</v>
       </c>
@@ -3321,7 +3957,7 @@
         <v>8.5970000000000005E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>41213</v>
       </c>
@@ -3335,7 +3971,7 @@
         <v>1.505E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>41243</v>
       </c>
@@ -3349,7 +3985,7 @@
         <v>7.5709999999999996E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>41274</v>
       </c>
@@ -3363,7 +3999,7 @@
         <v>8.1650000000000004E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>41305</v>
       </c>
@@ -3377,7 +4013,7 @@
         <v>1.3455999999999999E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>41333</v>
       </c>
@@ -3391,7 +4027,7 @@
         <v>7.4700000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>41364</v>
       </c>
@@ -3405,7 +4041,7 @@
         <v>1.5023999999999999E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>41394</v>
       </c>
@@ -3419,7 +4055,7 @@
         <v>2.5086000000000001E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>41425</v>
       </c>
@@ -3433,7 +4069,7 @@
         <v>-1.6670000000000001E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>41455</v>
       </c>
@@ -3447,7 +4083,7 @@
         <v>-1.8159999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>41486</v>
       </c>
@@ -3461,7 +4097,7 @@
         <v>1.4252000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>41517</v>
       </c>
@@ -3475,7 +4111,7 @@
         <v>-1.1036000000000001E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>41547</v>
       </c>
@@ -3489,7 +4125,7 @@
         <v>2.0114E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>41578</v>
       </c>
@@ -3503,7 +4139,7 @@
         <v>2.2227E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>41608</v>
       </c>
@@ -3517,7 +4153,7 @@
         <v>1.66E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>41639</v>
       </c>
@@ -3531,7 +4167,7 @@
         <v>7.3099999999999997E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>41670</v>
       </c>
@@ -3545,7 +4181,7 @@
         <v>1.8710000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>41698</v>
       </c>
@@ -3559,7 +4195,7 @@
         <v>2.2973E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>41729</v>
       </c>
@@ -3573,7 +4209,7 @@
         <v>7.5810000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>41759</v>
       </c>
@@ -3587,7 +4223,7 @@
         <v>2.565E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>41790</v>
       </c>
@@ -3601,7 +4237,7 @@
         <v>1.8616000000000001E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>41820</v>
       </c>
@@ -3615,7 +4251,7 @@
         <v>7.5900000000000004E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>41851</v>
       </c>
@@ -3629,7 +4265,7 @@
         <v>-3.5339999999999998E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>41882</v>
       </c>
@@ -3643,7 +4279,7 @@
         <v>2.4400000000000002E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>41912</v>
       </c>
@@ -3657,7 +4293,7 @@
         <v>-1.8789E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>41943</v>
       </c>
@@ -3671,7 +4307,7 @@
         <v>1.2253999999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>41973</v>
       </c>
@@ -3685,7 +4321,7 @@
         <v>1.6820000000000002E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>42004</v>
       </c>
@@ -3699,7 +4335,7 @@
         <v>2.0799999999999998E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>42035</v>
       </c>
@@ -3713,7 +4349,7 @@
         <v>2.3349999999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>42063</v>
       </c>
@@ -3727,7 +4363,7 @@
         <v>7.6709999999999999E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>42094</v>
       </c>
@@ -3741,7 +4377,7 @@
         <v>7.2499999999999995E-4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>42124</v>
       </c>
@@ -3755,7 +4391,7 @@
         <v>4.8299999999999998E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>42155</v>
       </c>
@@ -3769,7 +4405,7 @@
         <v>-1.4469999999999999E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>42185</v>
       </c>
@@ -3783,7 +4419,7 @@
         <v>-1.9127000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>42216</v>
       </c>
@@ -3797,7 +4433,7 @@
         <v>1.0714E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>42247</v>
       </c>
@@ -3811,7 +4447,7 @@
         <v>-2.7125E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>42277</v>
       </c>
@@ -3825,7 +4461,7 @@
         <v>-8.7589999999999994E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>42308</v>
       </c>
@@ -3839,7 +4475,7 @@
         <v>2.8798000000000001E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>42338</v>
       </c>
@@ -3853,7 +4489,7 @@
         <v>-3.8070000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>42369</v>
       </c>
@@ -3867,7 +4503,7 @@
         <v>-8.1840000000000003E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>42400</v>
       </c>
@@ -3881,7 +4517,7 @@
         <v>-1.4826000000000001E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>42429</v>
       </c>
@@ -3895,7 +4531,7 @@
         <v>7.1509999999999994E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>42460</v>
       </c>
@@ -3909,7 +4545,7 @@
         <v>3.4733E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>42490</v>
       </c>
@@ -3923,7 +4559,7 @@
         <v>9.2420000000000002E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>42521</v>
       </c>
@@ -3937,7 +4573,7 @@
         <v>1.884E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>42551</v>
       </c>
@@ -3951,7 +4587,7 @@
         <v>1.013E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>42582</v>
       </c>
@@ -3965,7 +4601,7 @@
         <v>2.1264000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>42613</v>
       </c>
@@ -3979,7 +4615,7 @@
         <v>1.1460000000000001E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>42643</v>
       </c>
@@ -3993,7 +4629,7 @@
         <v>8.3000000000000001E-4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>42674</v>
       </c>
@@ -4007,7 +4643,7 @@
         <v>-1.1778E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>42704</v>
       </c>
@@ -4021,7 +4657,7 @@
         <v>-1.1501000000000001E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>42735</v>
       </c>
@@ -4035,7 +4671,7 @@
         <v>1.0142999999999999E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>42766</v>
       </c>
@@ -4049,7 +4685,7 @@
         <v>1.1658E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>42794</v>
       </c>
@@ -4063,7 +4699,7 @@
         <v>1.7676999999999998E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>42825</v>
       </c>
@@ -4077,7 +4713,7 @@
         <v>5.195E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>42855</v>
       </c>
@@ -4091,7 +4727,7 @@
         <v>1.3598000000000001E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>42886</v>
       </c>
@@ -4105,7 +4741,7 @@
         <v>1.5262E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>42916</v>
       </c>
@@ -4119,7 +4755,7 @@
         <v>5.2639999999999996E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>42947</v>
       </c>
@@ -4133,7 +4769,7 @@
         <v>1.1306E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>42978</v>
       </c>
@@ -4147,7 +4783,7 @@
         <v>1.0725E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>43008</v>
       </c>
@@ -4161,7 +4797,7 @@
         <v>8.1069999999999996E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>43039</v>
       </c>
@@ -4175,7 +4811,7 @@
         <v>1.1963E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>43069</v>
       </c>
@@ -4189,7 +4825,7 @@
         <v>1.3356E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>43100</v>
       </c>
@@ -4203,7 +4839,7 @@
         <v>1.1977E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>43131</v>
       </c>
@@ -4217,7 +4853,7 @@
         <v>1.6299000000000001E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>43159</v>
       </c>
@@ -4231,7 +4867,7 @@
         <v>-2.9905000000000001E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>43190</v>
       </c>
@@ -4245,7 +4881,7 @@
         <v>8.9589999999999999E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>43220</v>
       </c>
@@ -4259,7 +4895,7 @@
         <v>-6.6360000000000004E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>43251</v>
       </c>
@@ -4273,7 +4909,7 @@
         <v>1.0673E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>43281</v>
       </c>
@@ -4287,7 +4923,7 @@
         <v>-1.519E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>43312</v>
       </c>
@@ -4301,7 +4937,7 @@
         <v>5.8109999999999993E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>43343</v>
       </c>
@@ -4315,7 +4951,7 @@
         <v>1.0220999999999999E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>43373</v>
       </c>
@@ -4329,7 +4965,7 @@
         <v>-1.1547E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>43404</v>
       </c>
@@ -4343,7 +4979,7 @@
         <v>-3.9562E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>43434</v>
       </c>
@@ -4357,7 +4993,7 @@
         <v>1.3939E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>43465</v>
       </c>
@@ -4371,7 +5007,7 @@
         <v>5.9259999999999998E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>43496</v>
       </c>
@@ -4385,7 +5021,7 @@
         <v>2.8361999999999998E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>43524</v>
       </c>
@@ -4399,7 +5035,7 @@
         <v>2.9329999999999998E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>43555</v>
       </c>
@@ -4413,7 +5049,7 @@
         <v>3.2959000000000002E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>43585</v>
       </c>
@@ -4427,7 +5063,7 @@
         <v>1.077E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>43616</v>
       </c>
@@ -4441,7 +5077,7 @@
         <v>2.0518999999999999E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>43646</v>
       </c>
@@ -4455,7 +5091,7 @@
         <v>2.6977999999999999E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>43677</v>
       </c>
@@ -4469,7 +5105,7 @@
         <v>4.3940000000000003E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>43708</v>
       </c>
@@ -4483,7 +5119,7 @@
         <v>5.8720000000000001E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>43738</v>
       </c>
@@ -4497,7 +5133,7 @@
         <v>-9.6229999999999996E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>43769</v>
       </c>
@@ -4511,7 +5147,7 @@
         <v>-1.5300000000000001E-4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>43799</v>
       </c>
@@ -4525,7 +5161,7 @@
         <v>6.3489999999999996E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>43830</v>
       </c>
@@ -4539,7 +5175,7 @@
         <v>-7.5079999999999999E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>43861</v>
       </c>
@@ -4553,7 +5189,7 @@
         <v>3.7941999999999997E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" s="2">
         <v>43890</v>
       </c>
@@ -4567,7 +5203,7 @@
         <v>1.8638999999999999E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>43921</v>
       </c>
@@ -4581,7 +5217,7 @@
         <v>-1.2191E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="2">
         <v>43951</v>
       </c>
@@ -4595,7 +5231,7 @@
         <v>3.7446E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" s="2">
         <v>43982</v>
       </c>
@@ -4609,7 +5245,7 @@
         <v>-4.5329999999999997E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="2">
         <v>44012</v>
       </c>
@@ -4623,7 +5259,7 @@
         <v>8.5900000000000004E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="2">
         <v>44043</v>
       </c>
@@ -4637,7 +5273,7 @@
         <v>4.4461000000000001E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="2">
         <v>44074</v>
       </c>
@@ -4651,7 +5287,7 @@
         <v>-1.7264999999999999E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="2">
         <v>44104</v>
       </c>
@@ -4665,7 +5301,7 @@
         <v>-5.0549999999999996E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="2">
         <v>44135</v>
       </c>
@@ -4679,7 +5315,7 @@
         <v>-2.3545E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="2">
         <v>44165</v>
       </c>
@@ -4693,7 +5329,7 @@
         <v>4.4108000000000001E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="2">
         <v>44196</v>
       </c>
@@ -4707,7 +5343,7 @@
         <v>7.5290000000000001E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" s="2">
         <v>44227</v>
       </c>
@@ -4721,7 +5357,7 @@
         <v>-2.63E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" s="2">
         <v>44255</v>
       </c>
@@ -4735,7 +5371,7 @@
         <v>-3.2485E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="2">
         <v>44286</v>
       </c>
@@ -4749,7 +5385,7 @@
         <v>-1.0056000000000001E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" s="2">
         <v>44316</v>
       </c>
@@ -4763,7 +5399,7 @@
         <v>2.9309000000000002E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" s="2">
         <v>44347</v>
       </c>
@@ -4777,7 +5413,7 @@
         <v>1.4168E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" s="2">
         <v>44377</v>
       </c>
@@ -4791,7 +5427,7 @@
         <v>2.8979999999999999E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="2">
         <v>44408</v>
       </c>
@@ -4805,7 +5441,7 @@
         <v>2.4878999999999998E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="2">
         <v>44439</v>
       </c>
@@ -4819,7 +5455,7 @@
         <v>7.5929999999999999E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" s="2">
         <v>44469</v>
       </c>
@@ -4833,7 +5469,7 @@
         <v>-3.0726E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" s="2">
         <v>44500</v>
       </c>
@@ -4847,7 +5483,7 @@
         <v>2.7293999999999999E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" s="2">
         <v>44530</v>
       </c>
@@ -4861,7 +5497,7 @@
         <v>1.7181999999999999E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="2">
         <v>44561</v>
       </c>
@@ -4875,7 +5511,7 @@
         <v>5.3790000000000001E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C170" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add back misc receivs to retirement and total mvs
</commit_message>
<xml_diff>
--- a/data/time_series/plan_data.xlsx
+++ b/data/time_series/plan_data.xlsx
@@ -454,10 +454,10 @@
         <v>2102497497.95</v>
       </c>
       <c r="D2" s="1">
-        <v>12454714514.06</v>
+        <v>12454906728.13</v>
       </c>
       <c r="E2" s="1">
-        <v>15489729218.43</v>
+        <v>15489921432.5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -471,10 +471,10 @@
         <v>2128528078.25</v>
       </c>
       <c r="D3" s="1">
-        <v>12582416484.82</v>
+        <v>12582607840.79</v>
       </c>
       <c r="E3" s="1">
-        <v>15775048697.14</v>
+        <v>15775240053.11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -488,10 +488,10 @@
         <v>2204069195.06</v>
       </c>
       <c r="D4" s="1">
-        <v>13025662728.84</v>
+        <v>13025853226.71</v>
       </c>
       <c r="E4" s="1">
-        <v>16704873758.75</v>
+        <v>16705064256.62</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -505,10 +505,10 @@
         <v>2249160289.73</v>
       </c>
       <c r="D5" s="1">
-        <v>13260440725.69</v>
+        <v>13260630365.46</v>
       </c>
       <c r="E5" s="1">
-        <v>17132130003.51</v>
+        <v>17132319643.28</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -522,10 +522,10 @@
         <v>2151316976.44</v>
       </c>
       <c r="D6" s="1">
-        <v>12652381383.56</v>
+        <v>12652570165.23</v>
       </c>
       <c r="E6" s="1">
-        <v>16351241876.8</v>
+        <v>16351430658.47</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -539,10 +539,10 @@
         <v>2126807551.94</v>
       </c>
       <c r="D7" s="1">
-        <v>12475038374.8</v>
+        <v>12475226298.37</v>
       </c>
       <c r="E7" s="1">
-        <v>16127227316.29</v>
+        <v>16127415239.86</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -556,10 +556,10 @@
         <v>2217049566.92</v>
       </c>
       <c r="D8" s="1">
-        <v>12970168980.82</v>
+        <v>12970356046.29</v>
       </c>
       <c r="E8" s="1">
-        <v>16894210925.62</v>
+        <v>16894397991.09</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -573,10 +573,10 @@
         <v>2218270319.77</v>
       </c>
       <c r="D9" s="1">
-        <v>12942973012.13</v>
+        <v>12943159219.5</v>
       </c>
       <c r="E9" s="1">
-        <v>16864762411.98</v>
+        <v>16864948619.35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -590,10 +590,10 @@
         <v>2429501039.02</v>
       </c>
       <c r="D10" s="1">
-        <v>13480205460.32</v>
+        <v>13480390809.59</v>
       </c>
       <c r="E10" s="1">
-        <v>17683853962.58</v>
+        <v>17684039311.85</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -607,10 +607,10 @@
         <v>2451294838.87</v>
       </c>
       <c r="D11" s="1">
-        <v>13443063041.03</v>
+        <v>13443247532.2</v>
       </c>
       <c r="E11" s="1">
-        <v>17795005221.62</v>
+        <v>17795189712.79</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -624,10 +624,10 @@
         <v>2932628117.61</v>
       </c>
       <c r="D12" s="1">
-        <v>14814700195.87</v>
+        <v>14814883828.94</v>
       </c>
       <c r="E12" s="1">
-        <v>19628314376.71</v>
+        <v>19628498009.78</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -641,10 +641,10 @@
         <v>3016301371.7</v>
       </c>
       <c r="D13" s="1">
-        <v>15090047197.56</v>
+        <v>15090229972.53</v>
       </c>
       <c r="E13" s="1">
-        <v>20035126948.73</v>
+        <v>20035309723.7</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -658,10 +658,10 @@
         <v>3010941131.67</v>
       </c>
       <c r="D14" s="1">
-        <v>15034722562.56</v>
+        <v>15034904479.43</v>
       </c>
       <c r="E14" s="1">
-        <v>21163701726.8</v>
+        <v>21163883643.67</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -675,10 +675,10 @@
         <v>3072606771.41</v>
       </c>
       <c r="D15" s="1">
-        <v>15339223946.43</v>
+        <v>15339405005.2</v>
       </c>
       <c r="E15" s="1">
-        <v>21592868236.35</v>
+        <v>21593049295.12</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -692,10 +692,10 @@
         <v>3077934373.48</v>
       </c>
       <c r="D16" s="1">
-        <v>15338075937.65</v>
+        <v>15338256138.32</v>
       </c>
       <c r="E16" s="1">
-        <v>21597393553.6</v>
+        <v>21597573754.27</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -709,10 +709,10 @@
         <v>3168259937.35</v>
       </c>
       <c r="D17" s="1">
-        <v>15759188122.62</v>
+        <v>15759367465.19</v>
       </c>
       <c r="E17" s="1">
-        <v>22196442158.83</v>
+        <v>22196621501.4</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -726,10 +726,10 @@
         <v>3185699769.88</v>
       </c>
       <c r="D18" s="1">
-        <v>15817399042.18</v>
+        <v>15817577526.65</v>
       </c>
       <c r="E18" s="1">
-        <v>22284623894.07</v>
+        <v>22284802378.54</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -743,10 +743,10 @@
         <v>3131056633.27</v>
       </c>
       <c r="D19" s="1">
-        <v>15518354156.14</v>
+        <v>15518531782.51</v>
       </c>
       <c r="E19" s="1">
-        <v>21869129586.24</v>
+        <v>21869307212.61</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -760,10 +760,10 @@
         <v>3162162793.97</v>
       </c>
       <c r="D20" s="1">
-        <v>15643951036.32</v>
+        <v>15644127804.59</v>
       </c>
       <c r="E20" s="1">
-        <v>22052015022.44</v>
+        <v>22052191790.71</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -777,10 +777,10 @@
         <v>3139082692.54</v>
       </c>
       <c r="D21" s="1">
-        <v>15501631744.31</v>
+        <v>15501807654.48</v>
       </c>
       <c r="E21" s="1">
-        <v>21857152498.61</v>
+        <v>21857328408.78</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -794,10 +794,10 @@
         <v>3200272417.15</v>
       </c>
       <c r="D22" s="1">
-        <v>15478669634.76</v>
+        <v>15478844686.83</v>
       </c>
       <c r="E22" s="1">
-        <v>21890587182.54</v>
+        <v>21890762234.61</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -811,10 +811,10 @@
         <v>3311931768.5</v>
       </c>
       <c r="D23" s="1">
-        <v>15988684918.42</v>
+        <v>15988859112.39</v>
       </c>
       <c r="E23" s="1">
-        <v>22617832290.32</v>
+        <v>22618006484.29</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -828,10 +828,10 @@
         <v>3286738232.03</v>
       </c>
       <c r="D24" s="1">
-        <v>15838131556.61</v>
+        <v>15838304892.48</v>
       </c>
       <c r="E24" s="1">
-        <v>22404660643.81</v>
+        <v>22404833979.68</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -845,10 +845,10 @@
         <v>3322199318.6</v>
       </c>
       <c r="D25" s="1">
-        <v>15979851739.54</v>
+        <v>15980024217.31</v>
       </c>
       <c r="E25" s="1">
-        <v>22610566714.97</v>
+        <v>22610739192.74</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -862,10 +862,10 @@
         <v>3411636959.78</v>
       </c>
       <c r="D26" s="1">
-        <v>16380190274.37</v>
+        <v>16380361894.04</v>
       </c>
       <c r="E26" s="1">
-        <v>23182541487.51</v>
+        <v>23182713107.18</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -879,10 +879,10 @@
         <v>3465240303.9</v>
       </c>
       <c r="D27" s="1">
-        <v>16632293380.49</v>
+        <v>16632464142.06</v>
       </c>
       <c r="E27" s="1">
-        <v>23538890877.4</v>
+        <v>23539061638.97</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -896,10 +896,10 @@
         <v>3448893913.05</v>
       </c>
       <c r="D28" s="1">
-        <v>16525290668.17</v>
+        <v>16525460571.64</v>
       </c>
       <c r="E28" s="1">
-        <v>23568457835.1</v>
+        <v>23568627738.57</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -913,10 +913,10 @@
         <v>3481026300.12</v>
       </c>
       <c r="D29" s="1">
-        <v>16649048720.64</v>
+        <v>16649217766.01</v>
       </c>
       <c r="E29" s="1">
-        <v>23750894239.67</v>
+        <v>23751063285.04</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -930,10 +930,10 @@
         <v>3453190328.12</v>
       </c>
       <c r="D30" s="1">
-        <v>16487003754.48</v>
+        <v>16487171941.75</v>
       </c>
       <c r="E30" s="1">
-        <v>23525188092.25</v>
+        <v>23525356279.52</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -947,10 +947,10 @@
         <v>3497243829.13</v>
       </c>
       <c r="D31" s="1">
-        <v>16666683230.14</v>
+        <v>16666850559.31</v>
       </c>
       <c r="E31" s="1">
-        <v>23966952669.71</v>
+        <v>23967119998.88</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -964,10 +964,10 @@
         <v>3572637746.48</v>
       </c>
       <c r="D32" s="1">
-        <v>16994661825.91</v>
+        <v>16994828296.98</v>
       </c>
       <c r="E32" s="1">
-        <v>24445028323.78</v>
+        <v>24445194794.85</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -981,10 +981,10 @@
         <v>3592909103.41</v>
       </c>
       <c r="D33" s="1">
-        <v>17060740670.37</v>
+        <v>17060906283.34</v>
       </c>
       <c r="E33" s="1">
-        <v>24546173849.48</v>
+        <v>24546339462.45</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -998,10 +998,10 @@
         <v>3620604152.58</v>
       </c>
       <c r="D34" s="1">
-        <v>17161797379.67</v>
+        <v>17161962134.54</v>
       </c>
       <c r="E34" s="1">
-        <v>24697695785.05</v>
+        <v>24697860539.92</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1015,10 +1015,10 @@
         <v>3622924774.95</v>
       </c>
       <c r="D35" s="1">
-        <v>17142269583.37</v>
+        <v>17142433480.14</v>
       </c>
       <c r="E35" s="1">
-        <v>24675625120.17</v>
+        <v>24675789016.94</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1032,10 +1032,10 @@
         <v>3646999015.16</v>
       </c>
       <c r="D36" s="1">
-        <v>17226232669.72</v>
+        <v>17226395708.39</v>
       </c>
       <c r="E36" s="1">
-        <v>24802249901.28</v>
+        <v>24802412939.95</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1049,10 +1049,10 @@
         <v>3654809047.65</v>
       </c>
       <c r="D37" s="1">
-        <v>17291185714.26</v>
+        <v>17291347894.83</v>
       </c>
       <c r="E37" s="1">
-        <v>24895725823.46</v>
+        <v>24895888004.03</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1066,10 +1066,10 @@
         <v>4490569394.41</v>
       </c>
       <c r="D38" s="1">
-        <v>16688192891.54</v>
+        <v>16688354214.01</v>
       </c>
       <c r="E38" s="1">
-        <v>25170361391.66</v>
+        <v>25170522714.13</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1083,10 +1083,10 @@
         <v>4511270646.88</v>
       </c>
       <c r="D39" s="1">
-        <v>16760318931.09</v>
+        <v>16760479395.46</v>
       </c>
       <c r="E39" s="1">
-        <v>25279056931.75</v>
+        <v>25279217396.12</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1100,10 +1100,10 @@
         <v>4573664426.03</v>
       </c>
       <c r="D40" s="1">
-        <v>16965972358.16</v>
+        <v>16966131964.43</v>
       </c>
       <c r="E40" s="1">
-        <v>25595461395.49</v>
+        <v>25595621001.76</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1117,10 +1117,10 @@
         <v>4682846886.27</v>
       </c>
       <c r="D41" s="1">
-        <v>17344551325.7</v>
+        <v>17344710073.87</v>
       </c>
       <c r="E41" s="1">
-        <v>26172807411.43</v>
+        <v>26172966159.6</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1134,10 +1134,10 @@
         <v>4599347535.9</v>
       </c>
       <c r="D42" s="1">
-        <v>17009919681.78</v>
+        <v>17010077571.85</v>
       </c>
       <c r="E42" s="1">
-        <v>25673836920.31</v>
+        <v>25673994810.38</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1151,10 +1151,10 @@
         <v>4510251396.91</v>
       </c>
       <c r="D43" s="1">
-        <v>16655048859.38</v>
+        <v>16655205891.35</v>
       </c>
       <c r="E43" s="1">
-        <v>25144097226.38</v>
+        <v>25144254258.35</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1168,10 +1168,10 @@
         <v>4568724212.7</v>
       </c>
       <c r="D44" s="1">
-        <v>16844754449.47</v>
+        <v>16844910623.34</v>
       </c>
       <c r="E44" s="1">
-        <v>25436535483.03</v>
+        <v>25436691656.9</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1185,10 +1185,10 @@
         <v>4512507452.03</v>
       </c>
       <c r="D45" s="1">
-        <v>16611704230.01</v>
+        <v>16611859545.78</v>
       </c>
       <c r="E45" s="1">
-        <v>25090551978.14</v>
+        <v>25090707293.91</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1202,10 +1202,10 @@
         <v>4749762591.53</v>
       </c>
       <c r="D46" s="1">
-        <v>16745140477.25</v>
+        <v>16745294934.92</v>
       </c>
       <c r="E46" s="1">
-        <v>25528342822.26</v>
+        <v>25528497279.93</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1219,10 +1219,10 @@
         <v>4848589342.72</v>
       </c>
       <c r="D47" s="1">
-        <v>17068600956.34</v>
+        <v>17068754555.91</v>
       </c>
       <c r="E47" s="1">
-        <v>26027210514.61</v>
+        <v>26027364114.18</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1236,10 +1236,10 @@
         <v>4850653743.4</v>
       </c>
       <c r="D48" s="1">
-        <v>17048811459.13</v>
+        <v>17048964200.6</v>
       </c>
       <c r="E48" s="1">
-        <v>26003668184.25</v>
+        <v>26003820925.72</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1253,10 +1253,10 @@
         <v>4879983265.38</v>
       </c>
       <c r="D49" s="1">
-        <v>17124920453.7</v>
+        <v>17125072337.07</v>
       </c>
       <c r="E49" s="1">
-        <v>26126136558.37</v>
+        <v>26126288441.74</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1270,10 +1270,10 @@
         <v>4882894726.29</v>
       </c>
       <c r="D50" s="1">
-        <v>17108427415.48</v>
+        <v>17108578440.75</v>
       </c>
       <c r="E50" s="1">
-        <v>26107545286.21</v>
+        <v>26107696311.48</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1287,10 +1287,10 @@
         <v>4988729007.27</v>
       </c>
       <c r="D51" s="1">
-        <v>17452044700.37</v>
+        <v>17452194867.54</v>
       </c>
       <c r="E51" s="1">
-        <v>26638014657</v>
+        <v>26638164824.17</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1304,10 +1304,10 @@
         <v>5019984158.58</v>
       </c>
       <c r="D52" s="1">
-        <v>17534458681.87</v>
+        <v>17534607990.94</v>
       </c>
       <c r="E52" s="1">
-        <v>26769907188.32</v>
+        <v>26770056497.39</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1321,10 +1321,10 @@
         <v>5026144812.31</v>
       </c>
       <c r="D53" s="1">
-        <v>17527323843.17</v>
+        <v>17527472294.14</v>
       </c>
       <c r="E53" s="1">
-        <v>26765961123.21</v>
+        <v>26766109574.18</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1338,10 +1338,10 @@
         <v>5112975530.56</v>
       </c>
       <c r="D54" s="1">
-        <v>17802031711.89</v>
+        <v>17802179304.76</v>
       </c>
       <c r="E54" s="1">
-        <v>27191839755.38</v>
+        <v>27191987348.25</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1355,10 +1355,10 @@
         <v>5144862372.52</v>
       </c>
       <c r="D55" s="1">
-        <v>17885536456.36</v>
+        <v>17885683191.13</v>
       </c>
       <c r="E55" s="1">
-        <v>27325539811.99</v>
+        <v>27325686546.76</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1372,10 +1372,10 @@
         <v>5119794037.99</v>
       </c>
       <c r="D56" s="1">
-        <v>17771447283.1</v>
+        <v>17771593159.77</v>
       </c>
       <c r="E56" s="1">
-        <v>27156693166.09</v>
+        <v>27156839042.76</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1389,10 +1389,10 @@
         <v>5237452701.82</v>
       </c>
       <c r="D57" s="1">
-        <v>18152061725.92</v>
+        <v>18152206744.49</v>
       </c>
       <c r="E57" s="1">
-        <v>27744061638.86</v>
+        <v>27744206657.43</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1406,10 +1406,10 @@
         <v>5131976211.71</v>
       </c>
       <c r="D58" s="1">
-        <v>17760389482.46</v>
+        <v>17760533642.93</v>
       </c>
       <c r="E58" s="1">
-        <v>27150516717.21</v>
+        <v>27150660877.68</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1423,10 +1423,10 @@
         <v>5172926233.01</v>
       </c>
       <c r="D59" s="1">
-        <v>17913492320.95</v>
+        <v>17913635623.32</v>
       </c>
       <c r="E59" s="1">
-        <v>27371582530.76</v>
+        <v>27371725833.13</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1440,10 +1440,10 @@
         <v>5252461885.84</v>
       </c>
       <c r="D60" s="1">
-        <v>18161633085.61</v>
+        <v>18161775529.88</v>
       </c>
       <c r="E60" s="1">
-        <v>27755791534.1</v>
+        <v>27755933978.37</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1457,10 +1457,10 @@
         <v>5448191101.38</v>
       </c>
       <c r="D61" s="1">
-        <v>18347484059.09</v>
+        <v>18347625645.26</v>
       </c>
       <c r="E61" s="1">
-        <v>28782286672.54</v>
+        <v>28782428258.71</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1474,10 +1474,10 @@
         <v>5567918737.12</v>
       </c>
       <c r="D62" s="1">
-        <v>18722609505.8</v>
+        <v>18722750233.87</v>
       </c>
       <c r="E62" s="1">
-        <v>29377893373.27</v>
+        <v>29378034101.34</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1491,10 +1491,10 @@
         <v>5603210665.94</v>
       </c>
       <c r="D63" s="1">
-        <v>18813632546.84</v>
+        <v>18813772416.81</v>
       </c>
       <c r="E63" s="1">
-        <v>29527582270.6</v>
+        <v>29527722140.57</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1508,10 +1508,10 @@
         <v>5599621915.28</v>
       </c>
       <c r="D64" s="1">
-        <v>18773915353.1</v>
+        <v>18774054364.97</v>
       </c>
       <c r="E64" s="1">
-        <v>29472066114.92</v>
+        <v>29472205126.79</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1525,10 +1525,10 @@
         <v>5594550723.83</v>
       </c>
       <c r="D65" s="1">
-        <v>18729047234.33</v>
+        <v>18729185388.1</v>
       </c>
       <c r="E65" s="1">
-        <v>29408499309.23</v>
+        <v>29408637463</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1542,10 +1542,10 @@
         <v>5578675769.67</v>
       </c>
       <c r="D66" s="1">
-        <v>18647811742.49</v>
+        <v>18647949038.16</v>
       </c>
       <c r="E66" s="1">
-        <v>29287873259.31</v>
+        <v>29288010554.98</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1559,10 +1559,10 @@
         <v>5464086350.67</v>
       </c>
       <c r="D67" s="1">
-        <v>18237344817.24</v>
+        <v>18237481254.81</v>
       </c>
       <c r="E67" s="1">
-        <v>28649880311.46</v>
+        <v>28650016749.03</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1576,10 +1576,10 @@
         <v>5514366076.03</v>
       </c>
       <c r="D68" s="1">
-        <v>18376949304.2</v>
+        <v>18377084883.67</v>
       </c>
       <c r="E68" s="1">
-        <v>28876049490.89</v>
+        <v>28876185070.36</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1593,10 +1593,10 @@
         <v>5356648129.15</v>
       </c>
       <c r="D69" s="1">
-        <v>17823822010.27</v>
+        <v>17823956731.64</v>
       </c>
       <c r="E69" s="1">
-        <v>28013794466.53</v>
+        <v>28013929187.9</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1610,10 +1610,10 @@
         <v>5301454591.47</v>
       </c>
       <c r="D70" s="1">
-        <v>17611674082.8</v>
+        <v>17611807946.07</v>
       </c>
       <c r="E70" s="1">
-        <v>27687481033.78</v>
+        <v>27687614897.05</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1627,10 +1627,10 @@
         <v>5397632819.49</v>
       </c>
       <c r="D71" s="1">
-        <v>18048333376.56</v>
+        <v>18048466381.73</v>
       </c>
       <c r="E71" s="1">
-        <v>28326214032.7</v>
+        <v>28326347037.87</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1644,10 +1644,10 @@
         <v>5368571908.98</v>
       </c>
       <c r="D72" s="1">
-        <v>17923305130.99</v>
+        <v>17923437278.06</v>
       </c>
       <c r="E72" s="1">
-        <v>28136428854.08</v>
+        <v>28136561001.15</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1661,10 +1661,10 @@
         <v>5709868087.27</v>
       </c>
       <c r="D73" s="1">
-        <v>17720678489.54</v>
+        <v>17720809778.51</v>
       </c>
       <c r="E73" s="1">
-        <v>28846123319.36</v>
+        <v>28846254608.33</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1678,10 +1678,10 @@
         <v>5616578571.14</v>
       </c>
       <c r="D74" s="1">
-        <v>17401580107.8</v>
+        <v>17401710538.67</v>
       </c>
       <c r="E74" s="1">
-        <v>28336242435.29</v>
+        <v>28336372866.16</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1695,10 +1695,10 @@
         <v>5647936294.45</v>
       </c>
       <c r="D75" s="1">
-        <v>17468918255.4</v>
+        <v>17469047828.17</v>
       </c>
       <c r="E75" s="1">
-        <v>28455548735.7</v>
+        <v>28455678308.47</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1712,10 +1712,10 @@
         <v>5834802926.8</v>
       </c>
       <c r="D76" s="1">
-        <v>18015825215.72</v>
+        <v>18015953930.39</v>
       </c>
       <c r="E76" s="1">
-        <v>29356543183.02</v>
+        <v>29356671897.69</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1729,10 +1729,10 @@
         <v>5879483219.72</v>
       </c>
       <c r="D77" s="1">
-        <v>18123427852.61</v>
+        <v>18123555709.18</v>
       </c>
       <c r="E77" s="1">
-        <v>29541899253.78</v>
+        <v>29542027110.35</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1746,10 +1746,10 @@
         <v>5881279255.87</v>
       </c>
       <c r="D78" s="1">
-        <v>18098420744.15</v>
+        <v>18098547742.62</v>
       </c>
       <c r="E78" s="1">
-        <v>29511294102.97</v>
+        <v>29511421101.44</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1763,10 +1763,10 @@
         <v>5931068967.2</v>
       </c>
       <c r="D79" s="1">
-        <v>18221304108.22</v>
+        <v>18221430248.59</v>
       </c>
       <c r="E79" s="1">
-        <v>29721707293.18</v>
+        <v>29721833433.55</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1780,10 +1780,10 @@
         <v>6047546128.94</v>
       </c>
       <c r="D80" s="1">
-        <v>18547786478.41</v>
+        <v>18547911760.68</v>
       </c>
       <c r="E80" s="1">
-        <v>30265017930.44</v>
+        <v>30265143212.71</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1797,10 +1797,10 @@
         <v>6044991482.23</v>
       </c>
       <c r="D81" s="1">
-        <v>18508832479.78</v>
+        <v>18508956903.95</v>
       </c>
       <c r="E81" s="1">
-        <v>30212130836.66</v>
+        <v>30212255260.83</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1814,10 +1814,10 @@
         <v>6489780168.17</v>
       </c>
       <c r="D82" s="1">
-        <v>18773993442.11</v>
+        <v>18774117008.18</v>
       </c>
       <c r="E82" s="1">
-        <v>31311065698.3</v>
+        <v>31311189264.37</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1831,10 +1831,10 @@
         <v>6361287062.33</v>
       </c>
       <c r="D83" s="1">
-        <v>18430042970.95</v>
+        <v>18430165678.92</v>
       </c>
       <c r="E83" s="1">
-        <v>30735579110.59</v>
+        <v>30735701818.56</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1848,10 +1848,10 @@
         <v>6278318762.68</v>
       </c>
       <c r="D84" s="1">
-        <v>18157757460.24</v>
+        <v>18157879310.11</v>
       </c>
       <c r="E84" s="1">
-        <v>30294027553</v>
+        <v>30294149402.87</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1865,10 +1865,10 @@
         <v>6361809245.25</v>
       </c>
       <c r="D85" s="1">
-        <v>18519115493.09</v>
+        <v>18519236484.86</v>
       </c>
       <c r="E85" s="1">
-        <v>31134438714.84</v>
+        <v>31134559706.61</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1882,10 +1882,10 @@
         <v>6425317655.9</v>
       </c>
       <c r="D86" s="1">
-        <v>18672728045.69</v>
+        <v>18672848179.36</v>
       </c>
       <c r="E86" s="1">
-        <v>31406508587.93</v>
+        <v>31406628721.6</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1899,10 +1899,10 @@
         <v>6526279467.15</v>
       </c>
       <c r="D87" s="1">
-        <v>18935552854.39</v>
+        <v>18935672129.96</v>
       </c>
       <c r="E87" s="1">
-        <v>31862808989.72</v>
+        <v>31862928265.29</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1916,10 +1916,10 @@
         <v>7337629420.28</v>
       </c>
       <c r="D88" s="1">
-        <v>19799498475.64</v>
+        <v>19799616893.11</v>
       </c>
       <c r="E88" s="1">
-        <v>34237099341.94</v>
+        <v>34237217759.41</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1933,10 +1933,10 @@
         <v>7422733235.89</v>
       </c>
       <c r="D89" s="1">
-        <v>20002234967.92</v>
+        <v>20002352527.29</v>
       </c>
       <c r="E89" s="1">
-        <v>34601102374.35</v>
+        <v>34601219933.72</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1950,10 +1950,10 @@
         <v>7523682920.77</v>
       </c>
       <c r="D90" s="1">
-        <v>20236725707.75</v>
+        <v>20236842409.02</v>
       </c>
       <c r="E90" s="1">
-        <v>35025362965.57</v>
+        <v>35025479666.84</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1967,10 +1967,10 @@
         <v>7549356808.18</v>
       </c>
       <c r="D91" s="1">
-        <v>20274704112.17</v>
+        <v>20274819955.34</v>
       </c>
       <c r="E91" s="1">
-        <v>35106467417.43</v>
+        <v>35106583260.6</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1984,10 +1984,10 @@
         <v>7623588366.49</v>
       </c>
       <c r="D92" s="1">
-        <v>20438444305.61</v>
+        <v>20438559290.68</v>
       </c>
       <c r="E92" s="1">
-        <v>35405676882.5</v>
+        <v>35405791867.57</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2001,10 +2001,10 @@
         <v>7693916997.08</v>
       </c>
       <c r="D93" s="1">
-        <v>20590369678.54</v>
+        <v>20590483805.51</v>
       </c>
       <c r="E93" s="1">
-        <v>35685401140.06</v>
+        <v>35685515267.03</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2018,10 +2018,10 @@
         <v>7744728806.72</v>
       </c>
       <c r="D94" s="1">
-        <v>20690747320.22</v>
+        <v>20690860589.09</v>
       </c>
       <c r="E94" s="1">
-        <v>35874830645.56</v>
+        <v>35874943914.43</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2035,10 +2035,10 @@
         <v>7797612927.14</v>
       </c>
       <c r="D95" s="1">
-        <v>20816031800.59</v>
+        <v>20816144211.36</v>
       </c>
       <c r="E95" s="1">
-        <v>36114807334.97</v>
+        <v>36114919745.74</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2052,10 +2052,10 @@
         <v>7890046689.69</v>
       </c>
       <c r="D96" s="1">
-        <v>21026669979.09</v>
+        <v>21026781531.76</v>
       </c>
       <c r="E96" s="1">
-        <v>36495501947.44</v>
+        <v>36495613500.11</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2069,10 +2069,10 @@
         <v>8628245002.959999</v>
       </c>
       <c r="D97" s="1">
-        <v>24225492187.24</v>
+        <v>24225602881.81</v>
       </c>
       <c r="E97" s="1">
-        <v>41855947325.63</v>
+        <v>41856058020.2</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2086,10 +2086,10 @@
         <v>8830545061.309999</v>
       </c>
       <c r="D98" s="1">
-        <v>24550452831.88</v>
+        <v>24550562668.35</v>
       </c>
       <c r="E98" s="1">
-        <v>42583608483.91</v>
+        <v>42583718320.38</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2103,10 +2103,10 @@
         <v>8554843302.12</v>
       </c>
       <c r="D99" s="1">
-        <v>23751543939.11</v>
+        <v>23751652917.48</v>
       </c>
       <c r="E99" s="1">
-        <v>41211539283.34</v>
+        <v>41211648261.71</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2120,10 +2120,10 @@
         <v>8555117311.3</v>
       </c>
       <c r="D100" s="1">
-        <v>23895593642.49</v>
+        <v>23895701762.76</v>
       </c>
       <c r="E100" s="1">
-        <v>41345361923.7</v>
+        <v>41345470043.96999</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2137,10 +2137,10 @@
         <v>8525561703.78</v>
       </c>
       <c r="D101" s="1">
-        <v>23668065334.8</v>
+        <v>23668172596.97</v>
       </c>
       <c r="E101" s="1">
-        <v>41046653376.56</v>
+        <v>41046760638.73</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2154,10 +2154,10 @@
         <v>8572549061.9</v>
       </c>
       <c r="D102" s="1">
-        <v>23850014619.05</v>
+        <v>23850121023.12</v>
       </c>
       <c r="E102" s="1">
-        <v>41313125652.08</v>
+        <v>41313232056.15</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2171,10 +2171,10 @@
         <v>8535731069.89</v>
       </c>
       <c r="D103" s="1">
-        <v>23743724505.99</v>
+        <v>23743830051.96</v>
       </c>
       <c r="E103" s="1">
-        <v>41120926179.03</v>
+        <v>41121031725</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2188,10 +2188,10 @@
         <v>8637933457.639999</v>
       </c>
       <c r="D104" s="1">
-        <v>23810476668.13</v>
+        <v>23810581356</v>
       </c>
       <c r="E104" s="1">
-        <v>41384483579.77</v>
+        <v>41384588267.64</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2205,10 +2205,10 @@
         <v>8696018228.42</v>
       </c>
       <c r="D105" s="1">
-        <v>23982305364.47</v>
+        <v>23982409194.24</v>
       </c>
       <c r="E105" s="1">
-        <v>41662699191.55</v>
+        <v>41662803021.32</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2222,10 +2222,10 @@
         <v>8639086304.16</v>
       </c>
       <c r="D106" s="1">
-        <v>23633877037.77</v>
+        <v>23633980009.44</v>
       </c>
       <c r="E106" s="1">
-        <v>41186844593.33</v>
+        <v>41186947565</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2239,10 +2239,10 @@
         <v>8244001106.42</v>
       </c>
       <c r="D107" s="1">
-        <v>22616086896.59</v>
+        <v>22616189010.16</v>
       </c>
       <c r="E107" s="1">
-        <v>39382932997.41</v>
+        <v>39383035110.98</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2256,10 +2256,10 @@
         <v>8324970365.95</v>
       </c>
       <c r="D108" s="1">
-        <v>22855316166.62</v>
+        <v>22855417422.09</v>
       </c>
       <c r="E108" s="1">
-        <v>39775062674.71</v>
+        <v>39775163930.18</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2273,10 +2273,10 @@
         <v>8177279951.57</v>
       </c>
       <c r="D109" s="1">
-        <v>22914691512.65</v>
+        <v>22914791910.02</v>
       </c>
       <c r="E109" s="1">
-        <v>39522884974.1</v>
+        <v>39522985371.47</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2290,10 +2290,10 @@
         <v>8466374243.34</v>
       </c>
       <c r="D110" s="1">
-        <v>23486649000.34</v>
+        <v>23486748539.61</v>
       </c>
       <c r="E110" s="1">
-        <v>40669954095.65</v>
+        <v>40670053634.92</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2307,10 +2307,10 @@
         <v>8538970109.85</v>
       </c>
       <c r="D111" s="1">
-        <v>23478741957.66</v>
+        <v>23478840638.83</v>
       </c>
       <c r="E111" s="1">
-        <v>40797714345.53</v>
+        <v>40797813026.7</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2324,10 +2324,10 @@
         <v>8705342961.4</v>
       </c>
       <c r="D112" s="1">
-        <v>24171159309.13</v>
+        <v>24171257132.2</v>
       </c>
       <c r="E112" s="1">
-        <v>41816004324.67</v>
+        <v>41816102147.74</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2341,10 +2341,10 @@
         <v>9126959379.24</v>
       </c>
       <c r="D113" s="1">
-        <v>24607805892.51</v>
+        <v>24607902857.48</v>
       </c>
       <c r="E113" s="1">
-        <v>42743010048.03</v>
+        <v>42743107013</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2358,10 +2358,10 @@
         <v>9074029379.02</v>
       </c>
       <c r="D114" s="1">
-        <v>25031219112.64</v>
+        <v>25031315219.51</v>
       </c>
       <c r="E114" s="1">
-        <v>43049509347.52</v>
+        <v>43049605454.39</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2375,10 +2375,10 @@
         <v>9361706609.469999</v>
       </c>
       <c r="D115" s="1">
-        <v>25624099438.36</v>
+        <v>25624194687.13</v>
       </c>
       <c r="E115" s="1">
-        <v>44201801916.78</v>
+        <v>44201897165.55</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2392,10 +2392,10 @@
         <v>9396108735.549999</v>
       </c>
       <c r="D116" s="1">
-        <v>25654690308.73</v>
+        <v>25654784699.4</v>
       </c>
       <c r="E116" s="1">
-        <v>44289184114.95</v>
+        <v>44289278505.62</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2409,10 +2409,10 @@
         <v>9608738306.559999</v>
       </c>
       <c r="D117" s="1">
-        <v>27075142517.6</v>
+        <v>27075236050.17</v>
       </c>
       <c r="E117" s="1">
-        <v>46120218348.73</v>
+        <v>46120311881.3</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2426,10 +2426,10 @@
         <v>9614794478.780001</v>
       </c>
       <c r="D118" s="1">
-        <v>26732490993.1</v>
+        <v>26732583667.57</v>
       </c>
       <c r="E118" s="1">
-        <v>46949500920.5</v>
+        <v>46949593594.97</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2443,10 +2443,10 @@
         <v>9625407467.91</v>
       </c>
       <c r="D119" s="1">
-        <v>26631956752.71</v>
+        <v>26632048569.08</v>
       </c>
       <c r="E119" s="1">
-        <v>46865616845.86</v>
+        <v>46865708662.23</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2460,10 +2460,10 @@
         <v>9713037686.17</v>
       </c>
       <c r="D120" s="1">
-        <v>26718171624.69</v>
+        <v>26718262582.96</v>
       </c>
       <c r="E120" s="1">
-        <v>47123526214.26</v>
+        <v>47123617172.53</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2477,10 +2477,10 @@
         <v>9477691033.26</v>
       </c>
       <c r="D121" s="1">
-        <v>25905410180.56</v>
+        <v>25905500280.73</v>
       </c>
       <c r="E121" s="1">
-        <v>46141543427.79</v>
+        <v>46141633527.96</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2494,10 +2494,10 @@
         <v>9555218261.01</v>
       </c>
       <c r="D122" s="1">
-        <v>26801714204.06</v>
+        <v>26801803446.13</v>
       </c>
       <c r="E122" s="1">
-        <v>47197571777.95</v>
+        <v>47197661020.02</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2511,10 +2511,10 @@
         <v>9338936485.4</v>
       </c>
       <c r="D123" s="1">
-        <v>27210513709.58</v>
+        <v>27210602093.55</v>
       </c>
       <c r="E123" s="1">
-        <v>47123736418.86</v>
+        <v>47123824802.83</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2528,10 +2528,10 @@
         <v>8664875030.02</v>
       </c>
       <c r="D124" s="1">
-        <v>26774758277.92</v>
+        <v>26774845803.79</v>
       </c>
       <c r="E124" s="1">
-        <v>45203938859.3</v>
+        <v>45204026385.17001</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2545,10 +2545,10 @@
         <v>9107006952.52</v>
       </c>
       <c r="D125" s="1">
-        <v>27673823035.06</v>
+        <v>27673909702.83</v>
       </c>
       <c r="E125" s="1">
-        <v>47063924664.94</v>
+        <v>47064011332.71</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2562,10 +2562,10 @@
         <v>9213245024.98</v>
       </c>
       <c r="D126" s="1">
-        <v>27458625451.31</v>
+        <v>27458711260.98</v>
       </c>
       <c r="E126" s="1">
-        <v>47081053140.34</v>
+        <v>47081138950.00999</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2579,10 +2579,10 @@
         <v>9308097696.17</v>
       </c>
       <c r="D127" s="1">
-        <v>27604176824.2</v>
+        <v>27604261775.77</v>
       </c>
       <c r="E127" s="1">
-        <v>47426479912.61</v>
+        <v>47426564864.18</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2596,10 +2596,10 @@
         <v>9606421868.530001</v>
       </c>
       <c r="D128" s="1">
-        <v>28739709723.02</v>
+        <v>28739793816.49</v>
       </c>
       <c r="E128" s="1">
-        <v>49195581002.36</v>
+        <v>49195665095.83</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -2613,10 +2613,10 @@
         <v>9743289163.68</v>
       </c>
       <c r="D129" s="1">
-        <v>28157559771.86</v>
+        <v>28157643007.23</v>
       </c>
       <c r="E129" s="1">
-        <v>48906000373.67</v>
+        <v>48906083609.04</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -2630,10 +2630,10 @@
         <v>9894562298.549999</v>
       </c>
       <c r="D130" s="1">
-        <v>27927113005.67</v>
+        <v>27927195382.94</v>
       </c>
       <c r="E130" s="1">
-        <v>49328610123.34</v>
+        <v>49328692500.60999</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2647,10 +2647,10 @@
         <v>9700328704.629999</v>
       </c>
       <c r="D131" s="1">
-        <v>27087051809.87</v>
+        <v>27087133329.04</v>
       </c>
       <c r="E131" s="1">
-        <v>48025973012.38</v>
+        <v>48026054531.55</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2664,10 +2664,10 @@
         <v>10308274207.78</v>
       </c>
       <c r="D132" s="1">
-        <v>28190375144.73</v>
+        <v>28190455805.8</v>
       </c>
       <c r="E132" s="1">
-        <v>50439922757.96</v>
+        <v>50440003419.03</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2681,10 +2681,10 @@
         <v>11053433125.61</v>
       </c>
       <c r="D133" s="1">
-        <v>28978673408.57</v>
+        <v>28978753211.54</v>
       </c>
       <c r="E133" s="1">
-        <v>52788406154.49</v>
+        <v>52788485957.46</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -2698,10 +2698,10 @@
         <v>10900299506.57</v>
       </c>
       <c r="D134" s="1">
-        <v>28129381368.68</v>
+        <v>28129460313.55</v>
       </c>
       <c r="E134" s="1">
-        <v>51587924289.86</v>
+        <v>51588003234.73</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2715,10 +2715,10 @@
         <v>10872197550.37</v>
       </c>
       <c r="D135" s="1">
-        <v>27127339708.72</v>
+        <v>27127417795.49</v>
       </c>
       <c r="E135" s="1">
-        <v>50499267741.22</v>
+        <v>50499345827.99</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -2732,10 +2732,10 @@
         <v>10999754121.32</v>
       </c>
       <c r="D136" s="1">
-        <v>26762917954.49</v>
+        <v>26762995183.16</v>
       </c>
       <c r="E136" s="1">
-        <v>50392639291.64</v>
+        <v>50392716520.31</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2749,10 +2749,10 @@
         <v>11290601383.86</v>
       </c>
       <c r="D137" s="1">
-        <v>27451228205.64</v>
+        <v>27451304576.21</v>
       </c>
       <c r="E137" s="1">
-        <v>51700906918.14</v>
+        <v>51700983288.71</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -2766,10 +2766,10 @@
         <v>11478701164.89</v>
       </c>
       <c r="D138" s="1">
-        <v>27744608720.27</v>
+        <v>27744684232.74</v>
       </c>
       <c r="E138" s="1">
-        <v>52378479915.34</v>
+        <v>52378555427.81</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -2783,10 +2783,10 @@
         <v>11665454270.74</v>
       </c>
       <c r="D139" s="1">
-        <v>28450323789.22</v>
+        <v>28450398443.59</v>
       </c>
       <c r="E139" s="1">
-        <v>53479086658.27</v>
+        <v>53479161312.64</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2800,10 +2800,10 @@
         <v>11826970568.32</v>
       </c>
       <c r="D140" s="1">
-        <v>29059023657.56</v>
+        <v>29059097453.83</v>
       </c>
       <c r="E140" s="1">
-        <v>54428674790.35</v>
+        <v>54428748586.62</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2817,10 +2817,10 @@
         <v>11980671064.48</v>
       </c>
       <c r="D141" s="1">
-        <v>29181824781.04</v>
+        <v>29181897719.21</v>
       </c>
       <c r="E141" s="1">
-        <v>54870263825.59</v>
+        <v>54870336763.75999</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2834,10 +2834,10 @@
         <v>11508277149.59</v>
       </c>
       <c r="D142" s="1">
-        <v>28189152287.09</v>
+        <v>28189224367.16</v>
       </c>
       <c r="E142" s="1">
-        <v>52900976752.92</v>
+        <v>52901048832.99</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2851,10 +2851,10 @@
         <v>11898653834.64</v>
       </c>
       <c r="D143" s="1">
-        <v>28782352603.84</v>
+        <v>28782423825.81</v>
       </c>
       <c r="E143" s="1">
-        <v>54300695591.47</v>
+        <v>54300766813.44</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -2868,10 +2868,10 @@
         <v>12126631727.77</v>
       </c>
       <c r="D144" s="1">
-        <v>29177585592.27</v>
+        <v>29177655956.14</v>
       </c>
       <c r="E144" s="1">
-        <v>55089285603.9</v>
+        <v>55089355967.77</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -2885,10 +2885,10 @@
         <v>12222321130.28</v>
       </c>
       <c r="D145" s="1">
-        <v>29368978607.23</v>
+        <v>29369048113</v>
       </c>
       <c r="E145" s="1">
-        <v>55524799409.73</v>
+        <v>55524868915.5</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -2902,10 +2902,10 @@
         <v>11573834300.94</v>
       </c>
       <c r="D146" s="1">
-        <v>27989441863.54</v>
+        <v>27989510511.21</v>
       </c>
       <c r="E146" s="1">
-        <v>52791326720.55</v>
+        <v>52791395368.22</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -2919,10 +2919,10 @@
         <v>11299022364.73</v>
       </c>
       <c r="D147" s="1">
-        <v>27409938257.91</v>
+        <v>27410006047.48</v>
       </c>
       <c r="E147" s="1">
-        <v>51633196749.2</v>
+        <v>51633264538.77</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2936,10 +2936,10 @@
         <v>11031166589.13</v>
       </c>
       <c r="D148" s="1">
-        <v>26576281073.84</v>
+        <v>26576348005.31</v>
       </c>
       <c r="E148" s="1">
-        <v>50270219077.72</v>
+        <v>50270286009.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ldi data 9/30/2023
</commit_message>
<xml_diff>
--- a/data/time_series/plan_data.xlsx
+++ b/data/time_series/plan_data.xlsx
@@ -417,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM147"/>
+  <dimension ref="A1:ALM148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2925,13 +2925,30 @@
         <v>42632156030.68</v>
       </c>
     </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="3">
+        <v>45199</v>
+      </c>
+      <c r="B148" s="1">
+        <v>11184939337.99</v>
+      </c>
+      <c r="C148" s="1">
+        <v>8923504755.17</v>
+      </c>
+      <c r="D148" s="1">
+        <v>20040354305.93</v>
+      </c>
+      <c r="E148" s="1">
+        <v>40148798399.09</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A147">
+  <conditionalFormatting sqref="A1:A148">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E147">
+  <conditionalFormatting sqref="B2:E148">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
@@ -2942,7 +2959,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM147"/>
+  <dimension ref="A1:ALM148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5450,13 +5467,30 @@
         <v>-0.023792</v>
       </c>
     </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="3">
+        <v>45199</v>
+      </c>
+      <c r="B148" s="1">
+        <v>-0.051322</v>
+      </c>
+      <c r="C148" s="1">
+        <v>-0.056463</v>
+      </c>
+      <c r="D148" s="1">
+        <v>-0.05521</v>
+      </c>
+      <c r="E148" s="1">
+        <v>-0.054409</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A147">
+  <conditionalFormatting sqref="A1:A148">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E147">
+  <conditionalFormatting sqref="B2:E148">
     <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update LDI data 9/30 with UPS GT data
</commit_message>
<xml_diff>
--- a/data/time_series/plan_data.xlsx
+++ b/data/time_series/plan_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>IBT</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Total Consolidation</t>
   </si>
   <si>
     <t>Date</t>
@@ -426,9 +429,9 @@
     <col min="1" max="1001" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -442,8 +445,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>40755</v>
       </c>
@@ -459,8 +465,11 @@
       <c r="E2" s="1">
         <v>22052191790.71</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1">
+        <v>22231555271.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>40786</v>
       </c>
@@ -476,8 +485,11 @@
       <c r="E3" s="1">
         <v>21857328408.78</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1">
+        <v>22027918799.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>40816</v>
       </c>
@@ -493,8 +505,11 @@
       <c r="E4" s="1">
         <v>21890762234.61</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1">
+        <v>22052849274.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>40847</v>
       </c>
@@ -510,8 +525,11 @@
       <c r="E5" s="1">
         <v>22618006484.29</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="1">
+        <v>22778089729.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>40877</v>
       </c>
@@ -527,8 +545,11 @@
       <c r="E6" s="1">
         <v>22404833979.68</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="1">
+        <v>22555336103.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>40908</v>
       </c>
@@ -544,8 +565,11 @@
       <c r="E7" s="1">
         <v>22610739192.74</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="1">
+        <v>22760627152.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="3">
         <v>40939</v>
       </c>
@@ -561,8 +585,11 @@
       <c r="E8" s="1">
         <v>23182713107.18</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="1">
+        <v>23327836945.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>40968</v>
       </c>
@@ -578,8 +605,11 @@
       <c r="E9" s="1">
         <v>23539061638.97</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="1">
+        <v>23683533132.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3">
         <v>40999</v>
       </c>
@@ -595,8 +625,11 @@
       <c r="E10" s="1">
         <v>23568627738.57</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="1">
+        <v>23527415369.76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>41029</v>
       </c>
@@ -612,8 +645,11 @@
       <c r="E11" s="1">
         <v>23751063285.04</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="1">
+        <v>23878250766.57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3">
         <v>41060</v>
       </c>
@@ -629,8 +665,11 @@
       <c r="E12" s="1">
         <v>23525356279.52</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="1">
+        <v>23642315685.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3">
         <v>41090</v>
       </c>
@@ -646,8 +685,11 @@
       <c r="E13" s="1">
         <v>23967119998.88</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="1">
+        <v>23898064813.57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="3">
         <v>41121</v>
       </c>
@@ -663,8 +705,11 @@
       <c r="E14" s="1">
         <v>24445194794.85</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="1">
+        <v>24549514764.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="3">
         <v>41152</v>
       </c>
@@ -680,8 +725,11 @@
       <c r="E15" s="1">
         <v>24546339462.45</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="1">
+        <v>24642500384.21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="3">
         <v>41182</v>
       </c>
@@ -697,8 +745,11 @@
       <c r="E16" s="1">
         <v>24697860539.92</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="1">
+        <v>25154181675.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="3">
         <v>41213</v>
       </c>
@@ -714,8 +765,11 @@
       <c r="E17" s="1">
         <v>24675789016.94</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="1">
+        <v>25125272400.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3">
         <v>41243</v>
       </c>
@@ -731,8 +785,11 @@
       <c r="E18" s="1">
         <v>24802412939.95</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="1">
+        <v>25245243669.78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3">
         <v>41274</v>
       </c>
@@ -748,8 +805,11 @@
       <c r="E19" s="1">
         <v>24895888004.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="1">
+        <v>25331489787.35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>41305</v>
       </c>
@@ -765,8 +825,11 @@
       <c r="E20" s="1">
         <v>25170522714.13</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="1">
+        <v>26333049791.22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3">
         <v>41333</v>
       </c>
@@ -782,8 +845,11 @@
       <c r="E21" s="1">
         <v>25279217396.12</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="1">
+        <v>26437887737.61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>41364</v>
       </c>
@@ -799,8 +865,11 @@
       <c r="E22" s="1">
         <v>25595621001.76</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="1">
+        <v>26762244859.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="3">
         <v>41394</v>
       </c>
@@ -816,8 +885,11 @@
       <c r="E23" s="1">
         <v>26172966159.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="1">
+        <v>27354266269.36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="3">
         <v>41425</v>
       </c>
@@ -833,8 +905,11 @@
       <c r="E24" s="1">
         <v>25673994810.38</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="1">
+        <v>26825680454.21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <v>41455</v>
       </c>
@@ -850,8 +925,11 @@
       <c r="E25" s="1">
         <v>25144254258.35</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="1">
+        <v>26265676510.43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
         <v>41486</v>
       </c>
@@ -867,8 +945,11 @@
       <c r="E26" s="1">
         <v>25436691656.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="1">
+        <v>26565709631.94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="3">
         <v>41517</v>
       </c>
@@ -884,8 +965,11 @@
       <c r="E27" s="1">
         <v>25090707293.91</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="1">
+        <v>26201572226.35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="3">
         <v>41547</v>
       </c>
@@ -901,8 +985,11 @@
       <c r="E28" s="1">
         <v>25528497279.93</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="1">
+        <v>26650940234.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="3">
         <v>41578</v>
       </c>
@@ -918,8 +1005,11 @@
       <c r="E29" s="1">
         <v>26027364114.18</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="1">
+        <v>27164746657.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="3">
         <v>41608</v>
       </c>
@@ -935,8 +1025,11 @@
       <c r="E30" s="1">
         <v>26003820925.72</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="1">
+        <v>27132210456.28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="3">
         <v>41639</v>
       </c>
@@ -952,8 +1045,11 @@
       <c r="E31" s="1">
         <v>26126288441.74</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="1">
+        <v>27253687582.98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="3">
         <v>41670</v>
       </c>
@@ -969,8 +1065,11 @@
       <c r="E32" s="1">
         <v>26107696311.48</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="1">
+        <v>27226639980.42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3">
         <v>41698</v>
       </c>
@@ -986,8 +1085,11 @@
       <c r="E33" s="1">
         <v>26638164824.17</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="1">
+        <v>27769593035.21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="3">
         <v>41729</v>
       </c>
@@ -1003,8 +1105,11 @@
       <c r="E34" s="1">
         <v>26770056497.39</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="1">
+        <v>27900602168.04</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="3">
         <v>41759</v>
       </c>
@@ -1020,8 +1125,11 @@
       <c r="E35" s="1">
         <v>26766109574.18</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="1">
+        <v>27889292662.49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="3">
         <v>41790</v>
       </c>
@@ -1037,8 +1145,11 @@
       <c r="E36" s="1">
         <v>27191987348.25</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="1">
+        <v>28325272289.23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="3">
         <v>41820</v>
       </c>
@@ -1054,8 +1165,11 @@
       <c r="E37" s="1">
         <v>27325686546.76</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="1">
+        <v>28472678681.56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="3">
         <v>41851</v>
       </c>
@@ -1071,8 +1185,11 @@
       <c r="E38" s="1">
         <v>27156839042.76</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="1">
+        <v>28289948331.18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="3">
         <v>41882</v>
       </c>
@@ -1088,8 +1205,11 @@
       <c r="E39" s="1">
         <v>27744206657.43</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="1">
+        <v>28894470491.79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="3">
         <v>41912</v>
       </c>
@@ -1105,8 +1225,11 @@
       <c r="E40" s="1">
         <v>27150660877.68</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="1">
+        <v>28271789225.71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="3">
         <v>41943</v>
       </c>
@@ -1122,8 +1245,11 @@
       <c r="E41" s="1">
         <v>27371725833.13</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="1">
+        <v>28498525017</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="3">
         <v>41973</v>
       </c>
@@ -1139,8 +1265,11 @@
       <c r="E42" s="1">
         <v>27755933978.37</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="1">
+        <v>28890460746.39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="3">
         <v>42004</v>
       </c>
@@ -1156,8 +1285,11 @@
       <c r="E43" s="1">
         <v>28782428258.71</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="1">
+        <v>29909163526.79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="3">
         <v>42035</v>
       </c>
@@ -1173,8 +1305,11 @@
       <c r="E44" s="1">
         <v>29378034101.34</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="1">
+        <v>30520363399.73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="3">
         <v>42063</v>
       </c>
@@ -1190,8 +1325,11 @@
       <c r="E45" s="1">
         <v>29527722140.57</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="1">
+        <v>30682678579.16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="3">
         <v>42094</v>
       </c>
@@ -1207,8 +1345,11 @@
       <c r="E46" s="1">
         <v>29472205126.79</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="1">
+        <v>30617803151.79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="3">
         <v>42124</v>
       </c>
@@ -1224,8 +1365,11 @@
       <c r="E47" s="1">
         <v>29408637463</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="1">
+        <v>30544085686.26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="3">
         <v>42155</v>
       </c>
@@ -1241,8 +1385,11 @@
       <c r="E48" s="1">
         <v>29288010554.98</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="1">
+        <v>30411241858.39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="3">
         <v>42185</v>
       </c>
@@ -1258,8 +1405,11 @@
       <c r="E49" s="1">
         <v>28650016749.03</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="1">
+        <v>29741788892.27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="3">
         <v>42216</v>
       </c>
@@ -1275,8 +1425,11 @@
       <c r="E50" s="1">
         <v>28876185070.36</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="1">
+        <v>29968273775.33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="3">
         <v>42247</v>
       </c>
@@ -1292,8 +1445,11 @@
       <c r="E51" s="1">
         <v>28013929187.9</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="1">
+        <v>29066322305.74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="3">
         <v>42277</v>
       </c>
@@ -1309,8 +1465,11 @@
       <c r="E52" s="1">
         <v>27687614897.05</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="1">
+        <v>28720022246.88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="3">
         <v>42308</v>
       </c>
@@ -1326,8 +1485,11 @@
       <c r="E53" s="1">
         <v>28326347037.87</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="1">
+        <v>29360507839.81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="3">
         <v>42338</v>
       </c>
@@ -1343,8 +1505,11 @@
       <c r="E54" s="1">
         <v>28136561001.15</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="1">
+        <v>29172575288.71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="3">
         <v>42369</v>
       </c>
@@ -1360,8 +1525,11 @@
       <c r="E55" s="1">
         <v>28846254608.33</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="1">
+        <v>29862597627.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="3">
         <v>42400</v>
       </c>
@@ -1377,8 +1545,11 @@
       <c r="E56" s="1">
         <v>28336372866.16</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="1">
+        <v>29326075448.69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="3">
         <v>42429</v>
       </c>
@@ -1394,8 +1565,11 @@
       <c r="E57" s="1">
         <v>28455678308.47</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="1">
+        <v>29440765726.48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="3">
         <v>42460</v>
       </c>
@@ -1411,8 +1585,11 @@
       <c r="E58" s="1">
         <v>29356671897.69</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="1">
+        <v>30362580685</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="3">
         <v>42490</v>
       </c>
@@ -1428,8 +1605,11 @@
       <c r="E59" s="1">
         <v>29542027110.35</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="1">
+        <v>30560223568.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="3">
         <v>42521</v>
       </c>
@@ -1445,8 +1625,11 @@
       <c r="E60" s="1">
         <v>29511421101.44</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="1">
+        <v>30520464418.77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="3">
         <v>42551</v>
       </c>
@@ -1462,8 +1645,11 @@
       <c r="E61" s="1">
         <v>29721833433.55</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="1">
+        <v>30728992338.24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="3">
         <v>42582</v>
       </c>
@@ -1479,8 +1665,11 @@
       <c r="E62" s="1">
         <v>30265143212.71</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="1">
+        <v>31280132371.05</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="3">
         <v>42613</v>
       </c>
@@ -1496,8 +1685,11 @@
       <c r="E63" s="1">
         <v>30212255260.83</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="1">
+        <v>31218710837.63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="3">
         <v>42643</v>
       </c>
@@ -1513,8 +1705,11 @@
       <c r="E64" s="1">
         <v>31311189264.37</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="1">
+        <v>32306086725.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="3">
         <v>42674</v>
       </c>
@@ -1530,8 +1725,11 @@
       <c r="E65" s="1">
         <v>30735701818.56</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" s="1">
+        <v>31707560542.83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="3">
         <v>42704</v>
       </c>
@@ -1547,8 +1745,11 @@
       <c r="E66" s="1">
         <v>30294149402.87</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" s="1">
+        <v>31243895035.79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="3">
         <v>42735</v>
       </c>
@@ -1564,8 +1765,11 @@
       <c r="E67" s="1">
         <v>31134559706.61</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" s="1">
+        <v>31993862117.18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="3">
         <v>42766</v>
       </c>
@@ -1581,8 +1785,11 @@
       <c r="E68" s="1">
         <v>31406628721.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" s="1">
+        <v>32272409430.99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="3">
         <v>42794</v>
       </c>
@@ -1598,8 +1805,11 @@
       <c r="E69" s="1">
         <v>31862928265.29</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" s="1">
+        <v>32847863724.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="3">
         <v>42825</v>
       </c>
@@ -1615,8 +1825,11 @@
       <c r="E70" s="1">
         <v>34237217759.41</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70" s="1">
+        <v>35227095408.74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="3">
         <v>42855</v>
       </c>
@@ -1632,8 +1845,11 @@
       <c r="E71" s="1">
         <v>34601219933.72</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71" s="1">
+        <v>35605325711.35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="3">
         <v>42886</v>
       </c>
@@ -1649,8 +1865,11 @@
       <c r="E72" s="1">
         <v>35025479666.84</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72" s="1">
+        <v>36045330946.54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="3">
         <v>42916</v>
       </c>
@@ -1666,8 +1885,11 @@
       <c r="E73" s="1">
         <v>35106583260.6</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73" s="1">
+        <v>36131069554.68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="3">
         <v>42947</v>
       </c>
@@ -1683,8 +1905,11 @@
       <c r="E74" s="1">
         <v>35405791867.57</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" s="1">
+        <v>36440249931.02</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="3">
         <v>42978</v>
       </c>
@@ -1700,8 +1925,11 @@
       <c r="E75" s="1">
         <v>35685515267.03</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75" s="1">
+        <v>36731307884.26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="3">
         <v>43008</v>
       </c>
@@ -1717,8 +1945,11 @@
       <c r="E76" s="1">
         <v>35874943914.43</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76" s="1">
+        <v>36929261044</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="3">
         <v>43039</v>
       </c>
@@ -1734,8 +1965,11 @@
       <c r="E77" s="1">
         <v>36114919745.74</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77" s="1">
+        <v>37181963756.37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" s="3">
         <v>43069</v>
       </c>
@@ -1751,8 +1985,11 @@
       <c r="E78" s="1">
         <v>36495613500.11</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78" s="1">
+        <v>37576800847.56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="3">
         <v>43100</v>
       </c>
@@ -1768,8 +2005,11 @@
       <c r="E79" s="1">
         <v>41856058020.2</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79" s="1">
+        <v>37949036056.54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" s="3">
         <v>43131</v>
       </c>
@@ -1785,8 +2025,11 @@
       <c r="E80" s="1">
         <v>42583718320.38</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80" s="1">
+        <v>36126703368.99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="3">
         <v>43159</v>
       </c>
@@ -1802,8 +2045,11 @@
       <c r="E81" s="1">
         <v>41211648261.71</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" s="1">
+        <v>34947041283.19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="3">
         <v>43190</v>
       </c>
@@ -1819,8 +2065,11 @@
       <c r="E82" s="1">
         <v>41345470043.96999</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82" s="1">
+        <v>34893565647.81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="3">
         <v>43220</v>
       </c>
@@ -1836,8 +2085,11 @@
       <c r="E83" s="1">
         <v>41046760638.73</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83" s="1">
+        <v>34718322290.49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="3">
         <v>43251</v>
       </c>
@@ -1853,8 +2105,11 @@
       <c r="E84" s="1">
         <v>41313232056.15</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" s="1">
+        <v>34853430635.59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="3">
         <v>43281</v>
       </c>
@@ -1870,8 +2125,11 @@
       <c r="E85" s="1">
         <v>41121031725</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85" s="1">
+        <v>34649138195.13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="3">
         <v>43312</v>
       </c>
@@ -1887,8 +2145,11 @@
       <c r="E86" s="1">
         <v>41384588267.64</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86" s="1">
+        <v>35007279828.93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="3">
         <v>43343</v>
       </c>
@@ -1904,8 +2165,11 @@
       <c r="E87" s="1">
         <v>41662803021.32</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87" s="1">
+        <v>35185061352.95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="3">
         <v>43373</v>
       </c>
@@ -1921,8 +2185,11 @@
       <c r="E88" s="1">
         <v>41186947565</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88" s="1">
+        <v>34897241234.02</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="3">
         <v>43404</v>
       </c>
@@ -1938,8 +2205,11 @@
       <c r="E89" s="1">
         <v>39383035110.98</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89" s="1">
+        <v>33324461630.84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="3">
         <v>43434</v>
       </c>
@@ -1955,8 +2225,11 @@
       <c r="E90" s="1">
         <v>39775163930.18</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90" s="1">
+        <v>33590951046.18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="3">
         <v>43465</v>
       </c>
@@ -1972,8 +2245,11 @@
       <c r="E91" s="1">
         <v>39522985371.47</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91" s="1">
+        <v>32936056236.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="3">
         <v>43496</v>
       </c>
@@ -1989,8 +2265,11 @@
       <c r="E92" s="1">
         <v>40670053634.92</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92" s="1">
+        <v>34114984114.15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="3">
         <v>43524</v>
       </c>
@@ -2006,8 +2285,11 @@
       <c r="E93" s="1">
         <v>40797813026.7</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93" s="1">
+        <v>34345800814.97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="3">
         <v>43555</v>
       </c>
@@ -2023,8 +2305,11 @@
       <c r="E94" s="1">
         <v>41816102147.74</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94" s="1">
+        <v>34951519519.29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="3">
         <v>43585</v>
       </c>
@@ -2040,8 +2325,11 @@
       <c r="E95" s="1">
         <v>42743107013</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95" s="1">
+        <v>35544104423.43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="3">
         <v>43616</v>
       </c>
@@ -2057,8 +2345,11 @@
       <c r="E96" s="1">
         <v>43049605454.39</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" s="1">
+        <v>35353126027.34</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="3">
         <v>43646</v>
       </c>
@@ -2074,8 +2365,11 @@
       <c r="E97" s="1">
         <v>44201897165.55</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" s="1">
+        <v>36407955381.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="3">
         <v>43677</v>
       </c>
@@ -2091,8 +2385,11 @@
       <c r="E98" s="1">
         <v>44289278505.62</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" s="1">
+        <v>36475732007.89</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="3">
         <v>43708</v>
       </c>
@@ -2108,8 +2405,11 @@
       <c r="E99" s="1">
         <v>46120311881.3</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" s="1">
+        <v>37237277255.72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="3">
         <v>43738</v>
       </c>
@@ -2125,8 +2425,11 @@
       <c r="E100" s="1">
         <v>46949593594.97</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" s="1">
+        <v>37278149188.28</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="3">
         <v>43769</v>
       </c>
@@ -2142,8 +2445,11 @@
       <c r="E101" s="1">
         <v>46865708662.23</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" s="1">
+        <v>45620639518.53</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="3">
         <v>43799</v>
       </c>
@@ -2159,8 +2465,11 @@
       <c r="E102" s="1">
         <v>47123617172.53</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" s="1">
+        <v>46986534776.59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="3">
         <v>43830</v>
       </c>
@@ -2176,8 +2485,11 @@
       <c r="E103" s="1">
         <v>46141633527.96</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" s="1">
+        <v>46024238147.58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="3">
         <v>43861</v>
       </c>
@@ -2193,8 +2505,11 @@
       <c r="E104" s="1">
         <v>47197661020.02</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" s="1">
+        <v>47145264898.48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" s="3">
         <v>43890</v>
       </c>
@@ -2210,8 +2525,11 @@
       <c r="E105" s="1">
         <v>47123824802.83</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" s="1">
+        <v>47102840330.35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" s="3">
         <v>43921</v>
       </c>
@@ -2227,8 +2545,11 @@
       <c r="E106" s="1">
         <v>45204026385.17001</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" s="1">
+        <v>45203532515.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="3">
         <v>43951</v>
       </c>
@@ -2244,8 +2565,11 @@
       <c r="E107" s="1">
         <v>47064011332.71</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" s="1">
+        <v>47063659448.95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" s="3">
         <v>43982</v>
       </c>
@@ -2261,8 +2585,11 @@
       <c r="E108" s="1">
         <v>47081138950.00999</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" s="1">
+        <v>47080894938.3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" s="3">
         <v>44012</v>
       </c>
@@ -2278,8 +2605,11 @@
       <c r="E109" s="1">
         <v>47426564864.18</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" s="1">
+        <v>47425304505.7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" s="3">
         <v>44043</v>
       </c>
@@ -2295,8 +2625,11 @@
       <c r="E110" s="1">
         <v>49195665095.83</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" s="1">
+        <v>49191446952.15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="3">
         <v>44074</v>
       </c>
@@ -2312,8 +2645,11 @@
       <c r="E111" s="1">
         <v>48906083609.04</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" s="1">
+        <v>48904844973.57</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="3">
         <v>44104</v>
       </c>
@@ -2329,8 +2665,11 @@
       <c r="E112" s="1">
         <v>49328692500.60999</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112" s="1">
+        <v>49327891655.97</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" s="3">
         <v>44135</v>
       </c>
@@ -2346,8 +2685,11 @@
       <c r="E113" s="1">
         <v>48026054531.55</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113" s="1">
+        <v>48024908266.78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" s="3">
         <v>44165</v>
       </c>
@@ -2363,8 +2705,11 @@
       <c r="E114" s="1">
         <v>50440003419.03</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114" s="1">
+        <v>50438850250.79</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" s="3">
         <v>44196</v>
       </c>
@@ -2380,8 +2725,11 @@
       <c r="E115" s="1">
         <v>52788485957.46</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115" s="1">
+        <v>52787920332.11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" s="3">
         <v>44227</v>
       </c>
@@ -2397,8 +2745,11 @@
       <c r="E116" s="1">
         <v>51588003234.73</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" s="1">
+        <v>51586801167.14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" s="3">
         <v>44255</v>
       </c>
@@ -2414,8 +2765,11 @@
       <c r="E117" s="1">
         <v>50499345827.99</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" s="1">
+        <v>50498271333.38</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" s="3">
         <v>44286</v>
       </c>
@@ -2431,8 +2785,11 @@
       <c r="E118" s="1">
         <v>50392716520.31</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" s="1">
+        <v>50392459354.27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" s="3">
         <v>44316</v>
       </c>
@@ -2448,8 +2805,11 @@
       <c r="E119" s="1">
         <v>51700983288.71</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119" s="1">
+        <v>51699898092.8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="3">
         <v>44347</v>
       </c>
@@ -2465,8 +2825,11 @@
       <c r="E120" s="1">
         <v>52378555427.81</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120" s="1">
+        <v>52377491168.6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" s="3">
         <v>44377</v>
       </c>
@@ -2482,8 +2845,11 @@
       <c r="E121" s="1">
         <v>53479161312.64</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121" s="1">
+        <v>53478852821.66</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" s="3">
         <v>44408</v>
       </c>
@@ -2499,8 +2865,11 @@
       <c r="E122" s="1">
         <v>54428748586.62</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122" s="1">
+        <v>54427407343.81</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="3">
         <v>44439</v>
       </c>
@@ -2516,8 +2885,11 @@
       <c r="E123" s="1">
         <v>54870336763.75999</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123" s="1">
+        <v>54869685745.92</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" s="3">
         <v>44469</v>
       </c>
@@ -2533,8 +2905,11 @@
       <c r="E124" s="1">
         <v>52901048832.99</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124" s="1">
+        <v>52899987106.51</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" s="3">
         <v>44500</v>
       </c>
@@ -2550,8 +2925,11 @@
       <c r="E125" s="1">
         <v>54300766813.44</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125" s="1">
+        <v>54299678668.4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" s="3">
         <v>44530</v>
       </c>
@@ -2567,8 +2945,11 @@
       <c r="E126" s="1">
         <v>55089355967.77</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126" s="1">
+        <v>55088773683.99</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" s="3">
         <v>44561</v>
       </c>
@@ -2584,8 +2965,11 @@
       <c r="E127" s="1">
         <v>55524868915.5</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127" s="1">
+        <v>55524301502.51</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" s="3">
         <v>44592</v>
       </c>
@@ -2601,8 +2985,11 @@
       <c r="E128" s="1">
         <v>52791395368.22</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" s="1">
+        <v>52790186100.2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" s="3">
         <v>44620</v>
       </c>
@@ -2618,8 +3005,11 @@
       <c r="E129" s="1">
         <v>51633264538.77</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" s="1">
+        <v>51632693047.39</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" s="3">
         <v>44651</v>
       </c>
@@ -2635,8 +3025,11 @@
       <c r="E130" s="1">
         <v>50270286009.19</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" s="1">
+        <v>50269272742.92</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" s="3">
         <v>44681</v>
       </c>
@@ -2652,8 +3045,11 @@
       <c r="E131" s="1">
         <v>46107666188.3</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" s="1">
+        <v>46106802062.87</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" s="3">
         <v>44712</v>
       </c>
@@ -2669,8 +3065,11 @@
       <c r="E132" s="1">
         <v>45519094736.53999</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" s="1">
+        <v>45518750923.86</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" s="3">
         <v>44742</v>
       </c>
@@ -2686,8 +3085,11 @@
       <c r="E133" s="1">
         <v>43747443202.46</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" s="1">
+        <v>43746561277.33</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="3">
         <v>44773</v>
       </c>
@@ -2703,8 +3105,11 @@
       <c r="E134" s="1">
         <v>45304431259.36</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" s="1">
+        <v>45303131705.44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" s="3">
         <v>44804</v>
       </c>
@@ -2720,8 +3125,11 @@
       <c r="E135" s="1">
         <v>43237590005.3</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" s="1">
+        <v>43237193282.92</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" s="3">
         <v>44834</v>
       </c>
@@ -2737,8 +3145,11 @@
       <c r="E136" s="1">
         <v>41516674580.5</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" s="1">
+        <v>41515240522.93</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" s="3">
         <v>44865</v>
       </c>
@@ -2754,8 +3165,11 @@
       <c r="E137" s="1">
         <v>40713188313.89999</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" s="1">
+        <v>40712619772.52</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" s="3">
         <v>44895</v>
       </c>
@@ -2771,8 +3185,11 @@
       <c r="E138" s="1">
         <v>43028134029.84</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" s="1">
+        <v>43027359146.08</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="3">
         <v>44926</v>
       </c>
@@ -2788,8 +3205,11 @@
       <c r="E139" s="1">
         <v>41935279244.92</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" s="1">
+        <v>41933824136.41</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" s="3">
         <v>44957</v>
       </c>
@@ -2805,8 +3225,11 @@
       <c r="E140" s="1">
         <v>44189592455.97</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" s="1">
+        <v>44188047297.82</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" s="3">
         <v>44985</v>
       </c>
@@ -2822,8 +3245,11 @@
       <c r="E141" s="1">
         <v>42162539846.42001</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" s="1">
+        <v>42161279137.19</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" s="3">
         <v>45016</v>
       </c>
@@ -2839,8 +3265,11 @@
       <c r="E142" s="1">
         <v>44547460232.85</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" s="1">
+        <v>44546392777.65</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" s="3">
         <v>45046</v>
       </c>
@@ -2856,8 +3285,11 @@
       <c r="E143" s="1">
         <v>44883875298.93999</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" s="1">
+        <v>44882668038.45</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" s="3">
         <v>45077</v>
       </c>
@@ -2873,8 +3305,11 @@
       <c r="E144" s="1">
         <v>43673211970.93</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" s="1">
+        <v>43672633102.84</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="3">
         <v>45107</v>
       </c>
@@ -2890,8 +3325,11 @@
       <c r="E145" s="1">
         <v>44054561532.86</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" s="1">
+        <v>44053347326.72</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="3">
         <v>45138</v>
       </c>
@@ -2907,8 +3345,11 @@
       <c r="E146" s="1">
         <v>43842962755.64</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" s="1">
+        <v>43841971877.07</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="3">
         <v>45169</v>
       </c>
@@ -2924,8 +3365,11 @@
       <c r="E147" s="1">
         <v>42632156030.68</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" s="1">
+        <v>42630693021.69</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" s="3">
         <v>45199</v>
       </c>
@@ -2940,6 +3384,9 @@
       </c>
       <c r="E148" s="1">
         <v>40148798399.09</v>
+      </c>
+      <c r="F148" s="1">
+        <v>40147828579.02</v>
       </c>
     </row>
   </sheetData>
@@ -2948,7 +3395,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E148">
+  <conditionalFormatting sqref="B2:F148">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
@@ -2968,9 +3415,9 @@
     <col min="1" max="1001" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2984,8 +3431,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>40755</v>
       </c>
@@ -3001,8 +3451,11 @@
       <c r="E2" s="1">
         <v>0.010779</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1">
+        <v>0.010787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>40786</v>
       </c>
@@ -3018,8 +3471,11 @@
       <c r="E3" s="1">
         <v>-0.00649</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1">
+        <v>-0.006469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>40816</v>
       </c>
@@ -3035,8 +3491,11 @@
       <c r="E4" s="1">
         <v>0.001203</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1">
+        <v>0.001224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>40847</v>
       </c>
@@ -3052,8 +3511,11 @@
       <c r="E5" s="1">
         <v>0.035731</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="1">
+        <v>0.035742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>40877</v>
       </c>
@@ -3069,8 +3531,11 @@
       <c r="E6" s="1">
         <v>-0.006832</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="1">
+        <v>-0.006798999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="3">
         <v>40908</v>
       </c>
@@ -3086,8 +3551,11 @@
       <c r="E7" s="1">
         <v>0.011629</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="1">
+        <v>0.011646</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="3">
         <v>40939</v>
       </c>
@@ -3103,8 +3571,11 @@
       <c r="E8" s="1">
         <v>0.027752</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="1">
+        <v>0.02776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>40968</v>
       </c>
@@ -3120,8 +3591,11 @@
       <c r="E9" s="1">
         <v>0.018403</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="1">
+        <v>0.018452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3">
         <v>40999</v>
       </c>
@@ -3137,8 +3611,11 @@
       <c r="E10" s="1">
         <v>-0.003838</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="1">
+        <v>-0.003805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>41029</v>
       </c>
@@ -3154,8 +3631,11 @@
       <c r="E11" s="1">
         <v>0.010169</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="1">
+        <v>0.010181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3">
         <v>41060</v>
       </c>
@@ -3171,8 +3651,11 @@
       <c r="E12" s="1">
         <v>-0.007122000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="1">
+        <v>-0.007114000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3">
         <v>41090</v>
       </c>
@@ -3188,8 +3671,11 @@
       <c r="E13" s="1">
         <v>0.013655</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="1">
+        <v>0.013702</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="3">
         <v>41121</v>
       </c>
@@ -3205,8 +3691,11 @@
       <c r="E14" s="1">
         <v>0.022421</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="1">
+        <v>0.022443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="3">
         <v>41152</v>
       </c>
@@ -3222,8 +3711,11 @@
       <c r="E15" s="1">
         <v>0.006546</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="1">
+        <v>0.006599000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="3">
         <v>41182</v>
       </c>
@@ -3239,8 +3731,11 @@
       <c r="E16" s="1">
         <v>0.008597</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="1">
+        <v>0.008647999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="3">
         <v>41213</v>
       </c>
@@ -3256,8 +3751,11 @@
       <c r="E17" s="1">
         <v>0.001505</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="1">
+        <v>0.001537</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3">
         <v>41243</v>
       </c>
@@ -3273,8 +3771,11 @@
       <c r="E18" s="1">
         <v>0.007571</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="1">
+        <v>0.007581</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3">
         <v>41274</v>
       </c>
@@ -3290,8 +3791,11 @@
       <c r="E19" s="1">
         <v>0.008163999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="1">
+        <v>0.00821</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>41305</v>
       </c>
@@ -3307,8 +3811,11 @@
       <c r="E20" s="1">
         <v>0.013479</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="1">
+        <v>0.013506</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3">
         <v>41333</v>
       </c>
@@ -3324,8 +3831,11 @@
       <c r="E21" s="1">
         <v>0.007467000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="1">
+        <v>0.007503999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>41364</v>
       </c>
@@ -3341,8 +3851,11 @@
       <c r="E22" s="1">
         <v>0.015024</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="1">
+        <v>0.015067</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="3">
         <v>41394</v>
       </c>
@@ -3358,8 +3871,11 @@
       <c r="E23" s="1">
         <v>0.025087</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="1">
+        <v>0.025126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="3">
         <v>41425</v>
       </c>
@@ -3375,8 +3891,11 @@
       <c r="E24" s="1">
         <v>-0.01667</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="1">
+        <v>-0.016669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <v>41455</v>
       </c>
@@ -3392,8 +3911,11 @@
       <c r="E25" s="1">
         <v>-0.018162</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="1">
+        <v>-0.018117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
         <v>41486</v>
       </c>
@@ -3409,8 +3931,11 @@
       <c r="E26" s="1">
         <v>0.014253</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="1">
+        <v>0.014264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="3">
         <v>41517</v>
       </c>
@@ -3426,8 +3951,11 @@
       <c r="E27" s="1">
         <v>-0.011036</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="1">
+        <v>-0.010998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="3">
         <v>41547</v>
       </c>
@@ -3443,8 +3971,11 @@
       <c r="E28" s="1">
         <v>0.020116</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="1">
+        <v>0.020156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="3">
         <v>41578</v>
       </c>
@@ -3460,8 +3991,11 @@
       <c r="E29" s="1">
         <v>0.022229</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="1">
+        <v>0.022274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="3">
         <v>41608</v>
       </c>
@@ -3477,8 +4011,11 @@
       <c r="E30" s="1">
         <v>0.001659</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="1">
+        <v>0.001664</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="3">
         <v>41639</v>
       </c>
@@ -3494,8 +4031,11 @@
       <c r="E31" s="1">
         <v>0.00731</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="1">
+        <v>0.007331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="3">
         <v>41670</v>
       </c>
@@ -3511,8 +4051,11 @@
       <c r="E32" s="1">
         <v>0.001871</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="1">
+        <v>0.001873</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="3">
         <v>41698</v>
       </c>
@@ -3528,8 +4071,11 @@
       <c r="E33" s="1">
         <v>0.02296</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="1">
+        <v>0.022941</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="3">
         <v>41729</v>
       </c>
@@ -3545,8 +4091,11 @@
       <c r="E34" s="1">
         <v>0.007581</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="1">
+        <v>0.007613</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="3">
         <v>41759</v>
       </c>
@@ -3562,8 +4111,11 @@
       <c r="E35" s="1">
         <v>0.002563</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="1">
+        <v>0.002567</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="3">
         <v>41790</v>
       </c>
@@ -3579,8 +4131,11 @@
       <c r="E36" s="1">
         <v>0.018617</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="1">
+        <v>0.018658</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="3">
         <v>41820</v>
       </c>
@@ -3596,8 +4151,11 @@
       <c r="E37" s="1">
         <v>0.007591</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="1">
+        <v>0.007621</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="3">
         <v>41851</v>
       </c>
@@ -3613,8 +4171,11 @@
       <c r="E38" s="1">
         <v>-0.003535</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="1">
+        <v>-0.0035</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="3">
         <v>41882</v>
       </c>
@@ -3630,8 +4191,11 @@
       <c r="E39" s="1">
         <v>0.024399</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="1">
+        <v>0.02441</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="3">
         <v>41912</v>
       </c>
@@ -3647,8 +4211,11 @@
       <c r="E40" s="1">
         <v>-0.018796</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="1">
+        <v>-0.018787</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="3">
         <v>41943</v>
       </c>
@@ -3664,8 +4231,11 @@
       <c r="E41" s="1">
         <v>0.012251</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="1">
+        <v>0.012333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="3">
         <v>41973</v>
       </c>
@@ -3681,8 +4251,11 @@
       <c r="E42" s="1">
         <v>0.016818</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="1">
+        <v>0.016821</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="3">
         <v>42004</v>
       </c>
@@ -3698,8 +4271,11 @@
       <c r="E43" s="1">
         <v>0.002077</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="1">
+        <v>0.002126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="3">
         <v>42035</v>
       </c>
@@ -3715,8 +4291,11 @@
       <c r="E44" s="1">
         <v>0.023353</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="1">
+        <v>0.023417</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="3">
         <v>42063</v>
       </c>
@@ -3732,8 +4311,11 @@
       <c r="E45" s="1">
         <v>0.007671</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="1">
+        <v>0.007678000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="3">
         <v>42094</v>
       </c>
@@ -3749,8 +4331,11 @@
       <c r="E46" s="1">
         <v>0.000726</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="1">
+        <v>0.000746</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="3">
         <v>42124</v>
       </c>
@@ -3766,8 +4351,11 @@
       <c r="E47" s="1">
         <v>0.000483</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="1">
+        <v>0.0005070000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="3">
         <v>42155</v>
       </c>
@@ -3783,8 +4371,11 @@
       <c r="E48" s="1">
         <v>-0.001447</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="1">
+        <v>-0.001387</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="3">
         <v>42185</v>
       </c>
@@ -3800,8 +4391,11 @@
       <c r="E49" s="1">
         <v>-0.019128</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="1">
+        <v>-0.019088</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="3">
         <v>42216</v>
       </c>
@@ -3817,8 +4411,11 @@
       <c r="E50" s="1">
         <v>0.010714</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="1">
+        <v>0.01075</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="3">
         <v>42247</v>
       </c>
@@ -3834,8 +4431,11 @@
       <c r="E51" s="1">
         <v>-0.027126</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="1">
+        <v>-0.027093</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="3">
         <v>42277</v>
       </c>
@@ -3851,8 +4451,11 @@
       <c r="E52" s="1">
         <v>-0.00876</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="1">
+        <v>-0.008747</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="3">
         <v>42308</v>
       </c>
@@ -3868,8 +4471,11 @@
       <c r="E53" s="1">
         <v>0.028775</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="1">
+        <v>0.028836</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="3">
         <v>42338</v>
       </c>
@@ -3885,8 +4491,11 @@
       <c r="E54" s="1">
         <v>-0.003813</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="1">
+        <v>-0.003814</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="3">
         <v>42369</v>
       </c>
@@ -3902,8 +4511,11 @@
       <c r="E55" s="1">
         <v>-0.008185</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="1">
+        <v>-0.008107999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="3">
         <v>42400</v>
       </c>
@@ -3919,8 +4531,11 @@
       <c r="E56" s="1">
         <v>-0.014827</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="1">
+        <v>-0.014823</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="3">
         <v>42429</v>
       </c>
@@ -3936,8 +4551,11 @@
       <c r="E57" s="1">
         <v>0.00715</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="1">
+        <v>0.007228</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="3">
         <v>42460</v>
       </c>
@@ -3953,8 +4571,11 @@
       <c r="E58" s="1">
         <v>0.034734</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="1">
+        <v>0.034744</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="3">
         <v>42490</v>
       </c>
@@ -3970,8 +4591,11 @@
       <c r="E59" s="1">
         <v>0.009242999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="1">
+        <v>0.009256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="3">
         <v>42521</v>
       </c>
@@ -3987,8 +4611,11 @@
       <c r="E60" s="1">
         <v>0.001883</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="1">
+        <v>0.001941</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="3">
         <v>42551</v>
       </c>
@@ -4004,8 +4631,11 @@
       <c r="E61" s="1">
         <v>0.010112</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="1">
+        <v>0.010098</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="3">
         <v>42582</v>
       </c>
@@ -4021,8 +4651,11 @@
       <c r="E62" s="1">
         <v>0.021265</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="1">
+        <v>0.021276</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="3">
         <v>42613</v>
       </c>
@@ -4038,8 +4671,11 @@
       <c r="E63" s="1">
         <v>0.001145</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="1">
+        <v>0.001155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="3">
         <v>42643</v>
       </c>
@@ -4055,8 +4691,11 @@
       <c r="E64" s="1">
         <v>0.00083</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="1">
+        <v>0.0009120000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="3">
         <v>42674</v>
       </c>
@@ -4072,8 +4711,11 @@
       <c r="E65" s="1">
         <v>-0.011778</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" s="1">
+        <v>-0.011775</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="3">
         <v>42704</v>
       </c>
@@ -4089,8 +4731,11 @@
       <c r="E66" s="1">
         <v>-0.011502</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" s="1">
+        <v>-0.011447</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="3">
         <v>42735</v>
       </c>
@@ -4106,8 +4751,11 @@
       <c r="E67" s="1">
         <v>0.010141</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" s="1">
+        <v>0.010322</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="3">
         <v>42766</v>
       </c>
@@ -4123,8 +4771,11 @@
       <c r="E68" s="1">
         <v>0.011655</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" s="1">
+        <v>0.011698</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="3">
         <v>42794</v>
       </c>
@@ -4140,8 +4791,11 @@
       <c r="E69" s="1">
         <v>0.017674</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" s="1">
+        <v>0.017685</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="3">
         <v>42825</v>
       </c>
@@ -4157,8 +4811,11 @@
       <c r="E70" s="1">
         <v>0.005195</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70" s="1">
+        <v>0.005258000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="3">
         <v>42855</v>
       </c>
@@ -4174,8 +4831,11 @@
       <c r="E71" s="1">
         <v>0.013598</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71" s="1">
+        <v>0.013641</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="3">
         <v>42886</v>
       </c>
@@ -4191,8 +4851,11 @@
       <c r="E72" s="1">
         <v>0.015262</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72" s="1">
+        <v>0.01527</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="3">
         <v>42916</v>
       </c>
@@ -4208,8 +4871,11 @@
       <c r="E73" s="1">
         <v>0.005257</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73" s="1">
+        <v>0.005279000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="3">
         <v>42947</v>
       </c>
@@ -4225,8 +4891,11 @@
       <c r="E74" s="1">
         <v>0.011307</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" s="1">
+        <v>0.011318</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="3">
         <v>42978</v>
       </c>
@@ -4242,8 +4911,11 @@
       <c r="E75" s="1">
         <v>0.010725</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75" s="1">
+        <v>0.010768</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="3">
         <v>43008</v>
       </c>
@@ -4259,8 +4931,11 @@
       <c r="E76" s="1">
         <v>0.008107</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76" s="1">
+        <v>0.008131000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="3">
         <v>43039</v>
       </c>
@@ -4276,8 +4951,11 @@
       <c r="E77" s="1">
         <v>0.011964</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77" s="1">
+        <v>0.012022</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" s="3">
         <v>43069</v>
       </c>
@@ -4293,8 +4971,11 @@
       <c r="E78" s="1">
         <v>0.013355</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78" s="1">
+        <v>0.013356</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="3">
         <v>43100</v>
       </c>
@@ -4310,8 +4991,11 @@
       <c r="E79" s="1">
         <v>0.012016</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79" s="1">
+        <v>0.012674</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" s="3">
         <v>43131</v>
       </c>
@@ -4327,8 +5011,11 @@
       <c r="E80" s="1">
         <v>0.019876</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80" s="1">
+        <v>0.024838</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="3">
         <v>43159</v>
       </c>
@@ -4344,8 +5031,11 @@
       <c r="E81" s="1">
         <v>-0.029913</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" s="1">
+        <v>-0.029929</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="3">
         <v>43190</v>
       </c>
@@ -4361,8 +5051,11 @@
       <c r="E82" s="1">
         <v>0.005778999999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82" s="1">
+        <v>0.001458</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="3">
         <v>43220</v>
       </c>
@@ -4378,8 +5071,11 @@
       <c r="E83" s="1">
         <v>-0.004682</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83" s="1">
+        <v>-0.002009</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="3">
         <v>43251</v>
       </c>
@@ -4395,8 +5091,11 @@
       <c r="E84" s="1">
         <v>0.009103</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" s="1">
+        <v>0.006972000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="3">
         <v>43281</v>
       </c>
@@ -4412,8 +5111,11 @@
       <c r="E85" s="1">
         <v>-0.002073</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85" s="1">
+        <v>-0.002804</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="3">
         <v>43312</v>
       </c>
@@ -4429,8 +5131,11 @@
       <c r="E86" s="1">
         <v>0.009061</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86" s="1">
+        <v>0.013504</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="3">
         <v>43343</v>
       </c>
@@ -4446,8 +5151,11 @@
       <c r="E87" s="1">
         <v>0.00937</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87" s="1">
+        <v>0.008217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="3">
         <v>43373</v>
       </c>
@@ -4463,8 +5171,11 @@
       <c r="E88" s="1">
         <v>-0.008794</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88" s="1">
+        <v>-0.005053999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="3">
         <v>43404</v>
       </c>
@@ -4480,8 +5191,11 @@
       <c r="E89" s="1">
         <v>-0.039984</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89" s="1">
+        <v>-0.040558</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="3">
         <v>43434</v>
       </c>
@@ -4497,8 +5211,11 @@
       <c r="E90" s="1">
         <v>0.012878</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90" s="1">
+        <v>0.011452</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="3">
         <v>43465</v>
       </c>
@@ -4514,8 +5231,11 @@
       <c r="E91" s="1">
         <v>-0.003477</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91" s="1">
+        <v>-0.016145</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="3">
         <v>43496</v>
       </c>
@@ -4531,8 +5251,11 @@
       <c r="E92" s="1">
         <v>0.032009</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92" s="1">
+        <v>0.037042</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="3">
         <v>43524</v>
       </c>
@@ -4548,8 +5271,11 @@
       <c r="E93" s="1">
         <v>0.005999</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93" s="1">
+        <v>0.010191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="3">
         <v>43555</v>
       </c>
@@ -4565,8 +5291,11 @@
       <c r="E94" s="1">
         <v>0.027935</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94" s="1">
+        <v>0.021151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="3">
         <v>43585</v>
       </c>
@@ -4582,8 +5311,11 @@
       <c r="E95" s="1">
         <v>0.00509</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95" s="1">
+        <v>0.010597</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="3">
         <v>43616</v>
       </c>
@@ -4599,8 +5331,11 @@
       <c r="E96" s="1">
         <v>0.010002</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" s="1">
+        <v>-0.004249</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="3">
         <v>43646</v>
       </c>
@@ -4616,8 +5351,11 @@
       <c r="E97" s="1">
         <v>0.029644</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" s="1">
+        <v>0.033356</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="3">
         <v>43677</v>
       </c>
@@ -4633,8 +5371,11 @@
       <c r="E98" s="1">
         <v>0.004747</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" s="1">
+        <v>0.005241</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="3">
         <v>43708</v>
       </c>
@@ -4650,8 +5391,11 @@
       <c r="E99" s="1">
         <v>0.044206</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" s="1">
+        <v>0.024308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="3">
         <v>43738</v>
       </c>
@@ -4667,8 +5411,11 @@
       <c r="E100" s="1">
         <v>-0.004635</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" s="1">
+        <v>0.002227</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="3">
         <v>43769</v>
       </c>
@@ -4684,8 +5431,11 @@
       <c r="E101" s="1">
         <v>0.002441</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" s="1">
+        <v>0.002473</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="3">
         <v>43799</v>
       </c>
@@ -4701,8 +5451,11 @@
       <c r="E102" s="1">
         <v>0.008153000000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" s="1">
+        <v>0.008192</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="3">
         <v>43830</v>
       </c>
@@ -4718,8 +5471,11 @@
       <c r="E103" s="1">
         <v>-0.000751</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" s="1">
+        <v>-0.0007470000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="3">
         <v>43861</v>
       </c>
@@ -4735,8 +5491,11 @@
       <c r="E104" s="1">
         <v>0.02564</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" s="1">
+        <v>0.025673</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" s="3">
         <v>43890</v>
       </c>
@@ -4752,8 +5511,11 @@
       <c r="E105" s="1">
         <v>0.001266</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" s="1">
+        <v>0.001282</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" s="3">
         <v>43921</v>
       </c>
@@ -4769,8 +5531,11 @@
       <c r="E106" s="1">
         <v>-0.037684</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" s="1">
+        <v>-0.03767</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="3">
         <v>43951</v>
       </c>
@@ -4786,8 +5551,11 @@
       <c r="E107" s="1">
         <v>0.044486</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" s="1">
+        <v>0.044508</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" s="3">
         <v>43982</v>
       </c>
@@ -4803,8 +5571,11 @@
       <c r="E108" s="1">
         <v>0.003246</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" s="1">
+        <v>0.003265</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" s="3">
         <v>44012</v>
       </c>
@@ -4820,8 +5591,11 @@
       <c r="E109" s="1">
         <v>0.010239</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" s="1">
+        <v>0.010239</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" s="3">
         <v>44043</v>
       </c>
@@ -4837,8 +5611,11 @@
       <c r="E110" s="1">
         <v>0.040234</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" s="1">
+        <v>0.04024</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="3">
         <v>44074</v>
       </c>
@@ -4854,8 +5631,11 @@
       <c r="E111" s="1">
         <v>-0.003186</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" s="1">
+        <v>-0.003183</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="3">
         <v>44104</v>
       </c>
@@ -4871,8 +5651,11 @@
       <c r="E112" s="1">
         <v>-0.008924999999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112" s="1">
+        <v>-0.008980999999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" s="3">
         <v>44135</v>
       </c>
@@ -4888,8 +5671,11 @@
       <c r="E113" s="1">
         <v>-0.020374</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113" s="1">
+        <v>-0.020368</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" s="3">
         <v>44165</v>
       </c>
@@ -4905,8 +5691,11 @@
       <c r="E114" s="1">
         <v>0.053226</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114" s="1">
+        <v>0.05322499999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" s="3">
         <v>44196</v>
       </c>
@@ -4922,8 +5711,11 @@
       <c r="E115" s="1">
         <v>0.013933</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115" s="1">
+        <v>0.013948</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" s="3">
         <v>44227</v>
       </c>
@@ -4939,8 +5731,11 @@
       <c r="E116" s="1">
         <v>-0.020192</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" s="1">
+        <v>-0.020193</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" s="3">
         <v>44255</v>
       </c>
@@ -4956,8 +5751,11 @@
       <c r="E117" s="1">
         <v>-0.018451</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" s="1">
+        <v>-0.018448</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" s="3">
         <v>44286</v>
       </c>
@@ -4973,8 +5771,11 @@
       <c r="E118" s="1">
         <v>0.0006980000000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" s="1">
+        <v>0.0007159999999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" s="3">
         <v>44316</v>
       </c>
@@ -4990,8 +5791,11 @@
       <c r="E119" s="1">
         <v>0.028885</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119" s="1">
+        <v>0.028889</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="3">
         <v>44347</v>
       </c>
@@ -5007,8 +5811,11 @@
       <c r="E120" s="1">
         <v>0.015936</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120" s="1">
+        <v>0.015938</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" s="3">
         <v>44377</v>
       </c>
@@ -5024,8 +5831,11 @@
       <c r="E121" s="1">
         <v>0.023884</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121" s="1">
+        <v>0.02391</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" s="3">
         <v>44408</v>
       </c>
@@ -5041,8 +5851,11 @@
       <c r="E122" s="1">
         <v>0.020584</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122" s="1">
+        <v>0.020569</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="3">
         <v>44439</v>
       </c>
@@ -5058,8 +5871,11 @@
       <c r="E123" s="1">
         <v>0.010881</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123" s="1">
+        <v>0.010892</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" s="3">
         <v>44469</v>
       </c>
@@ -5075,8 +5891,11 @@
       <c r="E124" s="1">
         <v>-0.033223</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124" s="1">
+        <v>-0.033221</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" s="3">
         <v>44500</v>
       </c>
@@ -5092,8 +5911,11 @@
       <c r="E125" s="1">
         <v>0.031335</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125" s="1">
+        <v>0.031337</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" s="3">
         <v>44530</v>
       </c>
@@ -5109,8 +5931,11 @@
       <c r="E126" s="1">
         <v>0.017353</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126" s="1">
+        <v>0.01736</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" s="3">
         <v>44561</v>
       </c>
@@ -5126,8 +5951,11 @@
       <c r="E127" s="1">
         <v>0.00827</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127" s="1">
+        <v>0.008281</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" s="3">
         <v>44592</v>
       </c>
@@ -5143,8 +5971,11 @@
       <c r="E128" s="1">
         <v>-0.046588</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" s="1">
+        <v>-0.046586</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" s="3">
         <v>44620</v>
       </c>
@@ -5160,8 +5991,11 @@
       <c r="E129" s="1">
         <v>-0.019075</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" s="1">
+        <v>-0.019058</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" s="3">
         <v>44651</v>
       </c>
@@ -5177,8 +6011,11 @@
       <c r="E130" s="1">
         <v>-0.02338</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" s="1">
+        <v>-0.023376</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" s="3">
         <v>44681</v>
       </c>
@@ -5194,8 +6031,11 @@
       <c r="E131" s="1">
         <v>-0.07989399999999999</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" s="1">
+        <v>-0.079887</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" s="3">
         <v>44712</v>
       </c>
@@ -5211,8 +6051,11 @@
       <c r="E132" s="1">
         <v>-0.009348</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" s="1">
+        <v>-0.009331000000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" s="3">
         <v>44742</v>
       </c>
@@ -5228,8 +6071,11 @@
       <c r="E133" s="1">
         <v>-0.035533</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" s="1">
+        <v>-0.035525</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="3">
         <v>44773</v>
       </c>
@@ -5245,8 +6091,11 @@
       <c r="E134" s="1">
         <v>0.03943</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" s="1">
+        <v>0.039431</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" s="3">
         <v>44804</v>
       </c>
@@ -5262,8 +6111,11 @@
       <c r="E135" s="1">
         <v>-0.042222</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" s="1">
+        <v>-0.042204</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" s="3">
         <v>44834</v>
       </c>
@@ -5279,8 +6131,11 @@
       <c r="E136" s="1">
         <v>-0.07750499999999999</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" s="1">
+        <v>-0.077504</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" s="3">
         <v>44865</v>
       </c>
@@ -5296,8 +6151,11 @@
       <c r="E137" s="1">
         <v>-0.011631</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" s="1">
+        <v>-0.011611</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" s="3">
         <v>44895</v>
       </c>
@@ -5313,8 +6171,11 @@
       <c r="E138" s="1">
         <v>0.061094</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" s="1">
+        <v>0.061116</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="3">
         <v>44926</v>
       </c>
@@ -5330,8 +6191,11 @@
       <c r="E139" s="1">
         <v>-0.021664</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" s="1">
+        <v>-0.021662</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" s="3">
         <v>44957</v>
       </c>
@@ -5347,8 +6211,11 @@
       <c r="E140" s="1">
         <v>0.057892</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" s="1">
+        <v>0.057901</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" s="3">
         <v>44985</v>
       </c>
@@ -5364,8 +6231,11 @@
       <c r="E141" s="1">
         <v>-0.04226899999999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" s="1">
+        <v>-0.042256</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" s="3">
         <v>45016</v>
       </c>
@@ -5381,8 +6251,11 @@
       <c r="E142" s="1">
         <v>0.032184</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" s="1">
+        <v>0.032195</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" s="3">
         <v>45046</v>
       </c>
@@ -5398,8 +6271,11 @@
       <c r="E143" s="1">
         <v>0.011411</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" s="1">
+        <v>0.011419</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" s="3">
         <v>45077</v>
       </c>
@@ -5415,8 +6291,11 @@
       <c r="E144" s="1">
         <v>-0.02331</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" s="1">
+        <v>-0.023289</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="3">
         <v>45107</v>
       </c>
@@ -5432,8 +6311,11 @@
       <c r="E145" s="1">
         <v>0.012684</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" s="1">
+        <v>0.012691</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="3">
         <v>45138</v>
       </c>
@@ -5449,8 +6331,11 @@
       <c r="E146" s="1">
         <v>-0.000907</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" s="1">
+        <v>-0.000893</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="3">
         <v>45169</v>
       </c>
@@ -5466,8 +6351,11 @@
       <c r="E147" s="1">
         <v>-0.023792</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" s="1">
+        <v>-0.023789</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" s="3">
         <v>45199</v>
       </c>
@@ -5482,6 +6370,9 @@
       </c>
       <c r="E148" s="1">
         <v>-0.054409</v>
+      </c>
+      <c r="F148" s="1">
+        <v>-0.054394</v>
       </c>
     </row>
   </sheetData>
@@ -5490,7 +6381,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E148">
+  <conditionalFormatting sqref="B2:F148">
     <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update for new pv calculation
</commit_message>
<xml_diff>
--- a/data/time_series/plan_data.xlsx
+++ b/data/time_series/plan_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>IBT</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Total Consolidation</t>
   </si>
   <si>
     <t>Date</t>
@@ -429,9 +426,9 @@
     <col min="1" max="1001" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -445,11 +442,8 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>40816</v>
       </c>
@@ -465,11 +459,8 @@
       <c r="E2" s="1">
         <v>21890762234.61</v>
       </c>
-      <c r="F2" s="1">
-        <v>22052849274.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>40847</v>
       </c>
@@ -485,11 +476,8 @@
       <c r="E3" s="1">
         <v>22618006484.29</v>
       </c>
-      <c r="F3" s="1">
-        <v>22778089729.38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>40877</v>
       </c>
@@ -505,11 +493,8 @@
       <c r="E4" s="1">
         <v>22404833979.68</v>
       </c>
-      <c r="F4" s="1">
-        <v>22555336103.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>40908</v>
       </c>
@@ -525,11 +510,8 @@
       <c r="E5" s="1">
         <v>22610739192.74</v>
       </c>
-      <c r="F5" s="1">
-        <v>22760627152.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>40939</v>
       </c>
@@ -545,11 +527,8 @@
       <c r="E6" s="1">
         <v>23182713107.18</v>
       </c>
-      <c r="F6" s="1">
-        <v>23327836945.97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>40968</v>
       </c>
@@ -565,11 +544,8 @@
       <c r="E7" s="1">
         <v>23539061638.97</v>
       </c>
-      <c r="F7" s="1">
-        <v>23683533132.48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>40999</v>
       </c>
@@ -585,11 +561,8 @@
       <c r="E8" s="1">
         <v>23568627738.57</v>
       </c>
-      <c r="F8" s="1">
-        <v>23527415369.76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>41029</v>
       </c>
@@ -605,11 +578,8 @@
       <c r="E9" s="1">
         <v>23751063285.04</v>
       </c>
-      <c r="F9" s="1">
-        <v>23878250766.57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>41060</v>
       </c>
@@ -625,11 +595,8 @@
       <c r="E10" s="1">
         <v>23525356279.52</v>
       </c>
-      <c r="F10" s="1">
-        <v>23642315685.53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>41090</v>
       </c>
@@ -645,11 +612,8 @@
       <c r="E11" s="1">
         <v>23967119998.88</v>
       </c>
-      <c r="F11" s="1">
-        <v>23898064813.57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>41121</v>
       </c>
@@ -665,11 +629,8 @@
       <c r="E12" s="1">
         <v>24445194794.85</v>
       </c>
-      <c r="F12" s="1">
-        <v>24549514764.65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>41152</v>
       </c>
@@ -685,11 +646,8 @@
       <c r="E13" s="1">
         <v>24546339462.45</v>
       </c>
-      <c r="F13" s="1">
-        <v>24642500384.21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>41182</v>
       </c>
@@ -705,11 +663,8 @@
       <c r="E14" s="1">
         <v>24697860539.92</v>
       </c>
-      <c r="F14" s="1">
-        <v>25154181675.76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>41213</v>
       </c>
@@ -725,11 +680,8 @@
       <c r="E15" s="1">
         <v>24675789016.94</v>
       </c>
-      <c r="F15" s="1">
-        <v>25125272400.54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>41243</v>
       </c>
@@ -745,11 +697,8 @@
       <c r="E16" s="1">
         <v>24802412939.95</v>
       </c>
-      <c r="F16" s="1">
-        <v>25245243669.78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <v>41274</v>
       </c>
@@ -765,11 +714,8 @@
       <c r="E17" s="1">
         <v>24895888004.03</v>
       </c>
-      <c r="F17" s="1">
-        <v>25331489787.35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <v>41305</v>
       </c>
@@ -785,11 +731,8 @@
       <c r="E18" s="1">
         <v>25170522714.13</v>
       </c>
-      <c r="F18" s="1">
-        <v>26333049791.22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3">
         <v>41333</v>
       </c>
@@ -805,11 +748,8 @@
       <c r="E19" s="1">
         <v>25279217396.12</v>
       </c>
-      <c r="F19" s="1">
-        <v>26437887737.61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="3">
         <v>41364</v>
       </c>
@@ -825,11 +765,8 @@
       <c r="E20" s="1">
         <v>25595621001.76</v>
       </c>
-      <c r="F20" s="1">
-        <v>26762244859.97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3">
         <v>41394</v>
       </c>
@@ -845,11 +782,8 @@
       <c r="E21" s="1">
         <v>26172966159.6</v>
       </c>
-      <c r="F21" s="1">
-        <v>27354266269.36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>41425</v>
       </c>
@@ -865,11 +799,8 @@
       <c r="E22" s="1">
         <v>25673994810.38</v>
       </c>
-      <c r="F22" s="1">
-        <v>26825680454.21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>41455</v>
       </c>
@@ -885,11 +816,8 @@
       <c r="E23" s="1">
         <v>25144254258.35</v>
       </c>
-      <c r="F23" s="1">
-        <v>26265676510.43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="3">
         <v>41486</v>
       </c>
@@ -905,11 +833,8 @@
       <c r="E24" s="1">
         <v>25436691656.9</v>
       </c>
-      <c r="F24" s="1">
-        <v>26565709631.94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="3">
         <v>41517</v>
       </c>
@@ -925,11 +850,8 @@
       <c r="E25" s="1">
         <v>25090707293.91</v>
       </c>
-      <c r="F25" s="1">
-        <v>26201572226.35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="3">
         <v>41547</v>
       </c>
@@ -945,11 +867,8 @@
       <c r="E26" s="1">
         <v>25528497279.93</v>
       </c>
-      <c r="F26" s="1">
-        <v>26650940234.76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="3">
         <v>41578</v>
       </c>
@@ -965,11 +884,8 @@
       <c r="E27" s="1">
         <v>26027364114.18</v>
       </c>
-      <c r="F27" s="1">
-        <v>27164746657.23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="3">
         <v>41608</v>
       </c>
@@ -985,11 +901,8 @@
       <c r="E28" s="1">
         <v>26003820925.72</v>
       </c>
-      <c r="F28" s="1">
-        <v>27132210456.28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="3">
         <v>41639</v>
       </c>
@@ -1005,11 +918,8 @@
       <c r="E29" s="1">
         <v>26126288441.74</v>
       </c>
-      <c r="F29" s="1">
-        <v>27253687582.98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="3">
         <v>41670</v>
       </c>
@@ -1025,11 +935,8 @@
       <c r="E30" s="1">
         <v>26107696311.48</v>
       </c>
-      <c r="F30" s="1">
-        <v>27226639980.42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="3">
         <v>41698</v>
       </c>
@@ -1045,11 +952,8 @@
       <c r="E31" s="1">
         <v>26638164824.17</v>
       </c>
-      <c r="F31" s="1">
-        <v>27769593035.21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="3">
         <v>41729</v>
       </c>
@@ -1065,11 +969,8 @@
       <c r="E32" s="1">
         <v>26770056497.39</v>
       </c>
-      <c r="F32" s="1">
-        <v>27900602168.04</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="3">
         <v>41759</v>
       </c>
@@ -1085,11 +986,8 @@
       <c r="E33" s="1">
         <v>26766109574.18</v>
       </c>
-      <c r="F33" s="1">
-        <v>27889292662.49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="3">
         <v>41790</v>
       </c>
@@ -1105,11 +1003,8 @@
       <c r="E34" s="1">
         <v>27191987348.25</v>
       </c>
-      <c r="F34" s="1">
-        <v>28325272289.23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="3">
         <v>41820</v>
       </c>
@@ -1125,11 +1020,8 @@
       <c r="E35" s="1">
         <v>27325686546.76</v>
       </c>
-      <c r="F35" s="1">
-        <v>28472678681.56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="3">
         <v>41851</v>
       </c>
@@ -1145,11 +1037,8 @@
       <c r="E36" s="1">
         <v>27156839042.76</v>
       </c>
-      <c r="F36" s="1">
-        <v>28289948331.18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="3">
         <v>41882</v>
       </c>
@@ -1165,11 +1054,8 @@
       <c r="E37" s="1">
         <v>27744206657.43</v>
       </c>
-      <c r="F37" s="1">
-        <v>28894470491.79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="3">
         <v>41912</v>
       </c>
@@ -1185,11 +1071,8 @@
       <c r="E38" s="1">
         <v>27150660877.68</v>
       </c>
-      <c r="F38" s="1">
-        <v>28271789225.71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="3">
         <v>41943</v>
       </c>
@@ -1205,11 +1088,8 @@
       <c r="E39" s="1">
         <v>27371725833.13</v>
       </c>
-      <c r="F39" s="1">
-        <v>28498525017</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="3">
         <v>41973</v>
       </c>
@@ -1225,11 +1105,8 @@
       <c r="E40" s="1">
         <v>27755933978.37</v>
       </c>
-      <c r="F40" s="1">
-        <v>28890460746.39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="3">
         <v>42004</v>
       </c>
@@ -1245,11 +1122,8 @@
       <c r="E41" s="1">
         <v>28782428258.71</v>
       </c>
-      <c r="F41" s="1">
-        <v>29909163526.79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="3">
         <v>42035</v>
       </c>
@@ -1265,11 +1139,8 @@
       <c r="E42" s="1">
         <v>29378034101.34</v>
       </c>
-      <c r="F42" s="1">
-        <v>30520363399.73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="3">
         <v>42063</v>
       </c>
@@ -1285,11 +1156,8 @@
       <c r="E43" s="1">
         <v>29527722140.57</v>
       </c>
-      <c r="F43" s="1">
-        <v>30682678579.16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="3">
         <v>42094</v>
       </c>
@@ -1305,11 +1173,8 @@
       <c r="E44" s="1">
         <v>29472205126.79</v>
       </c>
-      <c r="F44" s="1">
-        <v>30617803151.79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="3">
         <v>42124</v>
       </c>
@@ -1325,11 +1190,8 @@
       <c r="E45" s="1">
         <v>29408637463</v>
       </c>
-      <c r="F45" s="1">
-        <v>30544085686.26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="3">
         <v>42155</v>
       </c>
@@ -1345,11 +1207,8 @@
       <c r="E46" s="1">
         <v>29288010554.98</v>
       </c>
-      <c r="F46" s="1">
-        <v>30411241858.39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="3">
         <v>42185</v>
       </c>
@@ -1365,11 +1224,8 @@
       <c r="E47" s="1">
         <v>28650016749.03</v>
       </c>
-      <c r="F47" s="1">
-        <v>29741788892.27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="3">
         <v>42216</v>
       </c>
@@ -1385,11 +1241,8 @@
       <c r="E48" s="1">
         <v>28876185070.36</v>
       </c>
-      <c r="F48" s="1">
-        <v>29968273775.33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="3">
         <v>42247</v>
       </c>
@@ -1405,11 +1258,8 @@
       <c r="E49" s="1">
         <v>28013929187.9</v>
       </c>
-      <c r="F49" s="1">
-        <v>29066322305.74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="3">
         <v>42277</v>
       </c>
@@ -1425,11 +1275,8 @@
       <c r="E50" s="1">
         <v>27687614897.05</v>
       </c>
-      <c r="F50" s="1">
-        <v>28720022246.88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="3">
         <v>42308</v>
       </c>
@@ -1445,11 +1292,8 @@
       <c r="E51" s="1">
         <v>28326347037.87</v>
       </c>
-      <c r="F51" s="1">
-        <v>29360507839.81</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="3">
         <v>42338</v>
       </c>
@@ -1465,11 +1309,8 @@
       <c r="E52" s="1">
         <v>28136561001.15</v>
       </c>
-      <c r="F52" s="1">
-        <v>29172575288.71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="3">
         <v>42369</v>
       </c>
@@ -1485,11 +1326,8 @@
       <c r="E53" s="1">
         <v>28846254608.33</v>
       </c>
-      <c r="F53" s="1">
-        <v>29862597627.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="3">
         <v>42400</v>
       </c>
@@ -1505,11 +1343,8 @@
       <c r="E54" s="1">
         <v>28336372866.16</v>
       </c>
-      <c r="F54" s="1">
-        <v>29326075448.69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="3">
         <v>42429</v>
       </c>
@@ -1525,11 +1360,8 @@
       <c r="E55" s="1">
         <v>28455678308.47</v>
       </c>
-      <c r="F55" s="1">
-        <v>29440765726.48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="3">
         <v>42460</v>
       </c>
@@ -1545,11 +1377,8 @@
       <c r="E56" s="1">
         <v>29356671897.69</v>
       </c>
-      <c r="F56" s="1">
-        <v>30362580685</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="3">
         <v>42490</v>
       </c>
@@ -1565,11 +1394,8 @@
       <c r="E57" s="1">
         <v>29542027110.35</v>
       </c>
-      <c r="F57" s="1">
-        <v>30560223568.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="3">
         <v>42521</v>
       </c>
@@ -1585,11 +1411,8 @@
       <c r="E58" s="1">
         <v>29511421101.44</v>
       </c>
-      <c r="F58" s="1">
-        <v>30520464418.77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="3">
         <v>42551</v>
       </c>
@@ -1605,11 +1428,8 @@
       <c r="E59" s="1">
         <v>29721833433.55</v>
       </c>
-      <c r="F59" s="1">
-        <v>30728992338.24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="3">
         <v>42582</v>
       </c>
@@ -1625,11 +1445,8 @@
       <c r="E60" s="1">
         <v>30265143212.71</v>
       </c>
-      <c r="F60" s="1">
-        <v>31280132371.05</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="3">
         <v>42613</v>
       </c>
@@ -1645,11 +1462,8 @@
       <c r="E61" s="1">
         <v>30212255260.83</v>
       </c>
-      <c r="F61" s="1">
-        <v>31218710837.63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="3">
         <v>42643</v>
       </c>
@@ -1665,11 +1479,8 @@
       <c r="E62" s="1">
         <v>31311189264.37</v>
       </c>
-      <c r="F62" s="1">
-        <v>32306086725.3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="3">
         <v>42674</v>
       </c>
@@ -1685,11 +1496,8 @@
       <c r="E63" s="1">
         <v>30735701818.56</v>
       </c>
-      <c r="F63" s="1">
-        <v>31707560542.83</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="3">
         <v>42704</v>
       </c>
@@ -1705,11 +1513,8 @@
       <c r="E64" s="1">
         <v>30294149402.87</v>
       </c>
-      <c r="F64" s="1">
-        <v>31243895035.79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="3">
         <v>42735</v>
       </c>
@@ -1725,11 +1530,8 @@
       <c r="E65" s="1">
         <v>31134559706.61</v>
       </c>
-      <c r="F65" s="1">
-        <v>31993862117.18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="3">
         <v>42766</v>
       </c>
@@ -1745,11 +1547,8 @@
       <c r="E66" s="1">
         <v>31406628721.6</v>
       </c>
-      <c r="F66" s="1">
-        <v>32272409430.99</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="3">
         <v>42794</v>
       </c>
@@ -1765,11 +1564,8 @@
       <c r="E67" s="1">
         <v>31862928265.29</v>
       </c>
-      <c r="F67" s="1">
-        <v>32847863724.8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="3">
         <v>42825</v>
       </c>
@@ -1785,11 +1581,8 @@
       <c r="E68" s="1">
         <v>34237217759.41</v>
       </c>
-      <c r="F68" s="1">
-        <v>35227095408.74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="3">
         <v>42855</v>
       </c>
@@ -1805,11 +1598,8 @@
       <c r="E69" s="1">
         <v>34601219933.72</v>
       </c>
-      <c r="F69" s="1">
-        <v>35605325711.35</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="3">
         <v>42886</v>
       </c>
@@ -1825,11 +1615,8 @@
       <c r="E70" s="1">
         <v>35025479666.84</v>
       </c>
-      <c r="F70" s="1">
-        <v>36045330946.54</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="3">
         <v>42916</v>
       </c>
@@ -1845,11 +1632,8 @@
       <c r="E71" s="1">
         <v>35106583260.6</v>
       </c>
-      <c r="F71" s="1">
-        <v>36131069554.68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="3">
         <v>42947</v>
       </c>
@@ -1865,11 +1649,8 @@
       <c r="E72" s="1">
         <v>35405791867.57</v>
       </c>
-      <c r="F72" s="1">
-        <v>36440249931.02</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="3">
         <v>42978</v>
       </c>
@@ -1885,11 +1666,8 @@
       <c r="E73" s="1">
         <v>35685515267.03</v>
       </c>
-      <c r="F73" s="1">
-        <v>36731307884.26</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="3">
         <v>43008</v>
       </c>
@@ -1905,11 +1683,8 @@
       <c r="E74" s="1">
         <v>35874943914.43</v>
       </c>
-      <c r="F74" s="1">
-        <v>36929261044</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="3">
         <v>43039</v>
       </c>
@@ -1925,11 +1700,8 @@
       <c r="E75" s="1">
         <v>36114919745.74</v>
       </c>
-      <c r="F75" s="1">
-        <v>37181963756.37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="3">
         <v>43069</v>
       </c>
@@ -1945,11 +1717,8 @@
       <c r="E76" s="1">
         <v>36495613500.11</v>
       </c>
-      <c r="F76" s="1">
-        <v>37576800847.56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="3">
         <v>43100</v>
       </c>
@@ -1965,11 +1734,8 @@
       <c r="E77" s="1">
         <v>41856058020.2</v>
       </c>
-      <c r="F77" s="1">
-        <v>37949036056.54</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="3">
         <v>43131</v>
       </c>
@@ -1985,11 +1751,8 @@
       <c r="E78" s="1">
         <v>42583718320.38</v>
       </c>
-      <c r="F78" s="1">
-        <v>36126703368.99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="3">
         <v>43159</v>
       </c>
@@ -2005,11 +1768,8 @@
       <c r="E79" s="1">
         <v>41211648261.71</v>
       </c>
-      <c r="F79" s="1">
-        <v>34947041283.19</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="3">
         <v>43190</v>
       </c>
@@ -2025,11 +1785,8 @@
       <c r="E80" s="1">
         <v>41345470043.96999</v>
       </c>
-      <c r="F80" s="1">
-        <v>34893565647.81</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="3">
         <v>43220</v>
       </c>
@@ -2045,11 +1802,8 @@
       <c r="E81" s="1">
         <v>41046760638.73</v>
       </c>
-      <c r="F81" s="1">
-        <v>34718322290.49</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="3">
         <v>43251</v>
       </c>
@@ -2065,11 +1819,8 @@
       <c r="E82" s="1">
         <v>41313232056.15</v>
       </c>
-      <c r="F82" s="1">
-        <v>34853430635.59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="3">
         <v>43281</v>
       </c>
@@ -2085,11 +1836,8 @@
       <c r="E83" s="1">
         <v>41121031725</v>
       </c>
-      <c r="F83" s="1">
-        <v>34649138195.13</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="3">
         <v>43312</v>
       </c>
@@ -2105,11 +1853,8 @@
       <c r="E84" s="1">
         <v>41384588267.64</v>
       </c>
-      <c r="F84" s="1">
-        <v>35007279828.93</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="3">
         <v>43343</v>
       </c>
@@ -2125,11 +1870,8 @@
       <c r="E85" s="1">
         <v>41662803021.32</v>
       </c>
-      <c r="F85" s="1">
-        <v>35185061352.95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="3">
         <v>43373</v>
       </c>
@@ -2145,11 +1887,8 @@
       <c r="E86" s="1">
         <v>41186947565</v>
       </c>
-      <c r="F86" s="1">
-        <v>34897241234.02</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="3">
         <v>43404</v>
       </c>
@@ -2165,11 +1904,8 @@
       <c r="E87" s="1">
         <v>39383035110.98</v>
       </c>
-      <c r="F87" s="1">
-        <v>33324461630.84</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="3">
         <v>43434</v>
       </c>
@@ -2185,11 +1921,8 @@
       <c r="E88" s="1">
         <v>39775163930.18</v>
       </c>
-      <c r="F88" s="1">
-        <v>33590951046.18</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="3">
         <v>43465</v>
       </c>
@@ -2205,11 +1938,8 @@
       <c r="E89" s="1">
         <v>39522985371.47</v>
       </c>
-      <c r="F89" s="1">
-        <v>32936056236.9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="3">
         <v>43496</v>
       </c>
@@ -2225,11 +1955,8 @@
       <c r="E90" s="1">
         <v>40670053634.92</v>
       </c>
-      <c r="F90" s="1">
-        <v>34114984114.15</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="3">
         <v>43524</v>
       </c>
@@ -2245,11 +1972,8 @@
       <c r="E91" s="1">
         <v>40797813026.7</v>
       </c>
-      <c r="F91" s="1">
-        <v>34345800814.97</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="3">
         <v>43555</v>
       </c>
@@ -2265,11 +1989,8 @@
       <c r="E92" s="1">
         <v>41816102147.74</v>
       </c>
-      <c r="F92" s="1">
-        <v>34951519519.29</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="3">
         <v>43585</v>
       </c>
@@ -2285,11 +2006,8 @@
       <c r="E93" s="1">
         <v>42743107013</v>
       </c>
-      <c r="F93" s="1">
-        <v>35544104423.43</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="3">
         <v>43616</v>
       </c>
@@ -2305,11 +2023,8 @@
       <c r="E94" s="1">
         <v>43049605454.39</v>
       </c>
-      <c r="F94" s="1">
-        <v>35353126027.34</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="3">
         <v>43646</v>
       </c>
@@ -2325,11 +2040,8 @@
       <c r="E95" s="1">
         <v>44201897165.55</v>
       </c>
-      <c r="F95" s="1">
-        <v>36407955381.8</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="3">
         <v>43677</v>
       </c>
@@ -2345,11 +2057,8 @@
       <c r="E96" s="1">
         <v>44289278505.62</v>
       </c>
-      <c r="F96" s="1">
-        <v>36475732007.89</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="3">
         <v>43708</v>
       </c>
@@ -2365,11 +2074,8 @@
       <c r="E97" s="1">
         <v>46120311881.3</v>
       </c>
-      <c r="F97" s="1">
-        <v>37237277255.72</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="3">
         <v>43738</v>
       </c>
@@ -2385,11 +2091,8 @@
       <c r="E98" s="1">
         <v>46949593594.97</v>
       </c>
-      <c r="F98" s="1">
-        <v>37278149188.28</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="3">
         <v>43769</v>
       </c>
@@ -2405,11 +2108,8 @@
       <c r="E99" s="1">
         <v>46865708662.23</v>
       </c>
-      <c r="F99" s="1">
-        <v>45620639518.53</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="3">
         <v>43799</v>
       </c>
@@ -2425,11 +2125,8 @@
       <c r="E100" s="1">
         <v>47123617172.53</v>
       </c>
-      <c r="F100" s="1">
-        <v>46986534776.59</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="3">
         <v>43830</v>
       </c>
@@ -2445,11 +2142,8 @@
       <c r="E101" s="1">
         <v>46141633527.96</v>
       </c>
-      <c r="F101" s="1">
-        <v>46024238147.58</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="3">
         <v>43861</v>
       </c>
@@ -2465,11 +2159,8 @@
       <c r="E102" s="1">
         <v>47197661020.02</v>
       </c>
-      <c r="F102" s="1">
-        <v>47145264898.48</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="3">
         <v>43890</v>
       </c>
@@ -2485,11 +2176,8 @@
       <c r="E103" s="1">
         <v>47123824802.83</v>
       </c>
-      <c r="F103" s="1">
-        <v>47102840330.35</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="3">
         <v>43921</v>
       </c>
@@ -2505,11 +2193,8 @@
       <c r="E104" s="1">
         <v>45204026385.17001</v>
       </c>
-      <c r="F104" s="1">
-        <v>45203532515.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="3">
         <v>43951</v>
       </c>
@@ -2525,11 +2210,8 @@
       <c r="E105" s="1">
         <v>47064011332.71</v>
       </c>
-      <c r="F105" s="1">
-        <v>47063659448.95</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="3">
         <v>43982</v>
       </c>
@@ -2545,11 +2227,8 @@
       <c r="E106" s="1">
         <v>47081138950.00999</v>
       </c>
-      <c r="F106" s="1">
-        <v>47080894938.3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="3">
         <v>44012</v>
       </c>
@@ -2565,11 +2244,8 @@
       <c r="E107" s="1">
         <v>47426564864.18</v>
       </c>
-      <c r="F107" s="1">
-        <v>47425304505.7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="3">
         <v>44043</v>
       </c>
@@ -2585,11 +2261,8 @@
       <c r="E108" s="1">
         <v>49195665095.83</v>
       </c>
-      <c r="F108" s="1">
-        <v>49191446952.15</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="3">
         <v>44074</v>
       </c>
@@ -2605,11 +2278,8 @@
       <c r="E109" s="1">
         <v>48906083609.04</v>
       </c>
-      <c r="F109" s="1">
-        <v>48904844973.57</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="3">
         <v>44104</v>
       </c>
@@ -2625,11 +2295,8 @@
       <c r="E110" s="1">
         <v>49328692500.60999</v>
       </c>
-      <c r="F110" s="1">
-        <v>49327891655.97</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="3">
         <v>44135</v>
       </c>
@@ -2645,11 +2312,8 @@
       <c r="E111" s="1">
         <v>48026054531.55</v>
       </c>
-      <c r="F111" s="1">
-        <v>48024908266.78</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="3">
         <v>44165</v>
       </c>
@@ -2665,11 +2329,8 @@
       <c r="E112" s="1">
         <v>50440003419.03</v>
       </c>
-      <c r="F112" s="1">
-        <v>50438850250.79</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="3">
         <v>44196</v>
       </c>
@@ -2685,11 +2346,8 @@
       <c r="E113" s="1">
         <v>52788485957.46</v>
       </c>
-      <c r="F113" s="1">
-        <v>52787920332.11</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="3">
         <v>44227</v>
       </c>
@@ -2705,11 +2363,8 @@
       <c r="E114" s="1">
         <v>51588003234.73</v>
       </c>
-      <c r="F114" s="1">
-        <v>51586801167.14</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="3">
         <v>44255</v>
       </c>
@@ -2725,11 +2380,8 @@
       <c r="E115" s="1">
         <v>50499345827.99</v>
       </c>
-      <c r="F115" s="1">
-        <v>50498271333.38</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="3">
         <v>44286</v>
       </c>
@@ -2745,11 +2397,8 @@
       <c r="E116" s="1">
         <v>50392716520.31</v>
       </c>
-      <c r="F116" s="1">
-        <v>50392459354.27</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="3">
         <v>44316</v>
       </c>
@@ -2765,11 +2414,8 @@
       <c r="E117" s="1">
         <v>51700983288.71</v>
       </c>
-      <c r="F117" s="1">
-        <v>51699898092.8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="3">
         <v>44347</v>
       </c>
@@ -2785,11 +2431,8 @@
       <c r="E118" s="1">
         <v>52378555427.81</v>
       </c>
-      <c r="F118" s="1">
-        <v>52377491168.6</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="3">
         <v>44377</v>
       </c>
@@ -2805,11 +2448,8 @@
       <c r="E119" s="1">
         <v>53479161312.64</v>
       </c>
-      <c r="F119" s="1">
-        <v>53478852821.66</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="3">
         <v>44408</v>
       </c>
@@ -2825,11 +2465,8 @@
       <c r="E120" s="1">
         <v>54428748586.62</v>
       </c>
-      <c r="F120" s="1">
-        <v>54427407343.81</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="3">
         <v>44439</v>
       </c>
@@ -2845,11 +2482,8 @@
       <c r="E121" s="1">
         <v>54870336763.75999</v>
       </c>
-      <c r="F121" s="1">
-        <v>54869685745.92</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="3">
         <v>44469</v>
       </c>
@@ -2865,11 +2499,8 @@
       <c r="E122" s="1">
         <v>52901048832.99</v>
       </c>
-      <c r="F122" s="1">
-        <v>52899987106.51</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="3">
         <v>44500</v>
       </c>
@@ -2885,11 +2516,8 @@
       <c r="E123" s="1">
         <v>54300766813.44</v>
       </c>
-      <c r="F123" s="1">
-        <v>54299678668.4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="3">
         <v>44530</v>
       </c>
@@ -2905,11 +2533,8 @@
       <c r="E124" s="1">
         <v>55089355967.77</v>
       </c>
-      <c r="F124" s="1">
-        <v>55088773683.99</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="3">
         <v>44561</v>
       </c>
@@ -2925,11 +2550,8 @@
       <c r="E125" s="1">
         <v>55524868915.5</v>
       </c>
-      <c r="F125" s="1">
-        <v>55524301502.51</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="3">
         <v>44592</v>
       </c>
@@ -2945,11 +2567,8 @@
       <c r="E126" s="1">
         <v>52791395368.22</v>
       </c>
-      <c r="F126" s="1">
-        <v>52790186100.2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="3">
         <v>44620</v>
       </c>
@@ -2965,11 +2584,8 @@
       <c r="E127" s="1">
         <v>51633264538.77</v>
       </c>
-      <c r="F127" s="1">
-        <v>51632693047.39</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="3">
         <v>44651</v>
       </c>
@@ -2985,11 +2601,8 @@
       <c r="E128" s="1">
         <v>50270286009.19</v>
       </c>
-      <c r="F128" s="1">
-        <v>50269272742.92</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="3">
         <v>44681</v>
       </c>
@@ -3005,11 +2618,8 @@
       <c r="E129" s="1">
         <v>46107666188.3</v>
       </c>
-      <c r="F129" s="1">
-        <v>46106802062.87</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="3">
         <v>44712</v>
       </c>
@@ -3025,11 +2635,8 @@
       <c r="E130" s="1">
         <v>45519094736.53999</v>
       </c>
-      <c r="F130" s="1">
-        <v>45518750923.86</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="3">
         <v>44742</v>
       </c>
@@ -3045,11 +2652,8 @@
       <c r="E131" s="1">
         <v>43747443202.46</v>
       </c>
-      <c r="F131" s="1">
-        <v>43746561277.33</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="3">
         <v>44773</v>
       </c>
@@ -3065,11 +2669,8 @@
       <c r="E132" s="1">
         <v>45304431259.36</v>
       </c>
-      <c r="F132" s="1">
-        <v>45303131705.44</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="3">
         <v>44804</v>
       </c>
@@ -3085,11 +2686,8 @@
       <c r="E133" s="1">
         <v>43237590005.3</v>
       </c>
-      <c r="F133" s="1">
-        <v>43237193282.92</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="3">
         <v>44834</v>
       </c>
@@ -3105,11 +2703,8 @@
       <c r="E134" s="1">
         <v>41516674580.5</v>
       </c>
-      <c r="F134" s="1">
-        <v>41515240522.93</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="3">
         <v>44865</v>
       </c>
@@ -3125,11 +2720,8 @@
       <c r="E135" s="1">
         <v>40713188313.89999</v>
       </c>
-      <c r="F135" s="1">
-        <v>40712619772.52</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="3">
         <v>44895</v>
       </c>
@@ -3145,11 +2737,8 @@
       <c r="E136" s="1">
         <v>43028134029.84</v>
       </c>
-      <c r="F136" s="1">
-        <v>43027359146.08</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="3">
         <v>44926</v>
       </c>
@@ -3165,11 +2754,8 @@
       <c r="E137" s="1">
         <v>41935279244.92</v>
       </c>
-      <c r="F137" s="1">
-        <v>41933824136.41</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="3">
         <v>44957</v>
       </c>
@@ -3185,11 +2771,8 @@
       <c r="E138" s="1">
         <v>44189592455.97</v>
       </c>
-      <c r="F138" s="1">
-        <v>44188047297.82</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="3">
         <v>44985</v>
       </c>
@@ -3205,11 +2788,8 @@
       <c r="E139" s="1">
         <v>42162539846.42001</v>
       </c>
-      <c r="F139" s="1">
-        <v>42161279137.19</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="3">
         <v>45016</v>
       </c>
@@ -3225,11 +2805,8 @@
       <c r="E140" s="1">
         <v>44547460232.85</v>
       </c>
-      <c r="F140" s="1">
-        <v>44546392777.65</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="3">
         <v>45046</v>
       </c>
@@ -3245,11 +2822,8 @@
       <c r="E141" s="1">
         <v>44883875298.93999</v>
       </c>
-      <c r="F141" s="1">
-        <v>44882668038.45</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="3">
         <v>45077</v>
       </c>
@@ -3265,11 +2839,8 @@
       <c r="E142" s="1">
         <v>43673211970.93</v>
       </c>
-      <c r="F142" s="1">
-        <v>43672633102.84</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="3">
         <v>45107</v>
       </c>
@@ -3285,11 +2856,8 @@
       <c r="E143" s="1">
         <v>44054561532.86</v>
       </c>
-      <c r="F143" s="1">
-        <v>44053347326.72</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="3">
         <v>45138</v>
       </c>
@@ -3305,11 +2873,8 @@
       <c r="E144" s="1">
         <v>43842962755.64</v>
       </c>
-      <c r="F144" s="1">
-        <v>43841971877.07</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="3">
         <v>45169</v>
       </c>
@@ -3325,11 +2890,8 @@
       <c r="E145" s="1">
         <v>42632156030.68</v>
       </c>
-      <c r="F145" s="1">
-        <v>42630693021.69</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="3">
         <v>45199</v>
       </c>
@@ -3345,11 +2907,8 @@
       <c r="E146" s="1">
         <v>40148798399.09</v>
       </c>
-      <c r="F146" s="1">
-        <v>40147828579.02</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="3">
         <v>45230</v>
       </c>
@@ -3365,28 +2924,22 @@
       <c r="E147" s="1">
         <v>37877581293.31</v>
       </c>
-      <c r="F147" s="1">
-        <v>37876036916.22</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="3">
         <v>45260</v>
       </c>
       <c r="B148" s="1">
-        <v>11445210398.45</v>
+        <v>11428029547.35</v>
       </c>
       <c r="C148" s="1">
-        <v>8992734371.700001</v>
+        <v>8981127522.91</v>
       </c>
       <c r="D148" s="1">
-        <v>20528191545.96</v>
+        <v>20498874668.22</v>
       </c>
       <c r="E148" s="1">
-        <v>40966136316.11</v>
-      </c>
-      <c r="F148" s="1">
-        <v>40973390502.17</v>
+        <v>40908031738.48</v>
       </c>
     </row>
   </sheetData>
@@ -3395,7 +2948,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F148">
+  <conditionalFormatting sqref="B2:E148">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
@@ -3415,9 +2968,9 @@
     <col min="1" max="1001" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3431,11 +2984,8 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>40816</v>
       </c>
@@ -3451,11 +3001,8 @@
       <c r="E2" s="1">
         <v>0.001203</v>
       </c>
-      <c r="F2" s="1">
-        <v>0.001224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>40847</v>
       </c>
@@ -3471,11 +3018,8 @@
       <c r="E3" s="1">
         <v>0.035731</v>
       </c>
-      <c r="F3" s="1">
-        <v>0.035742</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>40877</v>
       </c>
@@ -3491,11 +3035,8 @@
       <c r="E4" s="1">
         <v>-0.006832</v>
       </c>
-      <c r="F4" s="1">
-        <v>-0.006798999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>40908</v>
       </c>
@@ -3511,11 +3052,8 @@
       <c r="E5" s="1">
         <v>0.011629</v>
       </c>
-      <c r="F5" s="1">
-        <v>0.011646</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>40939</v>
       </c>
@@ -3531,11 +3069,8 @@
       <c r="E6" s="1">
         <v>0.027752</v>
       </c>
-      <c r="F6" s="1">
-        <v>0.02776</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>40968</v>
       </c>
@@ -3551,11 +3086,8 @@
       <c r="E7" s="1">
         <v>0.018403</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.018452</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>40999</v>
       </c>
@@ -3571,11 +3103,8 @@
       <c r="E8" s="1">
         <v>-0.003838</v>
       </c>
-      <c r="F8" s="1">
-        <v>-0.003805</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>41029</v>
       </c>
@@ -3591,11 +3120,8 @@
       <c r="E9" s="1">
         <v>0.010169</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.010181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>41060</v>
       </c>
@@ -3611,11 +3137,8 @@
       <c r="E10" s="1">
         <v>-0.007122000000000001</v>
       </c>
-      <c r="F10" s="1">
-        <v>-0.007114000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>41090</v>
       </c>
@@ -3631,11 +3154,8 @@
       <c r="E11" s="1">
         <v>0.013655</v>
       </c>
-      <c r="F11" s="1">
-        <v>0.013702</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>41121</v>
       </c>
@@ -3651,11 +3171,8 @@
       <c r="E12" s="1">
         <v>0.022421</v>
       </c>
-      <c r="F12" s="1">
-        <v>0.022443</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>41152</v>
       </c>
@@ -3671,11 +3188,8 @@
       <c r="E13" s="1">
         <v>0.006546</v>
       </c>
-      <c r="F13" s="1">
-        <v>0.006599000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>41182</v>
       </c>
@@ -3691,11 +3205,8 @@
       <c r="E14" s="1">
         <v>0.008597</v>
       </c>
-      <c r="F14" s="1">
-        <v>0.008647999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>41213</v>
       </c>
@@ -3711,11 +3222,8 @@
       <c r="E15" s="1">
         <v>0.001505</v>
       </c>
-      <c r="F15" s="1">
-        <v>0.001537</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>41243</v>
       </c>
@@ -3731,11 +3239,8 @@
       <c r="E16" s="1">
         <v>0.007571</v>
       </c>
-      <c r="F16" s="1">
-        <v>0.007581</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <v>41274</v>
       </c>
@@ -3751,11 +3256,8 @@
       <c r="E17" s="1">
         <v>0.008163999999999999</v>
       </c>
-      <c r="F17" s="1">
-        <v>0.00821</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <v>41305</v>
       </c>
@@ -3771,11 +3273,8 @@
       <c r="E18" s="1">
         <v>0.013479</v>
       </c>
-      <c r="F18" s="1">
-        <v>0.013506</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3">
         <v>41333</v>
       </c>
@@ -3791,11 +3290,8 @@
       <c r="E19" s="1">
         <v>0.007467000000000001</v>
       </c>
-      <c r="F19" s="1">
-        <v>0.007503999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="3">
         <v>41364</v>
       </c>
@@ -3811,11 +3307,8 @@
       <c r="E20" s="1">
         <v>0.015024</v>
       </c>
-      <c r="F20" s="1">
-        <v>0.015067</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3">
         <v>41394</v>
       </c>
@@ -3831,11 +3324,8 @@
       <c r="E21" s="1">
         <v>0.025087</v>
       </c>
-      <c r="F21" s="1">
-        <v>0.025126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>41425</v>
       </c>
@@ -3851,11 +3341,8 @@
       <c r="E22" s="1">
         <v>-0.01667</v>
       </c>
-      <c r="F22" s="1">
-        <v>-0.016669</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>41455</v>
       </c>
@@ -3871,11 +3358,8 @@
       <c r="E23" s="1">
         <v>-0.018162</v>
       </c>
-      <c r="F23" s="1">
-        <v>-0.018117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="3">
         <v>41486</v>
       </c>
@@ -3891,11 +3375,8 @@
       <c r="E24" s="1">
         <v>0.014253</v>
       </c>
-      <c r="F24" s="1">
-        <v>0.014264</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="3">
         <v>41517</v>
       </c>
@@ -3911,11 +3392,8 @@
       <c r="E25" s="1">
         <v>-0.011036</v>
       </c>
-      <c r="F25" s="1">
-        <v>-0.010998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="3">
         <v>41547</v>
       </c>
@@ -3931,11 +3409,8 @@
       <c r="E26" s="1">
         <v>0.020116</v>
       </c>
-      <c r="F26" s="1">
-        <v>0.020156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="3">
         <v>41578</v>
       </c>
@@ -3951,11 +3426,8 @@
       <c r="E27" s="1">
         <v>0.022229</v>
       </c>
-      <c r="F27" s="1">
-        <v>0.022274</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="3">
         <v>41608</v>
       </c>
@@ -3971,11 +3443,8 @@
       <c r="E28" s="1">
         <v>0.001659</v>
       </c>
-      <c r="F28" s="1">
-        <v>0.001664</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="3">
         <v>41639</v>
       </c>
@@ -3991,11 +3460,8 @@
       <c r="E29" s="1">
         <v>0.00731</v>
       </c>
-      <c r="F29" s="1">
-        <v>0.007331</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="3">
         <v>41670</v>
       </c>
@@ -4011,11 +3477,8 @@
       <c r="E30" s="1">
         <v>0.001871</v>
       </c>
-      <c r="F30" s="1">
-        <v>0.001873</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="3">
         <v>41698</v>
       </c>
@@ -4031,11 +3494,8 @@
       <c r="E31" s="1">
         <v>0.02296</v>
       </c>
-      <c r="F31" s="1">
-        <v>0.022941</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="3">
         <v>41729</v>
       </c>
@@ -4051,11 +3511,8 @@
       <c r="E32" s="1">
         <v>0.007581</v>
       </c>
-      <c r="F32" s="1">
-        <v>0.007613</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="3">
         <v>41759</v>
       </c>
@@ -4071,11 +3528,8 @@
       <c r="E33" s="1">
         <v>0.002563</v>
       </c>
-      <c r="F33" s="1">
-        <v>0.002567</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="3">
         <v>41790</v>
       </c>
@@ -4091,11 +3545,8 @@
       <c r="E34" s="1">
         <v>0.018617</v>
       </c>
-      <c r="F34" s="1">
-        <v>0.018658</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="3">
         <v>41820</v>
       </c>
@@ -4111,11 +3562,8 @@
       <c r="E35" s="1">
         <v>0.007591</v>
       </c>
-      <c r="F35" s="1">
-        <v>0.007621</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="3">
         <v>41851</v>
       </c>
@@ -4131,11 +3579,8 @@
       <c r="E36" s="1">
         <v>-0.003535</v>
       </c>
-      <c r="F36" s="1">
-        <v>-0.0035</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="3">
         <v>41882</v>
       </c>
@@ -4151,11 +3596,8 @@
       <c r="E37" s="1">
         <v>0.024399</v>
       </c>
-      <c r="F37" s="1">
-        <v>0.02441</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="3">
         <v>41912</v>
       </c>
@@ -4171,11 +3613,8 @@
       <c r="E38" s="1">
         <v>-0.018796</v>
       </c>
-      <c r="F38" s="1">
-        <v>-0.018787</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="3">
         <v>41943</v>
       </c>
@@ -4191,11 +3630,8 @@
       <c r="E39" s="1">
         <v>0.012251</v>
       </c>
-      <c r="F39" s="1">
-        <v>0.012333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="3">
         <v>41973</v>
       </c>
@@ -4211,11 +3647,8 @@
       <c r="E40" s="1">
         <v>0.016818</v>
       </c>
-      <c r="F40" s="1">
-        <v>0.016821</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="3">
         <v>42004</v>
       </c>
@@ -4231,11 +3664,8 @@
       <c r="E41" s="1">
         <v>0.002077</v>
       </c>
-      <c r="F41" s="1">
-        <v>0.002126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="3">
         <v>42035</v>
       </c>
@@ -4251,11 +3681,8 @@
       <c r="E42" s="1">
         <v>0.023353</v>
       </c>
-      <c r="F42" s="1">
-        <v>0.023417</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="3">
         <v>42063</v>
       </c>
@@ -4271,11 +3698,8 @@
       <c r="E43" s="1">
         <v>0.007671</v>
       </c>
-      <c r="F43" s="1">
-        <v>0.007678000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="3">
         <v>42094</v>
       </c>
@@ -4291,11 +3715,8 @@
       <c r="E44" s="1">
         <v>0.000726</v>
       </c>
-      <c r="F44" s="1">
-        <v>0.000746</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="3">
         <v>42124</v>
       </c>
@@ -4311,11 +3732,8 @@
       <c r="E45" s="1">
         <v>0.000483</v>
       </c>
-      <c r="F45" s="1">
-        <v>0.0005070000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="3">
         <v>42155</v>
       </c>
@@ -4331,11 +3749,8 @@
       <c r="E46" s="1">
         <v>-0.001447</v>
       </c>
-      <c r="F46" s="1">
-        <v>-0.001387</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="3">
         <v>42185</v>
       </c>
@@ -4351,11 +3766,8 @@
       <c r="E47" s="1">
         <v>-0.019128</v>
       </c>
-      <c r="F47" s="1">
-        <v>-0.019088</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="3">
         <v>42216</v>
       </c>
@@ -4371,11 +3783,8 @@
       <c r="E48" s="1">
         <v>0.010714</v>
       </c>
-      <c r="F48" s="1">
-        <v>0.01075</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="3">
         <v>42247</v>
       </c>
@@ -4391,11 +3800,8 @@
       <c r="E49" s="1">
         <v>-0.027126</v>
       </c>
-      <c r="F49" s="1">
-        <v>-0.027093</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="3">
         <v>42277</v>
       </c>
@@ -4411,11 +3817,8 @@
       <c r="E50" s="1">
         <v>-0.00876</v>
       </c>
-      <c r="F50" s="1">
-        <v>-0.008747</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="3">
         <v>42308</v>
       </c>
@@ -4431,11 +3834,8 @@
       <c r="E51" s="1">
         <v>0.028775</v>
       </c>
-      <c r="F51" s="1">
-        <v>0.028836</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="3">
         <v>42338</v>
       </c>
@@ -4451,11 +3851,8 @@
       <c r="E52" s="1">
         <v>-0.003813</v>
       </c>
-      <c r="F52" s="1">
-        <v>-0.003814</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="3">
         <v>42369</v>
       </c>
@@ -4471,11 +3868,8 @@
       <c r="E53" s="1">
         <v>-0.008185</v>
       </c>
-      <c r="F53" s="1">
-        <v>-0.008107999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="3">
         <v>42400</v>
       </c>
@@ -4491,11 +3885,8 @@
       <c r="E54" s="1">
         <v>-0.014827</v>
       </c>
-      <c r="F54" s="1">
-        <v>-0.014823</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="3">
         <v>42429</v>
       </c>
@@ -4511,11 +3902,8 @@
       <c r="E55" s="1">
         <v>0.00715</v>
       </c>
-      <c r="F55" s="1">
-        <v>0.007228</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="3">
         <v>42460</v>
       </c>
@@ -4531,11 +3919,8 @@
       <c r="E56" s="1">
         <v>0.034734</v>
       </c>
-      <c r="F56" s="1">
-        <v>0.034744</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="3">
         <v>42490</v>
       </c>
@@ -4551,11 +3936,8 @@
       <c r="E57" s="1">
         <v>0.009242999999999999</v>
       </c>
-      <c r="F57" s="1">
-        <v>0.009256</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="3">
         <v>42521</v>
       </c>
@@ -4571,11 +3953,8 @@
       <c r="E58" s="1">
         <v>0.001883</v>
       </c>
-      <c r="F58" s="1">
-        <v>0.001941</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="3">
         <v>42551</v>
       </c>
@@ -4591,11 +3970,8 @@
       <c r="E59" s="1">
         <v>0.010112</v>
       </c>
-      <c r="F59" s="1">
-        <v>0.010098</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="3">
         <v>42582</v>
       </c>
@@ -4611,11 +3987,8 @@
       <c r="E60" s="1">
         <v>0.021265</v>
       </c>
-      <c r="F60" s="1">
-        <v>0.021276</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="3">
         <v>42613</v>
       </c>
@@ -4631,11 +4004,8 @@
       <c r="E61" s="1">
         <v>0.001145</v>
       </c>
-      <c r="F61" s="1">
-        <v>0.001155</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="3">
         <v>42643</v>
       </c>
@@ -4651,11 +4021,8 @@
       <c r="E62" s="1">
         <v>0.00083</v>
       </c>
-      <c r="F62" s="1">
-        <v>0.0009120000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="3">
         <v>42674</v>
       </c>
@@ -4671,11 +4038,8 @@
       <c r="E63" s="1">
         <v>-0.011778</v>
       </c>
-      <c r="F63" s="1">
-        <v>-0.011775</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="3">
         <v>42704</v>
       </c>
@@ -4691,11 +4055,8 @@
       <c r="E64" s="1">
         <v>-0.011502</v>
       </c>
-      <c r="F64" s="1">
-        <v>-0.011447</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="3">
         <v>42735</v>
       </c>
@@ -4711,11 +4072,8 @@
       <c r="E65" s="1">
         <v>0.010141</v>
       </c>
-      <c r="F65" s="1">
-        <v>0.010322</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="3">
         <v>42766</v>
       </c>
@@ -4731,11 +4089,8 @@
       <c r="E66" s="1">
         <v>0.011655</v>
       </c>
-      <c r="F66" s="1">
-        <v>0.011698</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="3">
         <v>42794</v>
       </c>
@@ -4751,11 +4106,8 @@
       <c r="E67" s="1">
         <v>0.017674</v>
       </c>
-      <c r="F67" s="1">
-        <v>0.017685</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="3">
         <v>42825</v>
       </c>
@@ -4771,11 +4123,8 @@
       <c r="E68" s="1">
         <v>0.005195</v>
       </c>
-      <c r="F68" s="1">
-        <v>0.005258000000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="3">
         <v>42855</v>
       </c>
@@ -4791,11 +4140,8 @@
       <c r="E69" s="1">
         <v>0.013598</v>
       </c>
-      <c r="F69" s="1">
-        <v>0.013641</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="3">
         <v>42886</v>
       </c>
@@ -4811,11 +4157,8 @@
       <c r="E70" s="1">
         <v>0.015262</v>
       </c>
-      <c r="F70" s="1">
-        <v>0.01527</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="3">
         <v>42916</v>
       </c>
@@ -4831,11 +4174,8 @@
       <c r="E71" s="1">
         <v>0.005257</v>
       </c>
-      <c r="F71" s="1">
-        <v>0.005279000000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="3">
         <v>42947</v>
       </c>
@@ -4851,11 +4191,8 @@
       <c r="E72" s="1">
         <v>0.011307</v>
       </c>
-      <c r="F72" s="1">
-        <v>0.011318</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="3">
         <v>42978</v>
       </c>
@@ -4871,11 +4208,8 @@
       <c r="E73" s="1">
         <v>0.010725</v>
       </c>
-      <c r="F73" s="1">
-        <v>0.010768</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="3">
         <v>43008</v>
       </c>
@@ -4891,11 +4225,8 @@
       <c r="E74" s="1">
         <v>0.008107</v>
       </c>
-      <c r="F74" s="1">
-        <v>0.008131000000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="3">
         <v>43039</v>
       </c>
@@ -4911,11 +4242,8 @@
       <c r="E75" s="1">
         <v>0.011964</v>
       </c>
-      <c r="F75" s="1">
-        <v>0.012022</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="3">
         <v>43069</v>
       </c>
@@ -4931,11 +4259,8 @@
       <c r="E76" s="1">
         <v>0.013355</v>
       </c>
-      <c r="F76" s="1">
-        <v>0.013356</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="3">
         <v>43100</v>
       </c>
@@ -4951,11 +4276,8 @@
       <c r="E77" s="1">
         <v>0.012016</v>
       </c>
-      <c r="F77" s="1">
-        <v>0.012674</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="3">
         <v>43131</v>
       </c>
@@ -4971,11 +4293,8 @@
       <c r="E78" s="1">
         <v>0.019876</v>
       </c>
-      <c r="F78" s="1">
-        <v>0.024838</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="3">
         <v>43159</v>
       </c>
@@ -4991,11 +4310,8 @@
       <c r="E79" s="1">
         <v>-0.029913</v>
       </c>
-      <c r="F79" s="1">
-        <v>-0.029929</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="3">
         <v>43190</v>
       </c>
@@ -5011,11 +4327,8 @@
       <c r="E80" s="1">
         <v>0.005778999999999999</v>
       </c>
-      <c r="F80" s="1">
-        <v>0.001458</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="3">
         <v>43220</v>
       </c>
@@ -5031,11 +4344,8 @@
       <c r="E81" s="1">
         <v>-0.004682</v>
       </c>
-      <c r="F81" s="1">
-        <v>-0.002009</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="3">
         <v>43251</v>
       </c>
@@ -5051,11 +4361,8 @@
       <c r="E82" s="1">
         <v>0.009103</v>
       </c>
-      <c r="F82" s="1">
-        <v>0.006972000000000001</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="3">
         <v>43281</v>
       </c>
@@ -5071,11 +4378,8 @@
       <c r="E83" s="1">
         <v>-0.002073</v>
       </c>
-      <c r="F83" s="1">
-        <v>-0.002804</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="3">
         <v>43312</v>
       </c>
@@ -5091,11 +4395,8 @@
       <c r="E84" s="1">
         <v>0.009061</v>
       </c>
-      <c r="F84" s="1">
-        <v>0.013504</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="3">
         <v>43343</v>
       </c>
@@ -5111,11 +4412,8 @@
       <c r="E85" s="1">
         <v>0.00937</v>
       </c>
-      <c r="F85" s="1">
-        <v>0.008217</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="3">
         <v>43373</v>
       </c>
@@ -5131,11 +4429,8 @@
       <c r="E86" s="1">
         <v>-0.008794</v>
       </c>
-      <c r="F86" s="1">
-        <v>-0.005053999999999999</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="3">
         <v>43404</v>
       </c>
@@ -5151,11 +4446,8 @@
       <c r="E87" s="1">
         <v>-0.039984</v>
       </c>
-      <c r="F87" s="1">
-        <v>-0.040558</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="3">
         <v>43434</v>
       </c>
@@ -5171,11 +4463,8 @@
       <c r="E88" s="1">
         <v>0.012878</v>
       </c>
-      <c r="F88" s="1">
-        <v>0.011452</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="3">
         <v>43465</v>
       </c>
@@ -5191,11 +4480,8 @@
       <c r="E89" s="1">
         <v>-0.003477</v>
       </c>
-      <c r="F89" s="1">
-        <v>-0.016145</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="3">
         <v>43496</v>
       </c>
@@ -5211,11 +4497,8 @@
       <c r="E90" s="1">
         <v>0.032009</v>
       </c>
-      <c r="F90" s="1">
-        <v>0.037042</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="3">
         <v>43524</v>
       </c>
@@ -5231,11 +4514,8 @@
       <c r="E91" s="1">
         <v>0.005999</v>
       </c>
-      <c r="F91" s="1">
-        <v>0.010191</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="3">
         <v>43555</v>
       </c>
@@ -5251,11 +4531,8 @@
       <c r="E92" s="1">
         <v>0.027935</v>
       </c>
-      <c r="F92" s="1">
-        <v>0.021151</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="3">
         <v>43585</v>
       </c>
@@ -5271,11 +4548,8 @@
       <c r="E93" s="1">
         <v>0.00509</v>
       </c>
-      <c r="F93" s="1">
-        <v>0.010597</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="3">
         <v>43616</v>
       </c>
@@ -5291,11 +4565,8 @@
       <c r="E94" s="1">
         <v>0.010002</v>
       </c>
-      <c r="F94" s="1">
-        <v>-0.004249</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="3">
         <v>43646</v>
       </c>
@@ -5311,11 +4582,8 @@
       <c r="E95" s="1">
         <v>0.029644</v>
       </c>
-      <c r="F95" s="1">
-        <v>0.033356</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="3">
         <v>43677</v>
       </c>
@@ -5331,11 +4599,8 @@
       <c r="E96" s="1">
         <v>0.004747</v>
       </c>
-      <c r="F96" s="1">
-        <v>0.005241</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="3">
         <v>43708</v>
       </c>
@@ -5351,11 +4616,8 @@
       <c r="E97" s="1">
         <v>0.044206</v>
       </c>
-      <c r="F97" s="1">
-        <v>0.024308</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="3">
         <v>43738</v>
       </c>
@@ -5371,11 +4633,8 @@
       <c r="E98" s="1">
         <v>-0.004635</v>
       </c>
-      <c r="F98" s="1">
-        <v>0.002227</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="3">
         <v>43769</v>
       </c>
@@ -5391,11 +4650,8 @@
       <c r="E99" s="1">
         <v>0.002441</v>
       </c>
-      <c r="F99" s="1">
-        <v>0.002473</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="3">
         <v>43799</v>
       </c>
@@ -5411,11 +4667,8 @@
       <c r="E100" s="1">
         <v>0.008153000000000001</v>
       </c>
-      <c r="F100" s="1">
-        <v>0.008192</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="3">
         <v>43830</v>
       </c>
@@ -5431,11 +4684,8 @@
       <c r="E101" s="1">
         <v>-0.000751</v>
       </c>
-      <c r="F101" s="1">
-        <v>-0.0007470000000000001</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="3">
         <v>43861</v>
       </c>
@@ -5451,11 +4701,8 @@
       <c r="E102" s="1">
         <v>0.02564</v>
       </c>
-      <c r="F102" s="1">
-        <v>0.025673</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="3">
         <v>43890</v>
       </c>
@@ -5471,11 +4718,8 @@
       <c r="E103" s="1">
         <v>0.001266</v>
       </c>
-      <c r="F103" s="1">
-        <v>0.001282</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="3">
         <v>43921</v>
       </c>
@@ -5491,11 +4735,8 @@
       <c r="E104" s="1">
         <v>-0.037684</v>
       </c>
-      <c r="F104" s="1">
-        <v>-0.03767</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="3">
         <v>43951</v>
       </c>
@@ -5511,11 +4752,8 @@
       <c r="E105" s="1">
         <v>0.044486</v>
       </c>
-      <c r="F105" s="1">
-        <v>0.044508</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="3">
         <v>43982</v>
       </c>
@@ -5531,11 +4769,8 @@
       <c r="E106" s="1">
         <v>0.003246</v>
       </c>
-      <c r="F106" s="1">
-        <v>0.003265</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="3">
         <v>44012</v>
       </c>
@@ -5551,11 +4786,8 @@
       <c r="E107" s="1">
         <v>0.010239</v>
       </c>
-      <c r="F107" s="1">
-        <v>0.010239</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="3">
         <v>44043</v>
       </c>
@@ -5571,11 +4803,8 @@
       <c r="E108" s="1">
         <v>0.040234</v>
       </c>
-      <c r="F108" s="1">
-        <v>0.04024</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="3">
         <v>44074</v>
       </c>
@@ -5591,11 +4820,8 @@
       <c r="E109" s="1">
         <v>-0.003186</v>
       </c>
-      <c r="F109" s="1">
-        <v>-0.003183</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="3">
         <v>44104</v>
       </c>
@@ -5611,11 +4837,8 @@
       <c r="E110" s="1">
         <v>-0.008924999999999999</v>
       </c>
-      <c r="F110" s="1">
-        <v>-0.008980999999999999</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="3">
         <v>44135</v>
       </c>
@@ -5631,11 +4854,8 @@
       <c r="E111" s="1">
         <v>-0.020374</v>
       </c>
-      <c r="F111" s="1">
-        <v>-0.020368</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="3">
         <v>44165</v>
       </c>
@@ -5651,11 +4871,8 @@
       <c r="E112" s="1">
         <v>0.053226</v>
       </c>
-      <c r="F112" s="1">
-        <v>0.05322499999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="3">
         <v>44196</v>
       </c>
@@ -5671,11 +4888,8 @@
       <c r="E113" s="1">
         <v>0.013933</v>
       </c>
-      <c r="F113" s="1">
-        <v>0.013948</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="3">
         <v>44227</v>
       </c>
@@ -5691,11 +4905,8 @@
       <c r="E114" s="1">
         <v>-0.020192</v>
       </c>
-      <c r="F114" s="1">
-        <v>-0.020193</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="3">
         <v>44255</v>
       </c>
@@ -5711,11 +4922,8 @@
       <c r="E115" s="1">
         <v>-0.018451</v>
       </c>
-      <c r="F115" s="1">
-        <v>-0.018448</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="3">
         <v>44286</v>
       </c>
@@ -5731,11 +4939,8 @@
       <c r="E116" s="1">
         <v>0.0006980000000000001</v>
       </c>
-      <c r="F116" s="1">
-        <v>0.0007159999999999999</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="3">
         <v>44316</v>
       </c>
@@ -5751,11 +4956,8 @@
       <c r="E117" s="1">
         <v>0.028885</v>
       </c>
-      <c r="F117" s="1">
-        <v>0.028889</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="3">
         <v>44347</v>
       </c>
@@ -5771,11 +4973,8 @@
       <c r="E118" s="1">
         <v>0.015936</v>
       </c>
-      <c r="F118" s="1">
-        <v>0.015938</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="3">
         <v>44377</v>
       </c>
@@ -5791,11 +4990,8 @@
       <c r="E119" s="1">
         <v>0.023884</v>
       </c>
-      <c r="F119" s="1">
-        <v>0.02391</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="3">
         <v>44408</v>
       </c>
@@ -5811,11 +5007,8 @@
       <c r="E120" s="1">
         <v>0.020584</v>
       </c>
-      <c r="F120" s="1">
-        <v>0.020569</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="3">
         <v>44439</v>
       </c>
@@ -5831,11 +5024,8 @@
       <c r="E121" s="1">
         <v>0.010881</v>
       </c>
-      <c r="F121" s="1">
-        <v>0.010892</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="3">
         <v>44469</v>
       </c>
@@ -5851,11 +5041,8 @@
       <c r="E122" s="1">
         <v>-0.033223</v>
       </c>
-      <c r="F122" s="1">
-        <v>-0.033221</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="3">
         <v>44500</v>
       </c>
@@ -5871,11 +5058,8 @@
       <c r="E123" s="1">
         <v>0.031335</v>
       </c>
-      <c r="F123" s="1">
-        <v>0.031337</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="3">
         <v>44530</v>
       </c>
@@ -5891,11 +5075,8 @@
       <c r="E124" s="1">
         <v>0.017353</v>
       </c>
-      <c r="F124" s="1">
-        <v>0.01736</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="3">
         <v>44561</v>
       </c>
@@ -5911,11 +5092,8 @@
       <c r="E125" s="1">
         <v>0.00827</v>
       </c>
-      <c r="F125" s="1">
-        <v>0.008281</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="3">
         <v>44592</v>
       </c>
@@ -5931,11 +5109,8 @@
       <c r="E126" s="1">
         <v>-0.046588</v>
       </c>
-      <c r="F126" s="1">
-        <v>-0.046586</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="3">
         <v>44620</v>
       </c>
@@ -5951,11 +5126,8 @@
       <c r="E127" s="1">
         <v>-0.019075</v>
       </c>
-      <c r="F127" s="1">
-        <v>-0.019058</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="3">
         <v>44651</v>
       </c>
@@ -5971,11 +5143,8 @@
       <c r="E128" s="1">
         <v>-0.02338</v>
       </c>
-      <c r="F128" s="1">
-        <v>-0.023376</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="3">
         <v>44681</v>
       </c>
@@ -5991,11 +5160,8 @@
       <c r="E129" s="1">
         <v>-0.07989399999999999</v>
       </c>
-      <c r="F129" s="1">
-        <v>-0.079887</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="3">
         <v>44712</v>
       </c>
@@ -6011,11 +5177,8 @@
       <c r="E130" s="1">
         <v>-0.009348</v>
       </c>
-      <c r="F130" s="1">
-        <v>-0.009331000000000001</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="3">
         <v>44742</v>
       </c>
@@ -6031,11 +5194,8 @@
       <c r="E131" s="1">
         <v>-0.035533</v>
       </c>
-      <c r="F131" s="1">
-        <v>-0.035525</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="3">
         <v>44773</v>
       </c>
@@ -6051,11 +5211,8 @@
       <c r="E132" s="1">
         <v>0.03943</v>
       </c>
-      <c r="F132" s="1">
-        <v>0.039431</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="3">
         <v>44804</v>
       </c>
@@ -6071,11 +5228,8 @@
       <c r="E133" s="1">
         <v>-0.042222</v>
       </c>
-      <c r="F133" s="1">
-        <v>-0.042204</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="3">
         <v>44834</v>
       </c>
@@ -6091,11 +5245,8 @@
       <c r="E134" s="1">
         <v>-0.07750499999999999</v>
       </c>
-      <c r="F134" s="1">
-        <v>-0.077504</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="3">
         <v>44865</v>
       </c>
@@ -6111,11 +5262,8 @@
       <c r="E135" s="1">
         <v>-0.011631</v>
       </c>
-      <c r="F135" s="1">
-        <v>-0.011611</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="3">
         <v>44895</v>
       </c>
@@ -6131,11 +5279,8 @@
       <c r="E136" s="1">
         <v>0.061094</v>
       </c>
-      <c r="F136" s="1">
-        <v>0.061116</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="3">
         <v>44926</v>
       </c>
@@ -6151,11 +5296,8 @@
       <c r="E137" s="1">
         <v>-0.021664</v>
       </c>
-      <c r="F137" s="1">
-        <v>-0.021662</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="3">
         <v>44957</v>
       </c>
@@ -6171,11 +5313,8 @@
       <c r="E138" s="1">
         <v>0.057892</v>
       </c>
-      <c r="F138" s="1">
-        <v>0.057901</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="3">
         <v>44985</v>
       </c>
@@ -6191,11 +5330,8 @@
       <c r="E139" s="1">
         <v>-0.04226899999999999</v>
       </c>
-      <c r="F139" s="1">
-        <v>-0.042256</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="3">
         <v>45016</v>
       </c>
@@ -6211,11 +5347,8 @@
       <c r="E140" s="1">
         <v>0.032184</v>
       </c>
-      <c r="F140" s="1">
-        <v>0.032195</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="3">
         <v>45046</v>
       </c>
@@ -6231,11 +5364,8 @@
       <c r="E141" s="1">
         <v>0.011411</v>
       </c>
-      <c r="F141" s="1">
-        <v>0.011419</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
+    </row>
+    <row r="142" spans="1:5">
       <c r="A142" s="3">
         <v>45077</v>
       </c>
@@ -6251,11 +5381,8 @@
       <c r="E142" s="1">
         <v>-0.02331</v>
       </c>
-      <c r="F142" s="1">
-        <v>-0.023289</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="3">
         <v>45107</v>
       </c>
@@ -6271,11 +5398,8 @@
       <c r="E143" s="1">
         <v>0.012684</v>
       </c>
-      <c r="F143" s="1">
-        <v>0.012691</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="3">
         <v>45138</v>
       </c>
@@ -6291,11 +5415,8 @@
       <c r="E144" s="1">
         <v>-0.000907</v>
       </c>
-      <c r="F144" s="1">
-        <v>-0.000893</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="3">
         <v>45169</v>
       </c>
@@ -6311,11 +5432,8 @@
       <c r="E145" s="1">
         <v>-0.023792</v>
       </c>
-      <c r="F145" s="1">
-        <v>-0.023789</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="3">
         <v>45199</v>
       </c>
@@ -6331,11 +5449,8 @@
       <c r="E146" s="1">
         <v>-0.054409</v>
       </c>
-      <c r="F146" s="1">
-        <v>-0.054394</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="3">
         <v>45230</v>
       </c>
@@ -6351,28 +5466,22 @@
       <c r="E147" s="1">
         <v>-0.043883</v>
       </c>
-      <c r="F147" s="1">
-        <v>-0.043884</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="3">
         <v>45260</v>
       </c>
       <c r="B148" s="1">
-        <v>0.08100300000000001</v>
+        <v>0.07937999999999999</v>
       </c>
       <c r="C148" s="1">
-        <v>0.083926</v>
+        <v>0.082527</v>
       </c>
       <c r="D148" s="1">
-        <v>0.09067500000000001</v>
+        <v>0.08911799999999999</v>
       </c>
       <c r="E148" s="1">
-        <v>0.086474</v>
-      </c>
-      <c r="F148" s="1">
-        <v>0.086684</v>
+        <v>0.08493299999999999</v>
       </c>
     </row>
   </sheetData>
@@ -6381,7 +5490,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F148">
+  <conditionalFormatting sqref="B2:E148">
     <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>